<commit_message>
feat: allow dynamic format & static cellStyle definition
</commit_message>
<xml_diff>
--- a/consumption.xlsx
+++ b/consumption.xlsx
@@ -518,407 +518,407 @@
     </row>
     <row r="2" ht="30" customHeight="1">
       <c r="A2" s="4" t="str">
-        <v>ff1f300c-91e3-425e-8f77-13a152b464ef</v>
+        <v>5ea26c56-8806-4af3-b786-320c92ea0b08</v>
       </c>
       <c r="B2" s="5" t="str">
-        <v>f759243c-b320-43c3-a6a3-caca5a19b816</v>
+        <v>8205dbdc-51d7-4bd0-a214-936b5769d8cd</v>
       </c>
       <c r="C2" s="5" t="str">
-        <v>Handcrafted Soft Car</v>
+        <v>Gorgeous Granite Bacon</v>
       </c>
       <c r="D2" s="5" t="str">
-        <v>9.1.5</v>
+        <v>0.0.9</v>
       </c>
       <c r="E2" s="5" t="str">
-        <v>July</v>
+        <v>January</v>
       </c>
       <c r="F2" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G2" s="5">
-        <v>26</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1">
       <c r="A3" s="4" t="str">
-        <v>3fb5119e-b4c1-4e46-837e-d7e6af24ee57</v>
+        <v>42fe9f54-2c45-4c86-aaf6-115c09b02d6e</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>529d9991-a60a-41c0-9cf8-8f708047ff8e</v>
+        <v>41734f69-4836-47b7-b905-a8e708cea16d</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>Modern Metal Ball</v>
+        <v>Sleek Concrete Computer</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>7.7.0</v>
+        <v>2.9.1</v>
       </c>
       <c r="E3" s="5" t="str">
-        <v>May</v>
+        <v>June</v>
       </c>
       <c r="F3" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G3" s="5">
-        <v>72</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" ht="30" customHeight="1">
       <c r="A4" s="4" t="str">
-        <v>947d2075-b6c4-4470-9e4e-5f09450fd6bb</v>
+        <v>63cc659e-0f87-44d7-b7f8-f724009f08af</v>
       </c>
       <c r="B4" s="5" t="str">
-        <v>56a8b0ba-a26a-4ed8-90d2-6400c3a5962c</v>
+        <v>f0f98488-050e-47b5-bc80-70211b87f5ec</v>
       </c>
       <c r="C4" s="5" t="str">
-        <v>Handmade Metal Ball</v>
+        <v>Electronic Bronze Gloves</v>
       </c>
       <c r="D4" s="5" t="str">
-        <v>7.7.0</v>
+        <v>0.2.8</v>
       </c>
       <c r="E4" s="5" t="str">
-        <v>July</v>
+        <v>October</v>
       </c>
       <c r="F4" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G4" s="5">
-        <v>45</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" ht="30" customHeight="1">
       <c r="A5" s="4" t="str">
-        <v>2cb6bc32-083d-42a6-99d0-8dc88aedc43f</v>
+        <v>b5012871-7271-46f5-9465-96cebfb1e276</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>2b0d11c0-55c6-4523-8e82-9485eaa2e39d</v>
+        <v>979913f8-08da-4c3a-9b34-5e9c1ce91fa0</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>Refined Soft Pants</v>
+        <v>Luxurious Steel Shirt</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>0.6.9</v>
+        <v>8.9.9</v>
       </c>
       <c r="E5" s="5" t="str">
-        <v>June</v>
+        <v>May</v>
       </c>
       <c r="F5" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G5" s="5">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" ht="30" customHeight="1">
       <c r="A6" s="4" t="str">
-        <v>eef36c09-17d1-4e07-add7-79a3b0704e50</v>
+        <v>de9ee68c-111e-4cc5-881d-75de59967099</v>
       </c>
       <c r="B6" s="5" t="str">
-        <v>bd96751c-7aaf-40bc-8cb6-fe154b50b5a2</v>
+        <v>90b20278-e9bc-462e-b59a-7674157c5c17</v>
       </c>
       <c r="C6" s="5" t="str">
-        <v>Handcrafted Bronze Tuna</v>
+        <v>Bespoke Rubber Chair</v>
       </c>
       <c r="D6" s="5" t="str">
-        <v>2.3.1</v>
+        <v>8.9.3</v>
       </c>
       <c r="E6" s="5" t="str">
-        <v>October</v>
+        <v>January</v>
       </c>
       <c r="F6" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G6" s="5">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" ht="30" customHeight="1">
       <c r="A7" s="4" t="str">
-        <v>cabee15c-c5c5-4195-8be8-e1bc6a2f2c6e</v>
+        <v>5a3de9c7-e5e2-4437-883f-446f18ac999f</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>7c729130-6dfd-4b44-b86e-0ef61d28e5e4</v>
+        <v>49a1cbaf-09c0-4597-8c25-3d395ad286db</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>Generic Concrete Car</v>
+        <v>Sleek Concrete Pants</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>5.8.8</v>
+        <v>2.6.2</v>
       </c>
       <c r="E7" s="5" t="str">
-        <v>October</v>
+        <v>August</v>
       </c>
       <c r="F7" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G7" s="5">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" ht="30" customHeight="1">
       <c r="A8" s="4" t="str">
-        <v>cd6b7bb8-4038-4f2a-b471-ba9e3e4b6ae4</v>
+        <v>5936451c-4804-440a-942f-bd773f8e1ccb</v>
       </c>
       <c r="B8" s="5" t="str">
-        <v>9bb12c45-7838-40b9-ac13-f8b71331a1aa</v>
+        <v>5bb8a36c-48d1-484c-9377-eedcc433eae0</v>
       </c>
       <c r="C8" s="5" t="str">
-        <v>Elegant Steel Chair</v>
+        <v>Refined Metal Towels</v>
       </c>
       <c r="D8" s="5" t="str">
-        <v>3.7.7</v>
+        <v>7.2.6</v>
       </c>
       <c r="E8" s="5" t="str">
-        <v>February</v>
+        <v>January</v>
       </c>
       <c r="F8" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G8" s="5">
-        <v>53</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" ht="30" customHeight="1">
       <c r="A9" s="4" t="str">
-        <v>b6b58d30-1227-4208-b9d9-5c6449266368</v>
+        <v>e4521659-2206-4ec0-95e3-a72aea188d33</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>d20f6649-2ff7-491b-9224-54b8af411513</v>
+        <v>3b1fe986-d11f-462f-8dac-2977caf1d014</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>Generic Metal Bike</v>
+        <v>Tasty Wooden Chicken</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>0.5.5</v>
+        <v>1.9.5</v>
       </c>
       <c r="E9" s="5" t="str">
-        <v>November</v>
+        <v>April</v>
       </c>
       <c r="F9" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G9" s="5">
-        <v>26</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" ht="30" customHeight="1">
       <c r="A10" s="4" t="str">
-        <v>6d89be72-bba8-42de-8b62-cc6e54ec15cb</v>
+        <v>bab313a5-24bb-4d7c-8ffc-518aafc8f1e2</v>
       </c>
       <c r="B10" s="5" t="str">
-        <v>0260f29a-a6ad-4766-9dd7-be222cd84936</v>
+        <v>64cb85fd-0d06-4776-9053-51119312384b</v>
       </c>
       <c r="C10" s="5" t="str">
-        <v>Handcrafted Wooden Computer</v>
+        <v>Practical Frozen Keyboard</v>
       </c>
       <c r="D10" s="5" t="str">
-        <v>6.2.0</v>
+        <v>8.0.6</v>
       </c>
       <c r="E10" s="5" t="str">
-        <v>May</v>
+        <v>September</v>
       </c>
       <c r="F10" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G10" s="5">
-        <v>47</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" ht="30" customHeight="1">
       <c r="A11" s="4" t="str">
-        <v>58ce8909-0762-4ac0-bc8e-dcd9a357f5e3</v>
+        <v>4ef1caf6-6a60-4ae2-ad6b-c538ab4bd937</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>5807438c-88d3-46b8-8f85-b345f00b4602</v>
+        <v>2b295dae-7a3e-41c9-a0a4-7d5eb43e6f51</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>Tasty Soft Shoes</v>
+        <v>Small Cotton Chair</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v>9.8.8</v>
+        <v>0.2.6</v>
       </c>
       <c r="E11" s="5" t="str">
-        <v>February</v>
+        <v>June</v>
       </c>
       <c r="F11" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G11" s="5">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" ht="30" customHeight="1">
       <c r="A12" s="4" t="str">
-        <v>5dde59bd-f9e7-4159-8e42-1c255035d93e</v>
+        <v>eafe3242-073f-42d6-a066-8500daee2754</v>
       </c>
       <c r="B12" s="5" t="str">
-        <v>e7f58f54-a6ee-400c-a47b-f83f689ddf67</v>
+        <v>0ea1a1d2-2ae7-47df-9799-1bb8b370e1ad</v>
       </c>
       <c r="C12" s="5" t="str">
-        <v>Gorgeous Concrete Keyboard</v>
+        <v>Refined Frozen Soap</v>
       </c>
       <c r="D12" s="5" t="str">
-        <v>1.9.7</v>
+        <v>9.9.7</v>
       </c>
       <c r="E12" s="5" t="str">
-        <v>July</v>
+        <v>June</v>
       </c>
       <c r="F12" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G12" s="5">
-        <v>4</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" ht="30" customHeight="1">
       <c r="A13" s="4" t="str">
-        <v>ccbccfce-0fe4-4437-9250-6cde17cc1a5d</v>
+        <v>b074c1ce-e6a3-4bb8-9ae2-873a9eaa0dcb</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>cd9e62c5-3b8b-4c82-a449-5ff410c968f5</v>
+        <v>d72c98a8-d0f1-44e2-8bb6-11eed1d0f910</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>Recycled Cotton Gloves</v>
+        <v>Generic Concrete Sausages</v>
       </c>
       <c r="D13" s="5" t="str">
-        <v>1.3.6</v>
+        <v>1.9.4</v>
       </c>
       <c r="E13" s="5" t="str">
-        <v>October</v>
+        <v>April</v>
       </c>
       <c r="F13" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G13" s="5">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" ht="30" customHeight="1">
       <c r="A14" s="4" t="str">
-        <v>c03901f4-b9e5-4335-a742-7aa5c4bf9bfc</v>
+        <v>41be3052-c7a6-4b26-ab4d-d4fe28a3c1e5</v>
       </c>
       <c r="B14" s="5" t="str">
-        <v>8edc45a2-1eb4-4dfb-9ee9-3927bff4ed43</v>
+        <v>f6443efa-f0ce-4b14-9411-aca56e37b8e9</v>
       </c>
       <c r="C14" s="5" t="str">
-        <v>Ergonomic Bronze Keyboard</v>
+        <v>Rustic Soft Chicken</v>
       </c>
       <c r="D14" s="5" t="str">
-        <v>9.3.6</v>
+        <v>5.6.8</v>
       </c>
       <c r="E14" s="5" t="str">
-        <v>July</v>
+        <v>September</v>
       </c>
       <c r="F14" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G14" s="5">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" ht="30" customHeight="1">
       <c r="A15" s="4" t="str">
-        <v>0ef8c7c0-44f0-4737-b741-a5ae618c6862</v>
+        <v>ee428ba8-2e19-440b-aba2-0a021a5d7a63</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>85ad311c-7a36-4cab-9647-228a7aa73283</v>
+        <v>a81c59ce-978b-4f43-a46b-8e6c8ee52217</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>Awesome Frozen Keyboard</v>
+        <v>Awesome Frozen Chips</v>
       </c>
       <c r="D15" s="5" t="str">
-        <v>4.4.7</v>
+        <v>3.3.3</v>
       </c>
       <c r="E15" s="5" t="str">
-        <v>May</v>
+        <v>March</v>
       </c>
       <c r="F15" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G15" s="5">
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" ht="30" customHeight="1">
       <c r="A16" s="4" t="str">
-        <v>eb997d0f-9b78-4f4c-8bdd-91605e95f8ab</v>
+        <v>4b7fc6c5-44b2-4a86-9315-d531f26bf78c</v>
       </c>
       <c r="B16" s="5" t="str">
-        <v>e1c9fbce-9103-48e5-8b86-7c9a30840b92</v>
+        <v>fec2ee66-aff7-4b93-a0e5-9712610899b4</v>
       </c>
       <c r="C16" s="5" t="str">
-        <v>Handcrafted Wooden Car</v>
+        <v>Fantastic Granite Fish</v>
       </c>
       <c r="D16" s="5" t="str">
-        <v>2.7.4</v>
+        <v>3.9.7</v>
       </c>
       <c r="E16" s="5" t="str">
-        <v>August</v>
+        <v>May</v>
       </c>
       <c r="F16" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G16" s="5">
-        <v>39</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" ht="30" customHeight="1">
       <c r="A17" s="4" t="str">
-        <v>68a15fb9-2c33-4075-8a5b-65cccbaa0d3d</v>
+        <v>b5f27cf3-b45b-475c-afff-13f500469607</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>19d9412d-44a9-4b91-83c0-4cb78adfc91d</v>
+        <v>67f2b52c-30ff-47a7-9575-5ee5d0e2cc9e</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>Modern Metal Chair</v>
+        <v>Recycled Plastic Shirt</v>
       </c>
       <c r="D17" s="5" t="str">
-        <v>2.2.4</v>
+        <v>9.2.4</v>
       </c>
       <c r="E17" s="5" t="str">
-        <v>September</v>
+        <v>March</v>
       </c>
       <c r="F17" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G17" s="5">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" ht="30" customHeight="1">
       <c r="A18" s="4" t="str">
-        <v>54358271-5fc1-4605-9281-fac8d911f05b</v>
+        <v>41cf6a0f-06a9-4f11-bf49-a5bce53337d9</v>
       </c>
       <c r="B18" s="5" t="str">
-        <v>eea4fc91-dc25-4edd-a472-5db846a3aeed</v>
+        <v>455edfdb-2fee-48c8-bd77-95329ca4228e</v>
       </c>
       <c r="C18" s="5" t="str">
-        <v>Intelligent Granite Pants</v>
+        <v>Sleek Granite Towels</v>
       </c>
       <c r="D18" s="5" t="str">
-        <v>1.4.8</v>
+        <v>7.3.9</v>
       </c>
       <c r="E18" s="5" t="str">
-        <v>March</v>
+        <v>November</v>
       </c>
       <c r="F18" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G18" s="5">
-        <v>18</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" ht="30" customHeight="1">
       <c r="A19" s="4" t="str">
-        <v>9accfe7c-04f6-471d-851a-ce2d7b0a2abc</v>
+        <v>922411c6-e50b-418c-9f33-f7299601fa71</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>44745ea0-e6b3-4242-a1f5-45a09d35eff0</v>
+        <v>98bb6d17-c7a5-4aca-bbe8-32eac5a359d3</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v>Bespoke Soft Mouse</v>
+        <v>Bespoke Cotton Chicken</v>
       </c>
       <c r="D19" s="5" t="str">
-        <v>1.2.1</v>
+        <v>1.7.4</v>
       </c>
       <c r="E19" s="5" t="str">
         <v>November</v>
@@ -927,205 +927,205 @@
         <v>2023</v>
       </c>
       <c r="G19" s="5">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" ht="30" customHeight="1">
       <c r="A20" s="4" t="str">
-        <v>3db02bb8-36ec-42cb-bb39-fc92fcf9cc1a</v>
+        <v>9aa3c325-0046-4283-8fca-756b6f0dad8e</v>
       </c>
       <c r="B20" s="5" t="str">
-        <v>6b96921f-bfc5-482d-b457-00ee378b6f96</v>
+        <v>5bee1d03-d877-4b1e-90e3-bb8eda6eb5b5</v>
       </c>
       <c r="C20" s="5" t="str">
-        <v>Modern Concrete Shoes</v>
+        <v>Tasty Metal Tuna</v>
       </c>
       <c r="D20" s="5" t="str">
-        <v>2.6.7</v>
+        <v>4.3.6</v>
       </c>
       <c r="E20" s="5" t="str">
-        <v>January</v>
+        <v>July</v>
       </c>
       <c r="F20" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G20" s="5">
-        <v>9</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" ht="30" customHeight="1">
       <c r="A21" s="4" t="str">
-        <v>a1a3d806-2c5f-42f5-8a3c-01738b5feb8e</v>
+        <v>d0d24664-fe48-40f2-9487-c99a464d3859</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>dba6a833-a555-4a62-b3f1-2b8d74fcd6f1</v>
+        <v>ea8e2653-2c97-4537-ae05-ad5873163bcf</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v>Ergonomic Cotton Chips</v>
+        <v>Sleek Cotton Table</v>
       </c>
       <c r="D21" s="5" t="str">
-        <v>6.9.2</v>
+        <v>1.8.5</v>
       </c>
       <c r="E21" s="5" t="str">
-        <v>August</v>
+        <v>April</v>
       </c>
       <c r="F21" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G21" s="5">
-        <v>78</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" ht="30" customHeight="1">
       <c r="A22" s="4" t="str">
-        <v>fdb8e690-33c9-4e94-b21a-0bd575946e15</v>
+        <v>1190278c-f8ab-4691-aa8d-76af5b6ad762</v>
       </c>
       <c r="B22" s="5" t="str">
-        <v>5f928dee-c9bd-44df-9c46-5b432283e3e6</v>
+        <v>ab454ed0-926f-43ce-9bb9-f5b48cd30f8a</v>
       </c>
       <c r="C22" s="5" t="str">
-        <v>Awesome Metal Chair</v>
+        <v>Fantastic Frozen Bacon</v>
       </c>
       <c r="D22" s="5" t="str">
-        <v>0.4.2</v>
+        <v>3.7.6</v>
       </c>
       <c r="E22" s="5" t="str">
-        <v>January</v>
+        <v>December</v>
       </c>
       <c r="F22" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G22" s="5">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" ht="30" customHeight="1">
       <c r="A23" s="4" t="str">
-        <v>d4f05cc6-d166-4306-aba3-965f8d1b820a</v>
+        <v>00b2df4f-2605-48fe-88e8-a6b09fb8d17e</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>eeb5e986-34a7-464e-b2c4-f45ef6aae529</v>
+        <v>f960c12a-821f-4c21-99f8-ed0e697604a8</v>
       </c>
       <c r="C23" s="5" t="str">
-        <v>Oriental Metal Sausages</v>
+        <v>Awesome Bronze Cheese</v>
       </c>
       <c r="D23" s="5" t="str">
-        <v>1.4.7</v>
+        <v>3.0.7</v>
       </c>
       <c r="E23" s="5" t="str">
-        <v>February</v>
+        <v>June</v>
       </c>
       <c r="F23" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G23" s="5">
-        <v>76</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" ht="30" customHeight="1">
       <c r="A24" s="4" t="str">
-        <v>37efafdb-7424-48ea-8cd8-6a2d8b272943</v>
+        <v>f75b4d26-5299-4f91-90a2-a77d90363b4e</v>
       </c>
       <c r="B24" s="5" t="str">
-        <v>f7c819b5-0d3c-42ff-9b27-6c5b03ece414</v>
+        <v>f7f61878-b1b0-4018-ae84-e8a5bf621009</v>
       </c>
       <c r="C24" s="5" t="str">
-        <v>Electronic Wooden Salad</v>
+        <v>Generic Cotton Gloves</v>
       </c>
       <c r="D24" s="5" t="str">
-        <v>0.6.7</v>
+        <v>1.4.6</v>
       </c>
       <c r="E24" s="5" t="str">
-        <v>January</v>
+        <v>June</v>
       </c>
       <c r="F24" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G24" s="5">
-        <v>9</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" ht="30" customHeight="1">
       <c r="A25" s="4" t="str">
-        <v>f151d0f4-4985-4048-9ae0-92db2cb4a316</v>
+        <v>d77464c4-d79f-4214-a2f9-062364889f1c</v>
       </c>
       <c r="B25" s="5" t="str">
-        <v>809ef6aa-ec5e-4b67-ada2-b1e48647fbb1</v>
+        <v>aaa93b2c-f22a-497f-a0f3-b27376e1d0fa</v>
       </c>
       <c r="C25" s="5" t="str">
-        <v>Recycled Wooden Ball</v>
+        <v>Electronic Cotton Pants</v>
       </c>
       <c r="D25" s="5" t="str">
-        <v>9.6.4</v>
+        <v>0.7.7</v>
       </c>
       <c r="E25" s="5" t="str">
-        <v>September</v>
+        <v>October</v>
       </c>
       <c r="F25" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G25" s="5">
-        <v>8</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1">
       <c r="A26" s="4" t="str">
-        <v>56efecc0-38ab-4944-b040-ff800f1f5a73</v>
+        <v>4fad16fc-f565-4f77-97a5-ddf5848469c7</v>
       </c>
       <c r="B26" s="5" t="str">
-        <v>dfdb21af-0a10-4b2b-9b35-fb1fb58c6150</v>
+        <v>6766109a-adbc-4c8d-9fc5-21b095614ea3</v>
       </c>
       <c r="C26" s="5" t="str">
-        <v>Intelligent Wooden Fish</v>
+        <v>Ergonomic Concrete Mouse</v>
       </c>
       <c r="D26" s="5" t="str">
-        <v>8.2.3</v>
+        <v>0.9.9</v>
       </c>
       <c r="E26" s="5" t="str">
-        <v>January</v>
+        <v>August</v>
       </c>
       <c r="F26" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G26" s="5">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1">
       <c r="A27" s="4" t="str">
-        <v>e8742a3f-bd06-400e-b9ec-2546f0dd5832</v>
+        <v>469c337c-c369-48e2-8215-9399f4f9072c</v>
       </c>
       <c r="B27" s="5" t="str">
-        <v>3faf2455-f806-472b-8df3-252c63a9c4a4</v>
+        <v>64035d32-dcde-4922-aa9a-6c2bf40602e7</v>
       </c>
       <c r="C27" s="5" t="str">
-        <v>Gorgeous Plastic Keyboard</v>
+        <v>Handmade Soft Fish</v>
       </c>
       <c r="D27" s="5" t="str">
-        <v>5.0.4</v>
+        <v>9.7.4</v>
       </c>
       <c r="E27" s="5" t="str">
-        <v>June</v>
+        <v>October</v>
       </c>
       <c r="F27" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G27" s="5">
-        <v>88</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1">
       <c r="A28" s="4" t="str">
-        <v>c15e6791-d621-47b0-8d6b-347896e2ff19</v>
+        <v>910e8d1f-563b-467a-852e-146318eb81a1</v>
       </c>
       <c r="B28" s="5" t="str">
-        <v>eb59ebb8-add7-4fb1-8c0a-502dc61313df</v>
+        <v>e77fa4c3-7025-47e8-a81e-cf89e5e23752</v>
       </c>
       <c r="C28" s="5" t="str">
-        <v>Generic Granite Mouse</v>
+        <v>Oriental Cotton Mouse</v>
       </c>
       <c r="D28" s="5" t="str">
-        <v>2.9.0</v>
+        <v>9.8.1</v>
       </c>
       <c r="E28" s="5" t="str">
         <v>March</v>
@@ -1134,297 +1134,297 @@
         <v>2023</v>
       </c>
       <c r="G28" s="5">
-        <v>88</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1">
       <c r="A29" s="4" t="str">
-        <v>3e03a555-5cb2-4a04-b121-31e2da985f48</v>
+        <v>8ea529e5-9fa3-4085-940c-618cb66b3092</v>
       </c>
       <c r="B29" s="5" t="str">
-        <v>cbaf0dc0-3099-408c-ac1f-ad4c94adef5f</v>
+        <v>6e2fc46f-8e17-4cb4-a929-49fdc8fdc11b</v>
       </c>
       <c r="C29" s="5" t="str">
-        <v>Ergonomic Bronze Bacon</v>
+        <v>Intelligent Cotton Bacon</v>
       </c>
       <c r="D29" s="5" t="str">
-        <v>1.4.6</v>
+        <v>4.5.9</v>
       </c>
       <c r="E29" s="5" t="str">
-        <v>August</v>
+        <v>October</v>
       </c>
       <c r="F29" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G29" s="5">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1">
       <c r="A30" s="4" t="str">
-        <v>0face167-dd7c-4191-bdc2-c77eccdd31a0</v>
+        <v>2451dd7e-be89-4b51-8828-ab3064aa4e7e</v>
       </c>
       <c r="B30" s="5" t="str">
-        <v>6cc86293-11b9-489b-bb62-bfba9046c772</v>
+        <v>cbd76ec6-419d-4060-956a-eba49e05f53e</v>
       </c>
       <c r="C30" s="5" t="str">
-        <v>Handmade Granite Shirt</v>
+        <v>Elegant Frozen Soap</v>
       </c>
       <c r="D30" s="5" t="str">
-        <v>2.1.0</v>
+        <v>6.3.9</v>
       </c>
       <c r="E30" s="5" t="str">
-        <v>December</v>
+        <v>May</v>
       </c>
       <c r="F30" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G30" s="5">
-        <v>6</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1">
       <c r="A31" s="4" t="str">
-        <v>f0d35023-9fa4-4c25-ba96-766f00454392</v>
+        <v>035322d1-2b3e-44fc-a0dc-6124caa5cb36</v>
       </c>
       <c r="B31" s="5" t="str">
-        <v>415ad78b-368a-4de3-ac60-b8e1c5db8465</v>
+        <v>c8398680-0428-4d8b-8998-c6caf21d76b1</v>
       </c>
       <c r="C31" s="5" t="str">
-        <v>Unbranded Frozen Hat</v>
+        <v>Rustic Wooden Towels</v>
       </c>
       <c r="D31" s="5" t="str">
-        <v>1.7.9</v>
+        <v>4.7.9</v>
       </c>
       <c r="E31" s="5" t="str">
-        <v>December</v>
+        <v>July</v>
       </c>
       <c r="F31" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G31" s="5">
-        <v>49</v>
+        <v>30</v>
       </c>
     </row>
     <row r="32" ht="30" customHeight="1">
       <c r="A32" s="4" t="str">
-        <v>b8494af2-3ade-4877-ba4d-27e763b80b79</v>
+        <v>2bcb622a-8c2d-42bf-b6d6-66f328cc3800</v>
       </c>
       <c r="B32" s="5" t="str">
-        <v>a7204bc1-5f83-4fad-a6c1-141a53f76325</v>
+        <v>e6152fe5-3374-46e7-b9d2-9ae15409c7f5</v>
       </c>
       <c r="C32" s="5" t="str">
-        <v>Bespoke Wooden Bacon</v>
+        <v>Rustic Frozen Chicken</v>
       </c>
       <c r="D32" s="5" t="str">
-        <v>7.5.1</v>
+        <v>1.8.8</v>
       </c>
       <c r="E32" s="5" t="str">
-        <v>April</v>
+        <v>February</v>
       </c>
       <c r="F32" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G32" s="5">
-        <v>39</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" ht="30" customHeight="1">
       <c r="A33" s="4" t="str">
-        <v>e4e99380-13d5-4fba-b34c-f4f5579b8fbb</v>
+        <v>9dfecbec-e53d-419d-8e5b-e139bc6682fe</v>
       </c>
       <c r="B33" s="5" t="str">
-        <v>b8f40757-1882-454b-9b38-e1a1e11efd20</v>
+        <v>02fba024-2f6c-4772-97ee-368132e411a9</v>
       </c>
       <c r="C33" s="5" t="str">
-        <v>Electronic Plastic Shirt</v>
+        <v>Elegant Plastic Fish</v>
       </c>
       <c r="D33" s="5" t="str">
-        <v>0.0.1</v>
+        <v>5.7.1</v>
       </c>
       <c r="E33" s="5" t="str">
-        <v>November</v>
+        <v>March</v>
       </c>
       <c r="F33" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G33" s="5">
-        <v>3</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1">
       <c r="A34" s="4" t="str">
-        <v>c615194e-298a-4d22-9390-b6eea76efbe5</v>
+        <v>9ce4627e-6ad4-4ecf-915e-34f8edbb5114</v>
       </c>
       <c r="B34" s="5" t="str">
-        <v>246468f6-bfb2-4081-988e-0d6c8a80946b</v>
+        <v>84b8e0f6-7a4c-4f2d-8683-27838e826a22</v>
       </c>
       <c r="C34" s="5" t="str">
-        <v>Intelligent Steel Gloves</v>
+        <v>Luxurious Bronze Cheese</v>
       </c>
       <c r="D34" s="5" t="str">
-        <v>6.7.4</v>
+        <v>6.6.1</v>
       </c>
       <c r="E34" s="5" t="str">
-        <v>January</v>
+        <v>May</v>
       </c>
       <c r="F34" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G34" s="5">
-        <v>18</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" ht="30" customHeight="1">
       <c r="A35" s="4" t="str">
-        <v>fc34374e-cef6-4c7e-a57f-babb380b96c6</v>
+        <v>df9c8217-e982-47a7-9e4c-76a309ab5337</v>
       </c>
       <c r="B35" s="5" t="str">
-        <v>d96e6ac1-207a-431e-b77c-f157e8831626</v>
+        <v>28b8dcc3-1696-4cd0-9911-ffe9d4dd38a5</v>
       </c>
       <c r="C35" s="5" t="str">
-        <v>Oriental Bronze Mouse</v>
+        <v>Awesome Rubber Sausages</v>
       </c>
       <c r="D35" s="5" t="str">
-        <v>2.4.3</v>
+        <v>0.0.8</v>
       </c>
       <c r="E35" s="5" t="str">
         <v>July</v>
       </c>
       <c r="F35" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G35" s="5">
-        <v>66</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" ht="30" customHeight="1">
       <c r="A36" s="4" t="str">
-        <v>2947603b-cdf7-4a7b-a218-65915b1eb452</v>
+        <v>8c271c88-be22-4c92-a20a-b1226d577d59</v>
       </c>
       <c r="B36" s="5" t="str">
-        <v>99b2d55f-62e5-4bb5-bff7-72b24d3a1ba4</v>
+        <v>479887c4-18e5-4670-8b24-05c134c6c55d</v>
       </c>
       <c r="C36" s="5" t="str">
-        <v>Unbranded Soft Soap</v>
+        <v>Sleek Granite Shoes</v>
       </c>
       <c r="D36" s="5" t="str">
-        <v>8.2.2</v>
+        <v>3.7.2</v>
       </c>
       <c r="E36" s="5" t="str">
-        <v>May</v>
+        <v>January</v>
       </c>
       <c r="F36" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G36" s="5">
-        <v>18</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" ht="30" customHeight="1">
       <c r="A37" s="4" t="str">
-        <v>0d53e056-89aa-48c6-a175-11ba8deec375</v>
+        <v>b4e4b1da-7c67-4a05-b3eb-c7de32125b4e</v>
       </c>
       <c r="B37" s="5" t="str">
-        <v>2cc57d5a-aaa4-48bb-94c4-e34b884a9980</v>
+        <v>2186c89a-2dad-40f7-960f-2a333ea58127</v>
       </c>
       <c r="C37" s="5" t="str">
-        <v>Elegant Rubber Table</v>
+        <v>Generic Frozen Salad</v>
       </c>
       <c r="D37" s="5" t="str">
-        <v>7.8.4</v>
+        <v>7.1.2</v>
       </c>
       <c r="E37" s="5" t="str">
-        <v>December</v>
+        <v>January</v>
       </c>
       <c r="F37" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G37" s="5">
-        <v>96</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" ht="30" customHeight="1">
       <c r="A38" s="4" t="str">
-        <v>cb26eb8e-1228-43a4-b505-02534ddd7897</v>
+        <v>b0b41839-f14a-4fa1-af28-7166aa923b89</v>
       </c>
       <c r="B38" s="5" t="str">
-        <v>c680e38a-2974-43a3-924a-c2cff1adb465</v>
+        <v>2eb5fbeb-4488-45e2-8814-fe3409afc6e0</v>
       </c>
       <c r="C38" s="5" t="str">
-        <v>Bespoke Bronze Shoes</v>
+        <v>Oriental Plastic Chair</v>
       </c>
       <c r="D38" s="5" t="str">
-        <v>1.2.0</v>
+        <v>5.9.2</v>
       </c>
       <c r="E38" s="5" t="str">
-        <v>October</v>
+        <v>January</v>
       </c>
       <c r="F38" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G38" s="5">
-        <v>16</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" ht="30" customHeight="1">
       <c r="A39" s="4" t="str">
-        <v>b3687404-00e1-46d7-8a3d-bffe257bae70</v>
+        <v>86440df6-456c-4b4b-89bf-2005b19272b4</v>
       </c>
       <c r="B39" s="5" t="str">
-        <v>574949c1-42a8-4a22-9c34-ff6038290253</v>
+        <v>75fff9da-9548-4471-8750-3da51097a35c</v>
       </c>
       <c r="C39" s="5" t="str">
-        <v>Incredible Wooden Ball</v>
+        <v>Bespoke Bronze Tuna</v>
       </c>
       <c r="D39" s="5" t="str">
-        <v>5.3.3</v>
+        <v>9.1.3</v>
       </c>
       <c r="E39" s="5" t="str">
-        <v>December</v>
+        <v>October</v>
       </c>
       <c r="F39" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G39" s="5">
-        <v>4</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" ht="30" customHeight="1">
       <c r="A40" s="4" t="str">
-        <v>e9b98180-d56c-40dd-bf75-3970ade9e7e2</v>
+        <v>19085622-b8a0-4fcc-b102-c8ce1fdee17b</v>
       </c>
       <c r="B40" s="5" t="str">
-        <v>cec197c1-509f-4654-8f6a-045f1f042aa9</v>
+        <v>12b12ca1-8456-4121-8e6b-14c162a45ffa</v>
       </c>
       <c r="C40" s="5" t="str">
-        <v>Gorgeous Granite Table</v>
+        <v>Bespoke Steel Tuna</v>
       </c>
       <c r="D40" s="5" t="str">
-        <v>3.2.7</v>
+        <v>7.5.2</v>
       </c>
       <c r="E40" s="5" t="str">
-        <v>November</v>
+        <v>January</v>
       </c>
       <c r="F40" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G40" s="5">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" ht="30" customHeight="1">
       <c r="A41" s="4" t="str">
-        <v>b7b2db2b-85c0-4ae4-82ad-ba2ffef5176a</v>
+        <v>6acf9a91-8a16-467b-9ac4-2c211f3d5781</v>
       </c>
       <c r="B41" s="5" t="str">
-        <v>4e30dceb-3001-43a6-9e6f-7d63fde811d2</v>
+        <v>0a4cb599-47a1-48fb-a95d-87246af5c1dc</v>
       </c>
       <c r="C41" s="5" t="str">
-        <v>Rustic Steel Chips</v>
+        <v>Licensed Fresh Mouse</v>
       </c>
       <c r="D41" s="5" t="str">
-        <v>0.7.6</v>
+        <v>3.0.5</v>
       </c>
       <c r="E41" s="5" t="str">
         <v>May</v>
@@ -1433,458 +1433,458 @@
         <v>2023</v>
       </c>
       <c r="G41" s="5">
-        <v>73</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" ht="30" customHeight="1">
       <c r="A42" s="4" t="str">
-        <v>b6b2d760-86cf-4579-98b4-407337b67633</v>
+        <v>2a13cc6e-d2ab-4795-91a7-fdca90e55cf1</v>
       </c>
       <c r="B42" s="5" t="str">
-        <v>94c63d30-e894-4e3a-9075-8fbb31b0e36a</v>
+        <v>c68a70f3-cdb3-4421-a7e2-f75ee152ee16</v>
       </c>
       <c r="C42" s="5" t="str">
-        <v>Incredible Concrete Gloves</v>
+        <v>Licensed Cotton Bacon</v>
       </c>
       <c r="D42" s="5" t="str">
-        <v>7.1.1</v>
+        <v>3.1.0</v>
       </c>
       <c r="E42" s="5" t="str">
-        <v>June</v>
+        <v>April</v>
       </c>
       <c r="F42" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G42" s="5">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" ht="30" customHeight="1">
       <c r="A43" s="4" t="str">
-        <v>4d691353-57eb-4e79-902e-6a0c4b910e5c</v>
+        <v>9ff8f035-d621-4e0c-80f2-b09f9261a83c</v>
       </c>
       <c r="B43" s="5" t="str">
-        <v>eb8dc61c-a55b-449e-8383-52a1b90e3acc</v>
+        <v>6b5d42cd-faa0-4c63-9ded-771b9a7d08a2</v>
       </c>
       <c r="C43" s="5" t="str">
-        <v>Elegant Bronze Hat</v>
+        <v>Incredible Rubber Computer</v>
       </c>
       <c r="D43" s="5" t="str">
-        <v>2.6.1</v>
+        <v>4.6.7</v>
       </c>
       <c r="E43" s="5" t="str">
-        <v>November</v>
+        <v>April</v>
       </c>
       <c r="F43" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G43" s="5">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" ht="30" customHeight="1">
       <c r="A44" s="4" t="str">
-        <v>5eaf8e9d-4f38-4c66-90e4-5b47a55c638b</v>
+        <v>95c42a11-594e-4e9c-9823-e4330749ca7c</v>
       </c>
       <c r="B44" s="5" t="str">
-        <v>a75122ad-5e68-4302-b962-b5d6cfa1e1b0</v>
+        <v>f4a62b14-c465-4899-8b52-3b3d0aebda22</v>
       </c>
       <c r="C44" s="5" t="str">
-        <v>Intelligent Frozen Sausages</v>
+        <v>Handcrafted Metal Shoes</v>
       </c>
       <c r="D44" s="5" t="str">
-        <v>5.0.4</v>
+        <v>5.6.3</v>
       </c>
       <c r="E44" s="5" t="str">
-        <v>March</v>
+        <v>October</v>
       </c>
       <c r="F44" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G44" s="5">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" ht="30" customHeight="1">
       <c r="A45" s="4" t="str">
-        <v>a90032cb-c628-4e7b-87e1-742106f895ac</v>
+        <v>8e339dde-8f79-44ae-9afc-003372990729</v>
       </c>
       <c r="B45" s="5" t="str">
-        <v>5099f4da-1616-4833-a68d-190a54c19758</v>
+        <v>af2038c2-53ea-4917-94f6-e53d16d9cc70</v>
       </c>
       <c r="C45" s="5" t="str">
-        <v>Incredible Bronze Mouse</v>
+        <v>Awesome Cotton Hat</v>
       </c>
       <c r="D45" s="5" t="str">
-        <v>0.7.7</v>
+        <v>1.5.5</v>
       </c>
       <c r="E45" s="5" t="str">
-        <v>August</v>
+        <v>April</v>
       </c>
       <c r="F45" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G45" s="5">
-        <v>19</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" ht="30" customHeight="1">
       <c r="A46" s="4" t="str">
-        <v>7a662766-1d33-4674-b3d5-cdb1981561ba</v>
+        <v>4582024b-c942-4170-8cac-8db9f2c21f4f</v>
       </c>
       <c r="B46" s="5" t="str">
-        <v>93499cf8-ea66-49c5-ad25-d29f2c1a1389</v>
+        <v>868e9bfd-709f-4f01-87c4-71279414c224</v>
       </c>
       <c r="C46" s="5" t="str">
-        <v>Rustic Rubber Salad</v>
+        <v>Incredible Rubber Tuna</v>
       </c>
       <c r="D46" s="5" t="str">
-        <v>3.7.9</v>
+        <v>4.5.8</v>
       </c>
       <c r="E46" s="5" t="str">
-        <v>June</v>
+        <v>December</v>
       </c>
       <c r="F46" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G46" s="5">
-        <v>29</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" ht="30" customHeight="1">
       <c r="A47" s="4" t="str">
-        <v>f08229c6-f788-4a3e-96eb-95af974cdd76</v>
+        <v>9658c0a5-593c-45bf-8e02-239ef9db0797</v>
       </c>
       <c r="B47" s="5" t="str">
-        <v>29b31b44-617a-4f4e-a4f7-e3e89009bbe4</v>
+        <v>81fd269b-9fc9-45e8-9d4e-506d34ab9d96</v>
       </c>
       <c r="C47" s="5" t="str">
-        <v>Awesome Soft Car</v>
+        <v>Sleek Bronze Shirt</v>
       </c>
       <c r="D47" s="5" t="str">
-        <v>4.5.6</v>
+        <v>6.6.5</v>
       </c>
       <c r="E47" s="5" t="str">
-        <v>April</v>
+        <v>June</v>
       </c>
       <c r="F47" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G47" s="5">
-        <v>8</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" ht="30" customHeight="1">
       <c r="A48" s="4" t="str">
-        <v>e15c5d19-b53a-472d-a36b-c342ee561d32</v>
+        <v>63c1b211-2bb8-47d9-ae97-ebd7d9430d96</v>
       </c>
       <c r="B48" s="5" t="str">
-        <v>535b4f39-42f7-43f3-940f-83012c2e92b2</v>
+        <v>2ee820db-ad6f-4e85-8a7e-48322a1cf4f8</v>
       </c>
       <c r="C48" s="5" t="str">
-        <v>Handcrafted Plastic Cheese</v>
+        <v>Ergonomic Frozen Chips</v>
       </c>
       <c r="D48" s="5" t="str">
-        <v>2.0.9</v>
+        <v>3.9.1</v>
       </c>
       <c r="E48" s="5" t="str">
-        <v>May</v>
+        <v>July</v>
       </c>
       <c r="F48" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G48" s="5">
-        <v>48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" ht="30" customHeight="1">
       <c r="A49" s="4" t="str">
-        <v>b827a291-5c7b-4f01-9168-cb7b06025d1a</v>
+        <v>835276e0-0beb-4343-9b3f-f831c7702f29</v>
       </c>
       <c r="B49" s="5" t="str">
-        <v>54c79f73-e331-4ae9-8850-2c167c48d638</v>
+        <v>05730539-bbc6-4320-b44a-34cae1032960</v>
       </c>
       <c r="C49" s="5" t="str">
-        <v>Incredible Fresh Hat</v>
+        <v>Bespoke Steel Tuna</v>
       </c>
       <c r="D49" s="5" t="str">
-        <v>9.1.0</v>
+        <v>9.3.8</v>
       </c>
       <c r="E49" s="5" t="str">
-        <v>November</v>
+        <v>December</v>
       </c>
       <c r="F49" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G49" s="5">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" ht="30" customHeight="1">
       <c r="A50" s="4" t="str">
-        <v>ca22f663-1883-4ba5-a303-aa9dfb738cba</v>
+        <v>5bd7b32e-2ef3-4d89-8c40-1789d7962159</v>
       </c>
       <c r="B50" s="5" t="str">
-        <v>b082606d-8612-45a7-a96c-b18eb521fe70</v>
+        <v>601be037-f587-40fb-bedf-786604c27560</v>
       </c>
       <c r="C50" s="5" t="str">
-        <v>Awesome Plastic Towels</v>
+        <v>Handmade Concrete Ball</v>
       </c>
       <c r="D50" s="5" t="str">
-        <v>7.9.2</v>
+        <v>1.1.9</v>
       </c>
       <c r="E50" s="5" t="str">
-        <v>November</v>
+        <v>August</v>
       </c>
       <c r="F50" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G50" s="5">
-        <v>85</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" ht="30" customHeight="1">
       <c r="A51" s="4" t="str">
-        <v>4386198d-8975-4344-a504-9264d6dc9a50</v>
+        <v>354d29ed-0e29-4048-a85d-d5023a8f5c55</v>
       </c>
       <c r="B51" s="5" t="str">
-        <v>77016565-3ab7-4b5d-98ec-67dc456e38a7</v>
+        <v>66691758-eecd-43ac-9dab-2e9d5ee93c98</v>
       </c>
       <c r="C51" s="5" t="str">
-        <v>Ergonomic Granite Chicken</v>
+        <v>Electronic Bronze Pizza</v>
       </c>
       <c r="D51" s="5" t="str">
-        <v>3.6.7</v>
+        <v>5.0.9</v>
       </c>
       <c r="E51" s="5" t="str">
-        <v>October</v>
+        <v>March</v>
       </c>
       <c r="F51" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G51" s="5">
-        <v>37</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" ht="30" customHeight="1">
       <c r="A52" s="4" t="str">
-        <v>e257d8bf-9b1a-4600-bcba-443f17e81bfb</v>
+        <v>eefe644c-2a72-48e8-856d-54f1e4ebe67e</v>
       </c>
       <c r="B52" s="5" t="str">
-        <v>58f33690-d08b-4ddf-8430-245854111a0e</v>
+        <v>c563c30f-0053-4a36-a1fe-cee07bcdfee5</v>
       </c>
       <c r="C52" s="5" t="str">
-        <v>Electronic Metal Table</v>
+        <v>Luxurious Wooden Bacon</v>
       </c>
       <c r="D52" s="5" t="str">
-        <v>7.8.7</v>
+        <v>8.8.0</v>
       </c>
       <c r="E52" s="5" t="str">
-        <v>July</v>
+        <v>November</v>
       </c>
       <c r="F52" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G52" s="5">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="53" ht="30" customHeight="1">
       <c r="A53" s="4" t="str">
-        <v>eb5afbe6-efbd-4b84-9755-61ca88fd41f1</v>
+        <v>c3bc06f7-7440-4981-9c5e-9639f302d439</v>
       </c>
       <c r="B53" s="5" t="str">
-        <v>49a61550-0a73-475e-b333-6e7b60fa6426</v>
+        <v>464f7767-68c5-4152-bace-76b6249206f3</v>
       </c>
       <c r="C53" s="5" t="str">
-        <v>Gorgeous Metal Chips</v>
+        <v>Incredible Cotton Gloves</v>
       </c>
       <c r="D53" s="5" t="str">
-        <v>6.8.0</v>
+        <v>4.9.5</v>
       </c>
       <c r="E53" s="5" t="str">
-        <v>December</v>
+        <v>March</v>
       </c>
       <c r="F53" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G53" s="5">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" ht="30" customHeight="1">
       <c r="A54" s="4" t="str">
-        <v>b73813b8-31ca-47c7-a43c-34c62f2d3fcb</v>
+        <v>2c7ff04c-1c15-4a12-9874-e55b15f72067</v>
       </c>
       <c r="B54" s="5" t="str">
-        <v>d054d84a-a6b2-4268-86ee-0f6985d2f447</v>
+        <v>6821cfb6-0a38-4545-b403-c0409c58e171</v>
       </c>
       <c r="C54" s="5" t="str">
-        <v>Elegant Frozen Pants</v>
+        <v>Refined Soft Chair</v>
       </c>
       <c r="D54" s="5" t="str">
-        <v>6.8.6</v>
+        <v>4.2.9</v>
       </c>
       <c r="E54" s="5" t="str">
-        <v>January</v>
+        <v>July</v>
       </c>
       <c r="F54" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G54" s="5">
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" ht="30" customHeight="1">
       <c r="A55" s="4" t="str">
-        <v>44f232b4-1437-48f1-bc9c-0b0d6e9e1be2</v>
+        <v>6be3a530-c846-4023-b43d-4e51834973ab</v>
       </c>
       <c r="B55" s="5" t="str">
-        <v>da31843b-fcb8-449b-81df-acce3f65888e</v>
+        <v>2ae66705-c7e7-4a4d-9f06-dee91eb71a99</v>
       </c>
       <c r="C55" s="5" t="str">
-        <v>Fantastic Cotton Table</v>
+        <v>Handcrafted Steel Soap</v>
       </c>
       <c r="D55" s="5" t="str">
-        <v>8.4.6</v>
+        <v>2.3.1</v>
       </c>
       <c r="E55" s="5" t="str">
-        <v>January</v>
+        <v>May</v>
       </c>
       <c r="F55" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G55" s="5">
-        <v>9</v>
+        <v>98</v>
       </c>
     </row>
     <row r="56" ht="30" customHeight="1">
       <c r="A56" s="4" t="str">
-        <v>a1a17f57-2cb8-4d99-b97d-46b8bf2d14e9</v>
+        <v>e99de7fc-4e8a-4679-9a8b-0bc1c868e178</v>
       </c>
       <c r="B56" s="5" t="str">
-        <v>e927311f-c53c-4a97-bcb5-3c1565380f06</v>
+        <v>1234be2b-63cb-4234-80e9-0d60704badcb</v>
       </c>
       <c r="C56" s="5" t="str">
-        <v>Practical Steel Soap</v>
+        <v>Sleek Bronze Hat</v>
       </c>
       <c r="D56" s="5" t="str">
-        <v>5.2.3</v>
+        <v>2.1.8</v>
       </c>
       <c r="E56" s="5" t="str">
-        <v>May</v>
+        <v>August</v>
       </c>
       <c r="F56" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G56" s="5">
-        <v>95</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57" ht="30" customHeight="1">
       <c r="A57" s="4" t="str">
-        <v>ad925850-7100-4ad5-a4b4-7bdd24400275</v>
+        <v>6db81d20-df88-435a-8dda-2ffae21d4378</v>
       </c>
       <c r="B57" s="5" t="str">
-        <v>12d571f2-fe98-4fd2-8f8e-cc89f1f875cf</v>
+        <v>870e2722-a807-4e47-aca7-c8de8491eda8</v>
       </c>
       <c r="C57" s="5" t="str">
-        <v>Bespoke Concrete Computer</v>
+        <v>Tasty Bronze Chips</v>
       </c>
       <c r="D57" s="5" t="str">
-        <v>0.4.9</v>
+        <v>5.4.0</v>
       </c>
       <c r="E57" s="5" t="str">
-        <v>October</v>
+        <v>February</v>
       </c>
       <c r="F57" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G57" s="5">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" ht="30" customHeight="1">
       <c r="A58" s="4" t="str">
-        <v>68f242c9-8c8e-4fed-86b8-0d14ac22f5cd</v>
+        <v>e37ecee1-7e79-4c3c-9ff1-04847b9b5b2d</v>
       </c>
       <c r="B58" s="5" t="str">
-        <v>88395f36-0805-4727-ba55-7cf125002961</v>
+        <v>8dc14153-5bf4-4239-a7b2-e703e01cca54</v>
       </c>
       <c r="C58" s="5" t="str">
-        <v>Incredible Wooden Pants</v>
+        <v>Electronic Steel Bacon</v>
       </c>
       <c r="D58" s="5" t="str">
-        <v>3.2.0</v>
+        <v>6.7.6</v>
       </c>
       <c r="E58" s="5" t="str">
-        <v>April</v>
+        <v>August</v>
       </c>
       <c r="F58" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G58" s="5">
-        <v>23</v>
+        <v>74</v>
       </c>
     </row>
     <row r="59" ht="30" customHeight="1">
       <c r="A59" s="4" t="str">
-        <v>e32c2402-d518-4639-9548-d7bee2930fb3</v>
+        <v>aa14a90f-e164-4149-b040-439acd5e5263</v>
       </c>
       <c r="B59" s="5" t="str">
-        <v>f328130e-7530-496a-8b47-c2d61b7b7aa6</v>
+        <v>1e6f07ad-8868-4a1c-94d1-d2c7ec35e998</v>
       </c>
       <c r="C59" s="5" t="str">
-        <v>Sleek Fresh Shoes</v>
+        <v>Luxurious Bronze Pants</v>
       </c>
       <c r="D59" s="5" t="str">
-        <v>3.8.3</v>
+        <v>7.9.2</v>
       </c>
       <c r="E59" s="5" t="str">
-        <v>May</v>
+        <v>July</v>
       </c>
       <c r="F59" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G59" s="5">
-        <v>35</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" ht="30" customHeight="1">
       <c r="A60" s="4" t="str">
-        <v>0b11173b-b904-448c-88d3-eca658be6144</v>
+        <v>914f4dc3-aa63-4581-b397-609fbdfb5dfb</v>
       </c>
       <c r="B60" s="5" t="str">
-        <v>7ed13988-041d-490d-b04c-d19bc4ea7121</v>
+        <v>a4b44115-3484-418e-87e6-779014fe7c1b</v>
       </c>
       <c r="C60" s="5" t="str">
-        <v>Unbranded Metal Towels</v>
+        <v>Bespoke Rubber Bike</v>
       </c>
       <c r="D60" s="5" t="str">
-        <v>2.8.4</v>
+        <v>2.9.7</v>
       </c>
       <c r="E60" s="5" t="str">
         <v>April</v>
       </c>
       <c r="F60" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G60" s="5">
-        <v>73</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61" ht="30" customHeight="1">
       <c r="A61" s="4" t="str">
-        <v>75e7e72f-5695-4226-8169-ed836f635a66</v>
+        <v>24cb97ac-a149-423d-91a4-0da7bf5240e1</v>
       </c>
       <c r="B61" s="5" t="str">
-        <v>3c8d59e2-77eb-498d-b642-dbda3b251ce2</v>
+        <v>0be10113-02d5-4b7c-8108-9cabf501d012</v>
       </c>
       <c r="C61" s="5" t="str">
-        <v>Bespoke Soft Shoes</v>
+        <v>Practical Rubber Chips</v>
       </c>
       <c r="D61" s="5" t="str">
-        <v>4.3.4</v>
+        <v>9.3.5</v>
       </c>
       <c r="E61" s="5" t="str">
         <v>June</v>
@@ -1893,24 +1893,24 @@
         <v>2023</v>
       </c>
       <c r="G61" s="5">
-        <v>34</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" ht="30" customHeight="1">
       <c r="A62" s="4" t="str">
-        <v>efce02b0-acea-418e-aa4b-76a9d50852ee</v>
+        <v>1788bca1-f6ac-496f-b674-6ccbb60cf3b9</v>
       </c>
       <c r="B62" s="5" t="str">
-        <v>9e57e227-4ae8-4fcf-b7d0-08d7304493e0</v>
+        <v>fad00c6a-6e0c-4b80-a8c2-5cce2eb14dc7</v>
       </c>
       <c r="C62" s="5" t="str">
-        <v>Generic Soft Salad</v>
+        <v>Practical Bronze Keyboard</v>
       </c>
       <c r="D62" s="5" t="str">
-        <v>0.4.0</v>
+        <v>1.5.9</v>
       </c>
       <c r="E62" s="5" t="str">
-        <v>February</v>
+        <v>October</v>
       </c>
       <c r="F62" s="5" t="str">
         <v>2023</v>
@@ -1921,292 +1921,292 @@
     </row>
     <row r="63" ht="30" customHeight="1">
       <c r="A63" s="4" t="str">
-        <v>11d21050-5ebf-4e1d-b4be-55a93226314b</v>
+        <v>55b78e92-a715-4f16-bf50-65fd39133ce0</v>
       </c>
       <c r="B63" s="5" t="str">
-        <v>a7c8f260-aea9-43e2-bba2-8a44f448f5d4</v>
+        <v>c0e60052-f4e6-4111-95c2-7d0383237612</v>
       </c>
       <c r="C63" s="5" t="str">
-        <v>Tasty Wooden Mouse</v>
+        <v>Small Frozen Pizza</v>
       </c>
       <c r="D63" s="5" t="str">
-        <v>1.0.2</v>
+        <v>3.7.3</v>
       </c>
       <c r="E63" s="5" t="str">
-        <v>August</v>
+        <v>January</v>
       </c>
       <c r="F63" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G63" s="5">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="64" ht="30" customHeight="1">
       <c r="A64" s="4" t="str">
-        <v>e568bd12-20aa-4efb-b8d8-99533f68a40f</v>
+        <v>6b031a32-fc11-497d-9c26-3bc91a8a47bf</v>
       </c>
       <c r="B64" s="5" t="str">
-        <v>6e44ec93-223c-4780-90da-e3abd50ccba7</v>
+        <v>9d1229b4-7689-4f4f-8192-3b22f4b09a2e</v>
       </c>
       <c r="C64" s="5" t="str">
-        <v>Small Metal Computer</v>
+        <v>Recycled Soft Bacon</v>
       </c>
       <c r="D64" s="5" t="str">
-        <v>1.9.7</v>
+        <v>1.2.2</v>
       </c>
       <c r="E64" s="5" t="str">
-        <v>October</v>
+        <v>February</v>
       </c>
       <c r="F64" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G64" s="5">
-        <v>59</v>
+        <v>79</v>
       </c>
     </row>
     <row r="65" ht="30" customHeight="1">
       <c r="A65" s="4" t="str">
-        <v>690bab2c-82dc-460f-8372-29c068777481</v>
+        <v>749650fa-4da2-48f2-8b5b-23ee3b56843b</v>
       </c>
       <c r="B65" s="5" t="str">
-        <v>61c993f0-a526-413b-84e7-a92d1db48431</v>
+        <v>3381d339-e39a-4a7f-9fe2-c817fb594156</v>
       </c>
       <c r="C65" s="5" t="str">
-        <v>Modern Fresh Bike</v>
+        <v>Electronic Granite Bacon</v>
       </c>
       <c r="D65" s="5" t="str">
-        <v>4.0.7</v>
+        <v>8.0.1</v>
       </c>
       <c r="E65" s="5" t="str">
-        <v>March</v>
+        <v>November</v>
       </c>
       <c r="F65" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G65" s="5">
-        <v>79</v>
+        <v>31</v>
       </c>
     </row>
     <row r="66" ht="30" customHeight="1">
       <c r="A66" s="4" t="str">
-        <v>2b785055-bfb0-4394-8813-470c3f10875f</v>
+        <v>de4507ed-2f68-4e34-b182-bbf29e6a6a7c</v>
       </c>
       <c r="B66" s="5" t="str">
-        <v>4a7980b9-3bf7-402a-8ed6-b899d7e211dd</v>
+        <v>da718708-4f09-418d-bcee-f4d5dd32c291</v>
       </c>
       <c r="C66" s="5" t="str">
-        <v>Intelligent Soft Car</v>
+        <v>Refined Fresh Pizza</v>
       </c>
       <c r="D66" s="5" t="str">
-        <v>4.2.5</v>
+        <v>0.2.9</v>
       </c>
       <c r="E66" s="5" t="str">
-        <v>July</v>
+        <v>June</v>
       </c>
       <c r="F66" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G66" s="5">
-        <v>89</v>
+        <v>33</v>
       </c>
     </row>
     <row r="67" ht="30" customHeight="1">
       <c r="A67" s="4" t="str">
-        <v>f405e57e-858c-41a3-9669-148ee552fcbe</v>
+        <v>ab1963c6-4079-49e8-8c22-42ae676abe51</v>
       </c>
       <c r="B67" s="5" t="str">
-        <v>264465c9-b66b-4033-91cb-cb06ce957283</v>
+        <v>19766afe-ef02-405c-8ed7-dcff903fe400</v>
       </c>
       <c r="C67" s="5" t="str">
-        <v>Ergonomic Plastic Bacon</v>
+        <v>Intelligent Soft Cheese</v>
       </c>
       <c r="D67" s="5" t="str">
-        <v>0.1.6</v>
+        <v>2.2.4</v>
       </c>
       <c r="E67" s="5" t="str">
-        <v>January</v>
+        <v>August</v>
       </c>
       <c r="F67" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G67" s="5">
-        <v>7</v>
+        <v>43</v>
       </c>
     </row>
     <row r="68" ht="30" customHeight="1">
       <c r="A68" s="4" t="str">
-        <v>94ae6816-40d9-4bf0-ae20-2cfdcc8f6d6f</v>
+        <v>56c66691-ae3c-48af-bffa-95336f05c897</v>
       </c>
       <c r="B68" s="5" t="str">
-        <v>a88d58ae-ff3c-4110-92bf-4766c826a628</v>
+        <v>fa557a6e-8e7e-4d74-9bb5-4e897f7d9851</v>
       </c>
       <c r="C68" s="5" t="str">
-        <v>Fantastic Concrete Chips</v>
+        <v>Fantastic Fresh Chicken</v>
       </c>
       <c r="D68" s="5" t="str">
-        <v>2.5.6</v>
+        <v>6.8.8</v>
       </c>
       <c r="E68" s="5" t="str">
-        <v>May</v>
+        <v>December</v>
       </c>
       <c r="F68" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G68" s="5">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="69" ht="30" customHeight="1">
       <c r="A69" s="4" t="str">
-        <v>8ca6206d-1262-4ff6-9121-12e175e4d1ab</v>
+        <v>34499e9b-da5a-4c3f-9dba-55b3c61123d0</v>
       </c>
       <c r="B69" s="5" t="str">
-        <v>296f5341-7c3f-4b4e-8731-a1619070e2bb</v>
+        <v>79636a8b-32e8-4668-b35e-f237ae934eaa</v>
       </c>
       <c r="C69" s="5" t="str">
-        <v>Small Plastic Bacon</v>
+        <v>Generic Bronze Mouse</v>
       </c>
       <c r="D69" s="5" t="str">
-        <v>1.7.4</v>
+        <v>8.6.3</v>
       </c>
       <c r="E69" s="5" t="str">
-        <v>May</v>
+        <v>December</v>
       </c>
       <c r="F69" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G69" s="5">
-        <v>62</v>
+        <v>35</v>
       </c>
     </row>
     <row r="70" ht="30" customHeight="1">
       <c r="A70" s="4" t="str">
-        <v>dc61047f-818a-4bc0-8c9b-319ecd4443a3</v>
+        <v>e0f61352-7910-4ef7-9e79-16724cd0f139</v>
       </c>
       <c r="B70" s="5" t="str">
-        <v>cb7e5536-72ee-4e01-988f-5978951ce765</v>
+        <v>8d3eca56-87c0-4606-9c4e-15efca4c08dd</v>
       </c>
       <c r="C70" s="5" t="str">
-        <v>Tasty Fresh Tuna</v>
+        <v>Elegant Granite Mouse</v>
       </c>
       <c r="D70" s="5" t="str">
-        <v>0.0.6</v>
+        <v>4.1.8</v>
       </c>
       <c r="E70" s="5" t="str">
-        <v>April</v>
+        <v>March</v>
       </c>
       <c r="F70" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G70" s="5">
-        <v>68</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" ht="30" customHeight="1">
       <c r="A71" s="4" t="str">
-        <v>4a473cd8-224d-4ffb-973e-f67855eed595</v>
+        <v>cb43706d-d9e6-4a3f-970e-7037f1dc2351</v>
       </c>
       <c r="B71" s="5" t="str">
-        <v>b24c55cb-cc8b-496b-96b4-b3292def654c</v>
+        <v>03e62f7b-bc6f-4817-98e9-af86e2095afd</v>
       </c>
       <c r="C71" s="5" t="str">
-        <v>Oriental Cotton Pizza</v>
+        <v>Fantastic Plastic Mouse</v>
       </c>
       <c r="D71" s="5" t="str">
-        <v>1.0.1</v>
+        <v>4.8.4</v>
       </c>
       <c r="E71" s="5" t="str">
-        <v>October</v>
+        <v>March</v>
       </c>
       <c r="F71" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G71" s="5">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="72" ht="30" customHeight="1">
       <c r="A72" s="4" t="str">
-        <v>82092278-43c3-4d2d-aba4-ab81e0138aa0</v>
+        <v>bd67d8bc-9ff9-431f-bfd4-a849b5d8e27d</v>
       </c>
       <c r="B72" s="5" t="str">
-        <v>bfc3f0f8-7f2f-40a0-b3c5-af5e8da93faa</v>
+        <v>5f518949-f0f6-4de2-819f-982783395be4</v>
       </c>
       <c r="C72" s="5" t="str">
-        <v>Gorgeous Concrete Gloves</v>
+        <v>Oriental Cotton Shirt</v>
       </c>
       <c r="D72" s="5" t="str">
-        <v>0.3.5</v>
+        <v>7.2.7</v>
       </c>
       <c r="E72" s="5" t="str">
-        <v>January</v>
+        <v>September</v>
       </c>
       <c r="F72" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G72" s="5">
-        <v>10</v>
+        <v>56</v>
       </c>
     </row>
     <row r="73" ht="30" customHeight="1">
       <c r="A73" s="4" t="str">
-        <v>1355b842-f2ec-4798-a723-cb5e7e5986f7</v>
+        <v>3c420f5c-6f92-4622-982c-548b9c40a84f</v>
       </c>
       <c r="B73" s="5" t="str">
-        <v>dcaf4d90-6c94-4177-ba34-dd5366f7839c</v>
+        <v>da452fa9-50ad-4c56-b943-bd263eee1549</v>
       </c>
       <c r="C73" s="5" t="str">
-        <v>Handmade Bronze Sausages</v>
+        <v>Bespoke Frozen Soap</v>
       </c>
       <c r="D73" s="5" t="str">
-        <v>6.1.7</v>
+        <v>7.4.3</v>
       </c>
       <c r="E73" s="5" t="str">
-        <v>September</v>
+        <v>May</v>
       </c>
       <c r="F73" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G73" s="5">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="74" ht="30" customHeight="1">
       <c r="A74" s="4" t="str">
-        <v>c3d9b65a-9282-41eb-ac79-ad35bd17a4b9</v>
+        <v>69e280b5-f8ef-4328-9d9a-aebd4106e864</v>
       </c>
       <c r="B74" s="5" t="str">
-        <v>fdc77292-40a2-481b-b4e9-f3087f2f4fb7</v>
+        <v>51056112-ad25-4e56-961f-70baeebeeb78</v>
       </c>
       <c r="C74" s="5" t="str">
-        <v>Elegant Frozen Tuna</v>
+        <v>Handmade Rubber Hat</v>
       </c>
       <c r="D74" s="5" t="str">
-        <v>6.5.9</v>
+        <v>1.7.8</v>
       </c>
       <c r="E74" s="5" t="str">
-        <v>October</v>
+        <v>May</v>
       </c>
       <c r="F74" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G74" s="5">
-        <v>48</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75" ht="30" customHeight="1">
       <c r="A75" s="4" t="str">
-        <v>be0555e2-0727-4c64-a045-d7d899b755bc</v>
+        <v>f8689c6a-39ae-4865-b5f4-cbffa7d1bfc9</v>
       </c>
       <c r="B75" s="5" t="str">
-        <v>308159ea-229c-4660-abcc-6063fc971cac</v>
+        <v>7c92f0a5-65b0-444f-8d7f-fe31a085683c</v>
       </c>
       <c r="C75" s="5" t="str">
-        <v>Practical Frozen Shoes</v>
+        <v>Intelligent Soft Fish</v>
       </c>
       <c r="D75" s="5" t="str">
-        <v>8.1.8</v>
+        <v>6.5.6</v>
       </c>
       <c r="E75" s="5" t="str">
         <v>March</v>
@@ -2215,24 +2215,24 @@
         <v>2023</v>
       </c>
       <c r="G75" s="5">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="76" ht="30" customHeight="1">
       <c r="A76" s="4" t="str">
-        <v>9bdcb0ea-6878-4876-b6f8-33e8ebb8ec65</v>
+        <v>0150f27e-33a7-4653-abc4-c329fa3a0a6b</v>
       </c>
       <c r="B76" s="5" t="str">
-        <v>a4adb8d0-5141-4e6f-b152-7657870a1de4</v>
+        <v>ce8f11c9-08df-4484-85cf-6161da484bea</v>
       </c>
       <c r="C76" s="5" t="str">
-        <v>Handcrafted Concrete Table</v>
+        <v>Handcrafted Plastic Chicken</v>
       </c>
       <c r="D76" s="5" t="str">
-        <v>2.3.5</v>
+        <v>1.8.7</v>
       </c>
       <c r="E76" s="5" t="str">
-        <v>February</v>
+        <v>January</v>
       </c>
       <c r="F76" s="5" t="str">
         <v>2023</v>
@@ -2243,577 +2243,577 @@
     </row>
     <row r="77" ht="30" customHeight="1">
       <c r="A77" s="4" t="str">
-        <v>c07a873a-5aac-444a-a8ad-1e5ea24dadcb</v>
+        <v>c653aebf-5567-414b-a286-0dd5b7d9d641</v>
       </c>
       <c r="B77" s="5" t="str">
-        <v>e0a3aa0e-ff55-45f2-b2dd-5bf7cf0056b3</v>
+        <v>d748f9b3-243d-41ab-bfb0-547a83ceba5f</v>
       </c>
       <c r="C77" s="5" t="str">
-        <v>Refined Rubber Chair</v>
+        <v>Elegant Steel Chicken</v>
       </c>
       <c r="D77" s="5" t="str">
-        <v>8.8.4</v>
+        <v>5.4.9</v>
       </c>
       <c r="E77" s="5" t="str">
-        <v>May</v>
+        <v>April</v>
       </c>
       <c r="F77" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G77" s="5">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" ht="30" customHeight="1">
       <c r="A78" s="4" t="str">
-        <v>b2591c54-c611-4021-9b24-db39b5531c62</v>
+        <v>46b6e175-45fd-4e7b-a301-4a1717da4b46</v>
       </c>
       <c r="B78" s="5" t="str">
-        <v>4fd33a89-cacb-4583-b2e5-626942f90f3e</v>
+        <v>14f7f2af-e684-4643-a728-be30c87274fb</v>
       </c>
       <c r="C78" s="5" t="str">
-        <v>Incredible Soft Towels</v>
+        <v>Luxurious Plastic Fish</v>
       </c>
       <c r="D78" s="5" t="str">
-        <v>9.9.8</v>
+        <v>5.9.7</v>
       </c>
       <c r="E78" s="5" t="str">
-        <v>July</v>
+        <v>August</v>
       </c>
       <c r="F78" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G78" s="5">
-        <v>67</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" ht="30" customHeight="1">
       <c r="A79" s="4" t="str">
-        <v>26c0cc41-f0a1-4fea-b6bf-a42553571f30</v>
+        <v>4c604dbb-df60-4d42-8a2e-f10faaf4b316</v>
       </c>
       <c r="B79" s="5" t="str">
-        <v>481c4a9a-f2c6-47aa-9ff2-b743a9334a43</v>
+        <v>14c7398a-f245-4667-91ae-a20e719d4ce9</v>
       </c>
       <c r="C79" s="5" t="str">
-        <v>Electronic Frozen Hat</v>
+        <v>Elegant Steel Shoes</v>
       </c>
       <c r="D79" s="5" t="str">
-        <v>4.1.7</v>
+        <v>4.9.8</v>
       </c>
       <c r="E79" s="5" t="str">
-        <v>January</v>
+        <v>July</v>
       </c>
       <c r="F79" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G79" s="5">
-        <v>10</v>
+        <v>97</v>
       </c>
     </row>
     <row r="80" ht="30" customHeight="1">
       <c r="A80" s="4" t="str">
-        <v>0c856237-6285-40d8-83fb-ab95ca23f0e0</v>
+        <v>591eca31-abfd-459a-b954-f52f9dbfc01d</v>
       </c>
       <c r="B80" s="5" t="str">
-        <v>c1518559-45e0-495e-be1a-448be9ced3ce</v>
+        <v>cd92080e-6f62-41c8-ae53-822353edfc25</v>
       </c>
       <c r="C80" s="5" t="str">
-        <v>Practical Plastic Ball</v>
+        <v>Recycled Cotton Fish</v>
       </c>
       <c r="D80" s="5" t="str">
-        <v>8.4.4</v>
+        <v>9.0.1</v>
       </c>
       <c r="E80" s="5" t="str">
-        <v>February</v>
+        <v>March</v>
       </c>
       <c r="F80" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G80" s="5">
-        <v>96</v>
+        <v>51</v>
       </c>
     </row>
     <row r="81" ht="30" customHeight="1">
       <c r="A81" s="4" t="str">
-        <v>98082ab5-62bd-4277-8c30-69606d5f644f</v>
+        <v>6d5d7e95-e777-45dd-8e3c-77275bbbb91f</v>
       </c>
       <c r="B81" s="5" t="str">
-        <v>4b91eb85-3e6f-4f9c-a8b6-b5dfc8cfcec6</v>
+        <v>90c61e50-45b8-41d8-b223-f58721f98587</v>
       </c>
       <c r="C81" s="5" t="str">
-        <v>Handmade Cotton Chair</v>
+        <v>Rustic Concrete Sausages</v>
       </c>
       <c r="D81" s="5" t="str">
-        <v>2.4.5</v>
+        <v>8.1.3</v>
       </c>
       <c r="E81" s="5" t="str">
-        <v>May</v>
+        <v>July</v>
       </c>
       <c r="F81" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G81" s="5">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="82" ht="30" customHeight="1">
       <c r="A82" s="4" t="str">
-        <v>0322f920-34c4-4f2d-95c0-3d347a30c77f</v>
+        <v>cb744bee-975f-4890-96f9-27793a1ec308</v>
       </c>
       <c r="B82" s="5" t="str">
-        <v>5741e966-4c46-4890-82a9-013bcab21e14</v>
+        <v>c158aa32-6230-408e-bca3-6090d22f8581</v>
       </c>
       <c r="C82" s="5" t="str">
-        <v>Awesome Granite Chips</v>
+        <v>Electronic Bronze Gloves</v>
       </c>
       <c r="D82" s="5" t="str">
-        <v>1.0.3</v>
+        <v>5.5.7</v>
       </c>
       <c r="E82" s="5" t="str">
-        <v>May</v>
+        <v>August</v>
       </c>
       <c r="F82" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G82" s="5">
-        <v>19</v>
+        <v>65</v>
       </c>
     </row>
     <row r="83" ht="30" customHeight="1">
       <c r="A83" s="4" t="str">
-        <v>81891e9c-dd9d-4c51-b17d-d181fb1c9dda</v>
+        <v>b6bea2ed-ea92-4112-9df8-201a18a71806</v>
       </c>
       <c r="B83" s="5" t="str">
-        <v>54e488cf-612d-43dc-972b-fed0d0213464</v>
+        <v>346f2deb-f473-4abe-a9da-f8879eabe80b</v>
       </c>
       <c r="C83" s="5" t="str">
-        <v>Licensed Granite Fish</v>
+        <v>Handmade Plastic Car</v>
       </c>
       <c r="D83" s="5" t="str">
-        <v>3.9.4</v>
+        <v>1.6.5</v>
       </c>
       <c r="E83" s="5" t="str">
-        <v>March</v>
+        <v>August</v>
       </c>
       <c r="F83" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G83" s="5">
-        <v>20</v>
+        <v>71</v>
       </c>
     </row>
     <row r="84" ht="30" customHeight="1">
       <c r="A84" s="4" t="str">
-        <v>f55fd5b0-dcde-4118-a7dd-a94f760a7b77</v>
+        <v>123fe60f-1666-406c-aeb0-aa523d5dac06</v>
       </c>
       <c r="B84" s="5" t="str">
-        <v>3f8e7fb5-4301-43f4-9262-66a39ca6b6ee</v>
+        <v>ed37af3e-2c67-4713-8299-296c6fd3cb14</v>
       </c>
       <c r="C84" s="5" t="str">
-        <v>Refined Frozen Shirt</v>
+        <v>Gorgeous Fresh Pants</v>
       </c>
       <c r="D84" s="5" t="str">
-        <v>1.0.1</v>
+        <v>0.6.4</v>
       </c>
       <c r="E84" s="5" t="str">
-        <v>July</v>
+        <v>October</v>
       </c>
       <c r="F84" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G84" s="5">
-        <v>5</v>
+        <v>31</v>
       </c>
     </row>
     <row r="85" ht="30" customHeight="1">
       <c r="A85" s="4" t="str">
-        <v>5bbabe5f-3529-42b7-84f5-c8fbcef472c0</v>
+        <v>9c6891f1-9610-44f7-b181-352928efc6a3</v>
       </c>
       <c r="B85" s="5" t="str">
-        <v>4089fc53-c3a8-492e-aaeb-b849e2f6c13e</v>
+        <v>222c03e7-4063-4a4a-a0de-c17435bb9397</v>
       </c>
       <c r="C85" s="5" t="str">
-        <v>Luxurious Metal Computer</v>
+        <v>Small Soft Table</v>
       </c>
       <c r="D85" s="5" t="str">
-        <v>8.5.2</v>
+        <v>7.6.1</v>
       </c>
       <c r="E85" s="5" t="str">
-        <v>December</v>
+        <v>September</v>
       </c>
       <c r="F85" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G85" s="5">
-        <v>99</v>
+        <v>75</v>
       </c>
     </row>
     <row r="86" ht="30" customHeight="1">
       <c r="A86" s="4" t="str">
-        <v>e8d1198a-c01e-48f2-b3f6-768e117687f3</v>
+        <v>b7d8b712-c1e3-4021-b08f-f77238c76dc5</v>
       </c>
       <c r="B86" s="5" t="str">
-        <v>6020e680-8893-41ee-a7cb-174d2e04ff52</v>
+        <v>f9ad247c-d335-48b6-833c-724f91ad887d</v>
       </c>
       <c r="C86" s="5" t="str">
-        <v>Rustic Plastic Chips</v>
+        <v>Unbranded Wooden Keyboard</v>
       </c>
       <c r="D86" s="5" t="str">
-        <v>9.6.9</v>
+        <v>4.7.5</v>
       </c>
       <c r="E86" s="5" t="str">
-        <v>May</v>
+        <v>December</v>
       </c>
       <c r="F86" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G86" s="5">
-        <v>20</v>
+        <v>68</v>
       </c>
     </row>
     <row r="87" ht="30" customHeight="1">
       <c r="A87" s="4" t="str">
-        <v>0a8c554d-f179-487f-a14b-83b96ed9cb72</v>
+        <v>fb1b0efc-4571-467e-af6f-04423fa532e2</v>
       </c>
       <c r="B87" s="5" t="str">
-        <v>9f044f5f-f0be-449c-8197-2add31d6b027</v>
+        <v>eb5bc999-9594-4a71-a564-948b171b2aca</v>
       </c>
       <c r="C87" s="5" t="str">
-        <v>Practical Bronze Computer</v>
+        <v>Incredible Wooden Ball</v>
       </c>
       <c r="D87" s="5" t="str">
-        <v>1.9.0</v>
+        <v>9.1.7</v>
       </c>
       <c r="E87" s="5" t="str">
-        <v>June</v>
+        <v>January</v>
       </c>
       <c r="F87" s="5" t="str">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G87" s="5">
-        <v>95</v>
+        <v>19</v>
       </c>
     </row>
     <row r="88" ht="30" customHeight="1">
       <c r="A88" s="4" t="str">
-        <v>0097c924-02d6-47f0-b7c9-70ed5167eb15</v>
+        <v>fc94902e-9a93-4c4c-924b-b4abe6531919</v>
       </c>
       <c r="B88" s="5" t="str">
-        <v>ff575ef5-286c-47ff-8173-c4ca656dddfa</v>
+        <v>be92b4d8-75c9-4b9d-b7db-3eb0e4a4a260</v>
       </c>
       <c r="C88" s="5" t="str">
-        <v>Luxurious Metal Computer</v>
+        <v>Rustic Rubber Computer</v>
       </c>
       <c r="D88" s="5" t="str">
-        <v>0.0.0</v>
+        <v>5.1.3</v>
       </c>
       <c r="E88" s="5" t="str">
-        <v>June</v>
+        <v>November</v>
       </c>
       <c r="F88" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G88" s="5">
-        <v>17</v>
+        <v>90</v>
       </c>
     </row>
     <row r="89" ht="30" customHeight="1">
       <c r="A89" s="4" t="str">
-        <v>aa2c6b9c-4500-47f8-a30e-43bead0084b9</v>
+        <v>13485624-49b4-43e6-bbb8-f7d19f4504ac</v>
       </c>
       <c r="B89" s="5" t="str">
-        <v>0f828382-0e13-4b5a-b02e-578572ccc330</v>
+        <v>960a526e-c3f4-4266-9f8c-3883e0eaaf78</v>
       </c>
       <c r="C89" s="5" t="str">
-        <v>Unbranded Wooden Mouse</v>
+        <v>Luxurious Cotton Tuna</v>
       </c>
       <c r="D89" s="5" t="str">
-        <v>0.7.0</v>
+        <v>4.9.1</v>
       </c>
       <c r="E89" s="5" t="str">
-        <v>February</v>
+        <v>March</v>
       </c>
       <c r="F89" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G89" s="5">
-        <v>46</v>
+        <v>97</v>
       </c>
     </row>
     <row r="90" ht="30" customHeight="1">
       <c r="A90" s="4" t="str">
-        <v>88e7cd2e-834d-4562-bfd4-f6b488097106</v>
+        <v>fa4060f5-1a3b-4640-96b3-c3b8355e63b2</v>
       </c>
       <c r="B90" s="5" t="str">
-        <v>9753bf64-8c63-42da-919f-873d7f032e7e</v>
+        <v>244640a2-be6c-4f2b-a19a-383b5aef9752</v>
       </c>
       <c r="C90" s="5" t="str">
-        <v>Practical Concrete Gloves</v>
+        <v>Tasty Cotton Sausages</v>
       </c>
       <c r="D90" s="5" t="str">
-        <v>2.1.5</v>
+        <v>8.5.9</v>
       </c>
       <c r="E90" s="5" t="str">
-        <v>February</v>
+        <v>November</v>
       </c>
       <c r="F90" s="5" t="str">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G90" s="5">
-        <v>35</v>
+        <v>73</v>
       </c>
     </row>
     <row r="91" ht="30" customHeight="1">
       <c r="A91" s="4" t="str">
-        <v>c11cbe41-367e-4a6d-a4b5-e850e6ae7bde</v>
+        <v>40e2d70f-abf4-4884-b247-7e0ebaccd793</v>
       </c>
       <c r="B91" s="5" t="str">
-        <v>b38c64c0-a4b9-426a-b8fe-954d2b85f722</v>
+        <v>be338f38-10ae-4c10-bc0a-4560bb6150d0</v>
       </c>
       <c r="C91" s="5" t="str">
-        <v>Gorgeous Soft Shoes</v>
+        <v>Elegant Granite Table</v>
       </c>
       <c r="D91" s="5" t="str">
-        <v>5.8.9</v>
+        <v>4.2.2</v>
       </c>
       <c r="E91" s="5" t="str">
-        <v>November</v>
+        <v>May</v>
       </c>
       <c r="F91" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G91" s="5">
-        <v>53</v>
+        <v>22</v>
       </c>
     </row>
     <row r="92" ht="30" customHeight="1">
       <c r="A92" s="4" t="str">
-        <v>eab9cf57-acf2-4a66-a783-df6e554802f3</v>
+        <v>d1a9c12b-edd8-43c6-91db-a2620ca711af</v>
       </c>
       <c r="B92" s="5" t="str">
-        <v>f860ced7-7991-4159-afc4-911620b12177</v>
+        <v>903c3283-8e4d-413b-8251-6e070b756aa6</v>
       </c>
       <c r="C92" s="5" t="str">
-        <v>Refined Rubber Hat</v>
+        <v>Awesome Plastic Computer</v>
       </c>
       <c r="D92" s="5" t="str">
-        <v>2.0.9</v>
+        <v>3.1.4</v>
       </c>
       <c r="E92" s="5" t="str">
-        <v>January</v>
+        <v>April</v>
       </c>
       <c r="F92" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G92" s="5">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="93" ht="30" customHeight="1">
       <c r="A93" s="4" t="str">
-        <v>3404303b-2cbd-429b-a6a1-316d434e032d</v>
+        <v>5cc2e9f7-7a52-4081-be54-bd189865c750</v>
       </c>
       <c r="B93" s="5" t="str">
-        <v>d489fe40-4f6c-4d1e-bfc5-9a9ef2f86763</v>
+        <v>324ff42c-b071-40a8-8bbc-19ed7eb3036f</v>
       </c>
       <c r="C93" s="5" t="str">
-        <v>Unbranded Wooden Mouse</v>
+        <v>Rustic Granite Table</v>
       </c>
       <c r="D93" s="5" t="str">
-        <v>7.4.2</v>
+        <v>6.1.9</v>
       </c>
       <c r="E93" s="5" t="str">
-        <v>July</v>
+        <v>January</v>
       </c>
       <c r="F93" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G93" s="5">
-        <v>62</v>
+        <v>96</v>
       </c>
     </row>
     <row r="94" ht="30" customHeight="1">
       <c r="A94" s="4" t="str">
-        <v>31e5868e-38a8-40a0-9421-e2cd05594a96</v>
+        <v>d773aa80-1089-41ed-8eba-b65dce86c72e</v>
       </c>
       <c r="B94" s="5" t="str">
-        <v>c4c87e54-5012-4137-8244-5fe4259b2534</v>
+        <v>ad8a82ce-ac7b-4925-8f7c-d87276798301</v>
       </c>
       <c r="C94" s="5" t="str">
-        <v>Oriental Metal Tuna</v>
+        <v>Fantastic Bronze Pants</v>
       </c>
       <c r="D94" s="5" t="str">
-        <v>0.7.6</v>
+        <v>1.7.8</v>
       </c>
       <c r="E94" s="5" t="str">
-        <v>June</v>
+        <v>July</v>
       </c>
       <c r="F94" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G94" s="5">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="95" ht="30" customHeight="1">
       <c r="A95" s="4" t="str">
-        <v>bb3cbbf6-24e1-435c-8d0c-1fc57a893af4</v>
+        <v>ad206f96-0609-47d1-b0a9-ba26b55fd66a</v>
       </c>
       <c r="B95" s="5" t="str">
-        <v>1f86f29d-7ec2-4145-af20-688f32a06b89</v>
+        <v>1fb376ae-bd31-4aba-b918-af440f26dd83</v>
       </c>
       <c r="C95" s="5" t="str">
-        <v>Rustic Frozen Towels</v>
+        <v>Licensed Rubber Chicken</v>
       </c>
       <c r="D95" s="5" t="str">
-        <v>6.8.0</v>
+        <v>8.9.5</v>
       </c>
       <c r="E95" s="5" t="str">
-        <v>March</v>
+        <v>September</v>
       </c>
       <c r="F95" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G95" s="5">
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="96" ht="30" customHeight="1">
       <c r="A96" s="4" t="str">
-        <v>c0b036c6-711b-4a8a-8615-88b4dbbc868b</v>
+        <v>2b39be18-a1a5-46fa-9c8c-f21f13f523eb</v>
       </c>
       <c r="B96" s="5" t="str">
-        <v>cb5fb1a1-f438-4da3-84f2-e4e6e533758e</v>
+        <v>30aeafdb-657b-4aa1-98d7-aa9ec18e30df</v>
       </c>
       <c r="C96" s="5" t="str">
-        <v>Handmade Steel Towels</v>
+        <v>Incredible Frozen Chicken</v>
       </c>
       <c r="D96" s="5" t="str">
-        <v>8.0.1</v>
+        <v>7.9.4</v>
       </c>
       <c r="E96" s="5" t="str">
-        <v>July</v>
+        <v>April</v>
       </c>
       <c r="F96" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G96" s="5">
-        <v>90</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" ht="30" customHeight="1">
       <c r="A97" s="4" t="str">
-        <v>a8911d6a-a0d7-4c2b-8937-59dc77843fab</v>
+        <v>ebb9f168-3a81-4ae8-b8eb-ddba7ef53bb8</v>
       </c>
       <c r="B97" s="5" t="str">
-        <v>a69b5021-05cc-421a-b1f2-07e4a4ea9589</v>
+        <v>20aabdc2-628c-4142-a2e9-88d53bef6a2f</v>
       </c>
       <c r="C97" s="5" t="str">
-        <v>Bespoke Fresh Computer</v>
+        <v>Modern Fresh Gloves</v>
       </c>
       <c r="D97" s="5" t="str">
-        <v>9.8.6</v>
+        <v>2.4.6</v>
       </c>
       <c r="E97" s="5" t="str">
-        <v>August</v>
+        <v>January</v>
       </c>
       <c r="F97" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G97" s="5">
-        <v>95</v>
+        <v>44</v>
       </c>
     </row>
     <row r="98" ht="30" customHeight="1">
       <c r="A98" s="4" t="str">
-        <v>84945a5c-cf03-4522-95b6-ce49fdbbee5e</v>
+        <v>e4e0bc62-c4ed-4fdb-8b31-3e6e0ac94001</v>
       </c>
       <c r="B98" s="5" t="str">
-        <v>f7501285-7733-439d-8658-ccd66feb7e2c</v>
+        <v>80108ebf-ff64-4c53-bdfc-1279cffe4343</v>
       </c>
       <c r="C98" s="5" t="str">
-        <v>Practical Cotton Ball</v>
+        <v>Generic Concrete Chair</v>
       </c>
       <c r="D98" s="5" t="str">
-        <v>3.7.7</v>
+        <v>8.4.7</v>
       </c>
       <c r="E98" s="5" t="str">
-        <v>July</v>
+        <v>December</v>
       </c>
       <c r="F98" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G98" s="5">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="99" ht="30" customHeight="1">
       <c r="A99" s="4" t="str">
-        <v>86d31a70-cd6f-4c05-9338-590576d2753a</v>
+        <v>be5247f4-79ee-476c-aded-0c15fbfee671</v>
       </c>
       <c r="B99" s="5" t="str">
-        <v>31aeb84c-a0f8-4729-9548-e903dd4b1d7e</v>
+        <v>d0a4d0a2-a304-450a-aee1-8bde0c4d7d95</v>
       </c>
       <c r="C99" s="5" t="str">
-        <v>Ergonomic Concrete Tuna</v>
+        <v>Handmade Metal Pizza</v>
       </c>
       <c r="D99" s="5" t="str">
-        <v>2.4.3</v>
+        <v>9.3.9</v>
       </c>
       <c r="E99" s="5" t="str">
-        <v>December</v>
+        <v>November</v>
       </c>
       <c r="F99" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G99" s="5">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="100" ht="30" customHeight="1">
       <c r="A100" s="4" t="str">
-        <v>0f3264a6-9c37-4fe0-b9de-0d2c8a2a8820</v>
+        <v>7e32749a-5aec-4203-85d4-5c17a9641441</v>
       </c>
       <c r="B100" s="5" t="str">
-        <v>baa13ba0-03e8-44b6-a41e-dff15fbacf09</v>
+        <v>e67774ab-4b7e-4f72-963a-253132e5dd60</v>
       </c>
       <c r="C100" s="5" t="str">
-        <v>Small Metal Pants</v>
+        <v>Fantastic Wooden Shirt</v>
       </c>
       <c r="D100" s="5" t="str">
-        <v>6.0.0</v>
+        <v>3.7.7</v>
       </c>
       <c r="E100" s="5" t="str">
-        <v>March</v>
+        <v>February</v>
       </c>
       <c r="F100" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G100" s="5">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="101" ht="30" customHeight="1">
       <c r="A101" s="4" t="str">
-        <v>c04dc015-d883-4092-b93b-271e33d758db</v>
+        <v>4da1b7c1-cd54-4a1b-b12d-b912ef26cef2</v>
       </c>
       <c r="B101" s="5" t="str">
-        <v>3aea83bd-352e-449e-ae27-1205570a368e</v>
+        <v>106a9b6f-53c3-4abb-9298-7ebf4c0214ed</v>
       </c>
       <c r="C101" s="5" t="str">
-        <v>Unbranded Fresh Chair</v>
+        <v>Licensed Granite Shirt</v>
       </c>
       <c r="D101" s="5" t="str">
-        <v>5.5.4</v>
+        <v>1.6.3</v>
       </c>
       <c r="E101" s="5" t="str">
-        <v>October</v>
+        <v>December</v>
       </c>
       <c r="F101" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G101" s="5">
-        <v>5</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add table summary support
</commit_message>
<xml_diff>
--- a/consumption.xlsx
+++ b/consumption.xlsx
@@ -486,7 +486,7 @@
   <cols>
     <col min="1" max="1" width="41.83203125" customWidth="1"/>
     <col min="2" max="2" width="41.83203125" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" customWidth="1"/>
+    <col min="3" max="3" width="31.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" customWidth="1"/>
     <col min="5" max="5" width="14.83203125" customWidth="1"/>
     <col min="6" max="6" width="9.83203125" customWidth="1"/>
@@ -518,1054 +518,1054 @@
     </row>
     <row r="2" ht="30" customHeight="1">
       <c r="A2" s="4" t="str">
-        <v>5ea26c56-8806-4af3-b786-320c92ea0b08</v>
+        <v>4613ac17-9ff8-444a-84bc-fd6266f1fd27</v>
       </c>
       <c r="B2" s="5" t="str">
-        <v>8205dbdc-51d7-4bd0-a214-936b5769d8cd</v>
+        <v>87a0ae47-5c6d-4bca-9fc5-5ad099373c8f</v>
       </c>
       <c r="C2" s="5" t="str">
-        <v>Gorgeous Granite Bacon</v>
+        <v>Licensed Plastic Computer</v>
       </c>
       <c r="D2" s="5" t="str">
-        <v>0.0.9</v>
+        <v>3.7.1</v>
       </c>
       <c r="E2" s="5" t="str">
-        <v>January</v>
+        <v>July</v>
       </c>
       <c r="F2" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G2" s="5">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1">
       <c r="A3" s="4" t="str">
-        <v>42fe9f54-2c45-4c86-aaf6-115c09b02d6e</v>
+        <v>b756d4bc-e5a7-4c85-8e05-c9c948dc655a</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>41734f69-4836-47b7-b905-a8e708cea16d</v>
+        <v>612a55b8-cd6e-42c8-a9d4-207ac7170ab1</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>Sleek Concrete Computer</v>
+        <v>Practical Fresh Sausages</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>2.9.1</v>
+        <v>1.0.7</v>
       </c>
       <c r="E3" s="5" t="str">
-        <v>June</v>
+        <v>December</v>
       </c>
       <c r="F3" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G3" s="5">
-        <v>34</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" ht="30" customHeight="1">
       <c r="A4" s="4" t="str">
-        <v>63cc659e-0f87-44d7-b7f8-f724009f08af</v>
+        <v>9f02d59a-f199-491f-8625-bb3bafe868f3</v>
       </c>
       <c r="B4" s="5" t="str">
-        <v>f0f98488-050e-47b5-bc80-70211b87f5ec</v>
+        <v>9331d5d2-e45e-4bce-9e56-b824ccfd2c7a</v>
       </c>
       <c r="C4" s="5" t="str">
-        <v>Electronic Bronze Gloves</v>
+        <v>Handmade Concrete Table</v>
       </c>
       <c r="D4" s="5" t="str">
-        <v>0.2.8</v>
+        <v>4.0.0</v>
       </c>
       <c r="E4" s="5" t="str">
-        <v>October</v>
+        <v>September</v>
       </c>
       <c r="F4" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G4" s="5">
-        <v>14</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" ht="30" customHeight="1">
       <c r="A5" s="4" t="str">
-        <v>b5012871-7271-46f5-9465-96cebfb1e276</v>
+        <v>b857659d-d027-459f-befa-6b522568f9ca</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>979913f8-08da-4c3a-9b34-5e9c1ce91fa0</v>
+        <v>844da8fc-4676-4f5c-ba25-db67a5159c42</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>Luxurious Steel Shirt</v>
+        <v>Small Rubber Chips</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>8.9.9</v>
+        <v>4.2.7</v>
       </c>
       <c r="E5" s="5" t="str">
-        <v>May</v>
+        <v>March</v>
       </c>
       <c r="F5" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G5" s="5">
-        <v>51</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" ht="30" customHeight="1">
       <c r="A6" s="4" t="str">
-        <v>de9ee68c-111e-4cc5-881d-75de59967099</v>
+        <v>982daf32-755c-4657-8580-7d2102675c3e</v>
       </c>
       <c r="B6" s="5" t="str">
-        <v>90b20278-e9bc-462e-b59a-7674157c5c17</v>
+        <v>5d4c8629-c32b-475b-805a-0347d7dfbd37</v>
       </c>
       <c r="C6" s="5" t="str">
-        <v>Bespoke Rubber Chair</v>
+        <v>Small Bronze Chips</v>
       </c>
       <c r="D6" s="5" t="str">
-        <v>8.9.3</v>
+        <v>2.2.9</v>
       </c>
       <c r="E6" s="5" t="str">
-        <v>January</v>
+        <v>February</v>
       </c>
       <c r="F6" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G6" s="5">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" ht="30" customHeight="1">
       <c r="A7" s="4" t="str">
-        <v>5a3de9c7-e5e2-4437-883f-446f18ac999f</v>
+        <v>477ba9c1-92bf-4916-a55a-ebf8ce0cb369</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>49a1cbaf-09c0-4597-8c25-3d395ad286db</v>
+        <v>2f4aff62-f4d3-438c-a483-0165f0cc006d</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>Sleek Concrete Pants</v>
+        <v>Fantastic Plastic Soap</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>2.6.2</v>
+        <v>0.4.1</v>
       </c>
       <c r="E7" s="5" t="str">
-        <v>August</v>
+        <v>January</v>
       </c>
       <c r="F7" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G7" s="5">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" ht="30" customHeight="1">
       <c r="A8" s="4" t="str">
-        <v>5936451c-4804-440a-942f-bd773f8e1ccb</v>
+        <v>7e7e59ec-e9db-4437-a3b9-8e0844a4155f</v>
       </c>
       <c r="B8" s="5" t="str">
-        <v>5bb8a36c-48d1-484c-9377-eedcc433eae0</v>
+        <v>3ceff741-0e15-4723-ab53-374715545318</v>
       </c>
       <c r="C8" s="5" t="str">
-        <v>Refined Metal Towels</v>
+        <v>Incredible Bronze Towels</v>
       </c>
       <c r="D8" s="5" t="str">
-        <v>7.2.6</v>
+        <v>6.5.2</v>
       </c>
       <c r="E8" s="5" t="str">
-        <v>January</v>
+        <v>June</v>
       </c>
       <c r="F8" s="5" t="str">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G8" s="5">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" ht="30" customHeight="1">
       <c r="A9" s="4" t="str">
-        <v>e4521659-2206-4ec0-95e3-a72aea188d33</v>
+        <v>ac20943f-e535-4bff-970d-0533e641f63f</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>3b1fe986-d11f-462f-8dac-2977caf1d014</v>
+        <v>132d8ddd-9fc4-4598-b470-de94da418f80</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>Tasty Wooden Chicken</v>
+        <v>Generic Bronze Car</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>1.9.5</v>
+        <v>5.6.2</v>
       </c>
       <c r="E9" s="5" t="str">
-        <v>April</v>
+        <v>August</v>
       </c>
       <c r="F9" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G9" s="5">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" ht="30" customHeight="1">
       <c r="A10" s="4" t="str">
-        <v>bab313a5-24bb-4d7c-8ffc-518aafc8f1e2</v>
+        <v>7eb4db9d-4adc-4e94-884b-16b634d08bfa</v>
       </c>
       <c r="B10" s="5" t="str">
-        <v>64cb85fd-0d06-4776-9053-51119312384b</v>
+        <v>c1e50f29-e941-4ab1-8cbb-0ba4a45a8c8c</v>
       </c>
       <c r="C10" s="5" t="str">
-        <v>Practical Frozen Keyboard</v>
+        <v>Rustic Soft Mouse</v>
       </c>
       <c r="D10" s="5" t="str">
-        <v>8.0.6</v>
+        <v>9.0.7</v>
       </c>
       <c r="E10" s="5" t="str">
-        <v>September</v>
+        <v>February</v>
       </c>
       <c r="F10" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G10" s="5">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" ht="30" customHeight="1">
       <c r="A11" s="4" t="str">
-        <v>4ef1caf6-6a60-4ae2-ad6b-c538ab4bd937</v>
+        <v>cecd6da0-99b5-46e5-9983-ec1309d1c3ff</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>2b295dae-7a3e-41c9-a0a4-7d5eb43e6f51</v>
+        <v>dad80883-9909-479c-8e72-d5462c092a2e</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>Small Cotton Chair</v>
+        <v>Small Wooden Ball</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v>0.2.6</v>
+        <v>5.5.0</v>
       </c>
       <c r="E11" s="5" t="str">
-        <v>June</v>
+        <v>October</v>
       </c>
       <c r="F11" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G11" s="5">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" ht="30" customHeight="1">
       <c r="A12" s="4" t="str">
-        <v>eafe3242-073f-42d6-a066-8500daee2754</v>
+        <v>3d8120c0-980d-4361-8e85-547639f9cd4b</v>
       </c>
       <c r="B12" s="5" t="str">
-        <v>0ea1a1d2-2ae7-47df-9799-1bb8b370e1ad</v>
+        <v>c887573c-79e7-41ae-9765-4e6a29fd377b</v>
       </c>
       <c r="C12" s="5" t="str">
-        <v>Refined Frozen Soap</v>
+        <v>Luxurious Steel Car</v>
       </c>
       <c r="D12" s="5" t="str">
-        <v>9.9.7</v>
+        <v>6.8.3</v>
       </c>
       <c r="E12" s="5" t="str">
-        <v>June</v>
+        <v>October</v>
       </c>
       <c r="F12" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G12" s="5">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" ht="30" customHeight="1">
       <c r="A13" s="4" t="str">
-        <v>b074c1ce-e6a3-4bb8-9ae2-873a9eaa0dcb</v>
+        <v>a462d786-d915-4857-bc8a-ebcfc8972151</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>d72c98a8-d0f1-44e2-8bb6-11eed1d0f910</v>
+        <v>a80d8975-3899-48a3-b9d3-352193eb381f</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>Generic Concrete Sausages</v>
+        <v>Small Plastic Gloves</v>
       </c>
       <c r="D13" s="5" t="str">
-        <v>1.9.4</v>
+        <v>8.3.0</v>
       </c>
       <c r="E13" s="5" t="str">
-        <v>April</v>
+        <v>July</v>
       </c>
       <c r="F13" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G13" s="5">
-        <v>83</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" ht="30" customHeight="1">
       <c r="A14" s="4" t="str">
-        <v>41be3052-c7a6-4b26-ab4d-d4fe28a3c1e5</v>
+        <v>8b91e5e6-10bc-44ee-b498-cf9041e320ee</v>
       </c>
       <c r="B14" s="5" t="str">
-        <v>f6443efa-f0ce-4b14-9411-aca56e37b8e9</v>
+        <v>bc1231f0-59a6-4815-af25-a2aa8ec939ad</v>
       </c>
       <c r="C14" s="5" t="str">
-        <v>Rustic Soft Chicken</v>
+        <v>Small Bronze Salad</v>
       </c>
       <c r="D14" s="5" t="str">
-        <v>5.6.8</v>
+        <v>7.0.0</v>
       </c>
       <c r="E14" s="5" t="str">
-        <v>September</v>
+        <v>August</v>
       </c>
       <c r="F14" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G14" s="5">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" ht="30" customHeight="1">
       <c r="A15" s="4" t="str">
-        <v>ee428ba8-2e19-440b-aba2-0a021a5d7a63</v>
+        <v>08b972f4-a417-42ab-a00d-ce19f064c00c</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>a81c59ce-978b-4f43-a46b-8e6c8ee52217</v>
+        <v>5c00f071-0f42-4a68-98ff-890d90adc405</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>Awesome Frozen Chips</v>
+        <v>Incredible Steel Shirt</v>
       </c>
       <c r="D15" s="5" t="str">
-        <v>3.3.3</v>
+        <v>8.6.9</v>
       </c>
       <c r="E15" s="5" t="str">
-        <v>March</v>
+        <v>July</v>
       </c>
       <c r="F15" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G15" s="5">
-        <v>55</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" ht="30" customHeight="1">
       <c r="A16" s="4" t="str">
-        <v>4b7fc6c5-44b2-4a86-9315-d531f26bf78c</v>
+        <v>07d4bb9b-5fbb-4efd-8fbe-fd5cd29aeb55</v>
       </c>
       <c r="B16" s="5" t="str">
-        <v>fec2ee66-aff7-4b93-a0e5-9712610899b4</v>
+        <v>55c4f630-f69a-4fe0-b52f-6d60d914e315</v>
       </c>
       <c r="C16" s="5" t="str">
-        <v>Fantastic Granite Fish</v>
+        <v>Awesome Cotton Cheese</v>
       </c>
       <c r="D16" s="5" t="str">
-        <v>3.9.7</v>
+        <v>6.2.8</v>
       </c>
       <c r="E16" s="5" t="str">
-        <v>May</v>
+        <v>August</v>
       </c>
       <c r="F16" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G16" s="5">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" ht="30" customHeight="1">
       <c r="A17" s="4" t="str">
-        <v>b5f27cf3-b45b-475c-afff-13f500469607</v>
+        <v>b302a143-bd18-4932-b35c-cb6322418d45</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>67f2b52c-30ff-47a7-9575-5ee5d0e2cc9e</v>
+        <v>111c6d64-72a3-475b-b871-7362a70d7078</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>Recycled Plastic Shirt</v>
+        <v>Awesome Fresh Chair</v>
       </c>
       <c r="D17" s="5" t="str">
-        <v>9.2.4</v>
+        <v>0.9.7</v>
       </c>
       <c r="E17" s="5" t="str">
-        <v>March</v>
+        <v>November</v>
       </c>
       <c r="F17" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G17" s="5">
-        <v>57</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" ht="30" customHeight="1">
       <c r="A18" s="4" t="str">
-        <v>41cf6a0f-06a9-4f11-bf49-a5bce53337d9</v>
+        <v>60c10d00-de7d-48bf-9985-0ce0faed0693</v>
       </c>
       <c r="B18" s="5" t="str">
-        <v>455edfdb-2fee-48c8-bd77-95329ca4228e</v>
+        <v>efd588bc-3791-4b5a-a4b6-1f951b66cf5d</v>
       </c>
       <c r="C18" s="5" t="str">
-        <v>Sleek Granite Towels</v>
+        <v>Sleek Rubber Bacon</v>
       </c>
       <c r="D18" s="5" t="str">
-        <v>7.3.9</v>
+        <v>9.9.0</v>
       </c>
       <c r="E18" s="5" t="str">
-        <v>November</v>
+        <v>August</v>
       </c>
       <c r="F18" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G18" s="5">
-        <v>91</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" ht="30" customHeight="1">
       <c r="A19" s="4" t="str">
-        <v>922411c6-e50b-418c-9f33-f7299601fa71</v>
+        <v>b1521c6d-09c3-447c-bdb1-bfeae5006797</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>98bb6d17-c7a5-4aca-bbe8-32eac5a359d3</v>
+        <v>ff224f8b-cce0-49e1-bc0d-5d1878bdb678</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v>Bespoke Cotton Chicken</v>
+        <v>Intelligent Plastic Cheese</v>
       </c>
       <c r="D19" s="5" t="str">
-        <v>1.7.4</v>
+        <v>4.2.7</v>
       </c>
       <c r="E19" s="5" t="str">
-        <v>November</v>
+        <v>June</v>
       </c>
       <c r="F19" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G19" s="5">
-        <v>3</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" ht="30" customHeight="1">
       <c r="A20" s="4" t="str">
-        <v>9aa3c325-0046-4283-8fca-756b6f0dad8e</v>
+        <v>72c01f58-a4af-4f03-b9a5-41fbdb0d5af5</v>
       </c>
       <c r="B20" s="5" t="str">
-        <v>5bee1d03-d877-4b1e-90e3-bb8eda6eb5b5</v>
+        <v>73439b8e-1ec6-4841-8661-1b8b04e7d296</v>
       </c>
       <c r="C20" s="5" t="str">
-        <v>Tasty Metal Tuna</v>
+        <v>Luxurious Bronze Shoes</v>
       </c>
       <c r="D20" s="5" t="str">
-        <v>4.3.6</v>
+        <v>5.3.1</v>
       </c>
       <c r="E20" s="5" t="str">
-        <v>July</v>
+        <v>August</v>
       </c>
       <c r="F20" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G20" s="5">
-        <v>56</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" ht="30" customHeight="1">
       <c r="A21" s="4" t="str">
-        <v>d0d24664-fe48-40f2-9487-c99a464d3859</v>
+        <v>937a79d3-6e32-43d7-b592-3ebcfb088317</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>ea8e2653-2c97-4537-ae05-ad5873163bcf</v>
+        <v>11accd79-ed95-4858-855d-b0ff596b7657</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v>Sleek Cotton Table</v>
+        <v>Handcrafted Wooden Cheese</v>
       </c>
       <c r="D21" s="5" t="str">
-        <v>1.8.5</v>
+        <v>7.8.8</v>
       </c>
       <c r="E21" s="5" t="str">
-        <v>April</v>
+        <v>May</v>
       </c>
       <c r="F21" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G21" s="5">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" ht="30" customHeight="1">
       <c r="A22" s="4" t="str">
-        <v>1190278c-f8ab-4691-aa8d-76af5b6ad762</v>
+        <v>ef7f8545-a45f-4c3e-a7b1-cb312c07fe61</v>
       </c>
       <c r="B22" s="5" t="str">
-        <v>ab454ed0-926f-43ce-9bb9-f5b48cd30f8a</v>
+        <v>35687b17-4cee-41fe-9fc6-d90ce6c6e833</v>
       </c>
       <c r="C22" s="5" t="str">
-        <v>Fantastic Frozen Bacon</v>
+        <v>Handcrafted Rubber Gloves</v>
       </c>
       <c r="D22" s="5" t="str">
-        <v>3.7.6</v>
+        <v>2.7.8</v>
       </c>
       <c r="E22" s="5" t="str">
-        <v>December</v>
+        <v>May</v>
       </c>
       <c r="F22" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G22" s="5">
-        <v>62</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" ht="30" customHeight="1">
       <c r="A23" s="4" t="str">
-        <v>00b2df4f-2605-48fe-88e8-a6b09fb8d17e</v>
+        <v>c783863a-7ff4-47f8-940d-d0f409009d04</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>f960c12a-821f-4c21-99f8-ed0e697604a8</v>
+        <v>f688b3a4-473d-4e1b-b8b6-98f4bd6946e1</v>
       </c>
       <c r="C23" s="5" t="str">
-        <v>Awesome Bronze Cheese</v>
+        <v>Recycled Bronze Chicken</v>
       </c>
       <c r="D23" s="5" t="str">
-        <v>3.0.7</v>
+        <v>4.4.8</v>
       </c>
       <c r="E23" s="5" t="str">
-        <v>June</v>
+        <v>September</v>
       </c>
       <c r="F23" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G23" s="5">
-        <v>4</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" ht="30" customHeight="1">
       <c r="A24" s="4" t="str">
-        <v>f75b4d26-5299-4f91-90a2-a77d90363b4e</v>
+        <v>30cd03fa-a779-48d0-b532-c90fe83acdff</v>
       </c>
       <c r="B24" s="5" t="str">
-        <v>f7f61878-b1b0-4018-ae84-e8a5bf621009</v>
+        <v>ff4e04c5-9d4d-45f2-8ce5-e9f2867bbfe0</v>
       </c>
       <c r="C24" s="5" t="str">
-        <v>Generic Cotton Gloves</v>
+        <v>Elegant Plastic Salad</v>
       </c>
       <c r="D24" s="5" t="str">
-        <v>1.4.6</v>
+        <v>2.4.8</v>
       </c>
       <c r="E24" s="5" t="str">
-        <v>June</v>
+        <v>September</v>
       </c>
       <c r="F24" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G24" s="5">
-        <v>59</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" ht="30" customHeight="1">
       <c r="A25" s="4" t="str">
-        <v>d77464c4-d79f-4214-a2f9-062364889f1c</v>
+        <v>659430ec-7ff2-4e48-9036-eb4bbd190d95</v>
       </c>
       <c r="B25" s="5" t="str">
-        <v>aaa93b2c-f22a-497f-a0f3-b27376e1d0fa</v>
+        <v>6961cfde-77b8-4a16-9477-b9eb6bd98c80</v>
       </c>
       <c r="C25" s="5" t="str">
-        <v>Electronic Cotton Pants</v>
+        <v>Oriental Fresh Hat</v>
       </c>
       <c r="D25" s="5" t="str">
-        <v>0.7.7</v>
+        <v>2.1.0</v>
       </c>
       <c r="E25" s="5" t="str">
-        <v>October</v>
+        <v>August</v>
       </c>
       <c r="F25" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G25" s="5">
-        <v>36</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1">
       <c r="A26" s="4" t="str">
-        <v>4fad16fc-f565-4f77-97a5-ddf5848469c7</v>
+        <v>b9ceccaa-0bba-49c7-9dcc-6c4c30f45bb6</v>
       </c>
       <c r="B26" s="5" t="str">
-        <v>6766109a-adbc-4c8d-9fc5-21b095614ea3</v>
+        <v>38ccc966-4c45-4faf-9c87-ac33be50ba05</v>
       </c>
       <c r="C26" s="5" t="str">
-        <v>Ergonomic Concrete Mouse</v>
+        <v>Tasty Rubber Tuna</v>
       </c>
       <c r="D26" s="5" t="str">
-        <v>0.9.9</v>
+        <v>1.3.9</v>
       </c>
       <c r="E26" s="5" t="str">
-        <v>August</v>
+        <v>November</v>
       </c>
       <c r="F26" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G26" s="5">
-        <v>25</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1">
       <c r="A27" s="4" t="str">
-        <v>469c337c-c369-48e2-8215-9399f4f9072c</v>
+        <v>dc7300b8-7009-42a1-b19f-e52f75fa4db2</v>
       </c>
       <c r="B27" s="5" t="str">
-        <v>64035d32-dcde-4922-aa9a-6c2bf40602e7</v>
+        <v>f08c65ae-3557-4141-bee0-6cf104da7ba9</v>
       </c>
       <c r="C27" s="5" t="str">
-        <v>Handmade Soft Fish</v>
+        <v>Sleek Plastic Shoes</v>
       </c>
       <c r="D27" s="5" t="str">
-        <v>9.7.4</v>
+        <v>4.4.7</v>
       </c>
       <c r="E27" s="5" t="str">
-        <v>October</v>
+        <v>March</v>
       </c>
       <c r="F27" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G27" s="5">
-        <v>96</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1">
       <c r="A28" s="4" t="str">
-        <v>910e8d1f-563b-467a-852e-146318eb81a1</v>
+        <v>c255c2c2-14cb-45b9-a9b5-2c8781ac95a4</v>
       </c>
       <c r="B28" s="5" t="str">
-        <v>e77fa4c3-7025-47e8-a81e-cf89e5e23752</v>
+        <v>97639545-0d6b-4336-9f01-878642bd95ff</v>
       </c>
       <c r="C28" s="5" t="str">
-        <v>Oriental Cotton Mouse</v>
+        <v>Small Concrete Chicken</v>
       </c>
       <c r="D28" s="5" t="str">
-        <v>9.8.1</v>
+        <v>9.0.3</v>
       </c>
       <c r="E28" s="5" t="str">
-        <v>March</v>
+        <v>December</v>
       </c>
       <c r="F28" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G28" s="5">
-        <v>53</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1">
       <c r="A29" s="4" t="str">
-        <v>8ea529e5-9fa3-4085-940c-618cb66b3092</v>
+        <v>d98f4314-1eb0-4b75-8e53-e358b327cdac</v>
       </c>
       <c r="B29" s="5" t="str">
-        <v>6e2fc46f-8e17-4cb4-a929-49fdc8fdc11b</v>
+        <v>dec2e37d-1438-4b1b-9fd7-28ba3d5656f6</v>
       </c>
       <c r="C29" s="5" t="str">
-        <v>Intelligent Cotton Bacon</v>
+        <v>Small Wooden Shoes</v>
       </c>
       <c r="D29" s="5" t="str">
-        <v>4.5.9</v>
+        <v>7.0.2</v>
       </c>
       <c r="E29" s="5" t="str">
-        <v>October</v>
+        <v>January</v>
       </c>
       <c r="F29" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G29" s="5">
-        <v>43</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1">
       <c r="A30" s="4" t="str">
-        <v>2451dd7e-be89-4b51-8828-ab3064aa4e7e</v>
+        <v>3e4866ad-89ee-4681-b7e9-adde6dcf0c17</v>
       </c>
       <c r="B30" s="5" t="str">
-        <v>cbd76ec6-419d-4060-956a-eba49e05f53e</v>
+        <v>7776f8c6-afca-4330-bf1f-378385ede03b</v>
       </c>
       <c r="C30" s="5" t="str">
-        <v>Elegant Frozen Soap</v>
+        <v>Handmade Steel Bike</v>
       </c>
       <c r="D30" s="5" t="str">
-        <v>6.3.9</v>
+        <v>6.6.7</v>
       </c>
       <c r="E30" s="5" t="str">
         <v>May</v>
       </c>
       <c r="F30" s="5" t="str">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G30" s="5">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1">
       <c r="A31" s="4" t="str">
-        <v>035322d1-2b3e-44fc-a0dc-6124caa5cb36</v>
+        <v>62d85c84-3151-4556-880b-b02d64cb2034</v>
       </c>
       <c r="B31" s="5" t="str">
-        <v>c8398680-0428-4d8b-8998-c6caf21d76b1</v>
+        <v>877a530f-98fb-4659-9184-a76ca3f8aea7</v>
       </c>
       <c r="C31" s="5" t="str">
-        <v>Rustic Wooden Towels</v>
+        <v>Sleek Wooden Cheese</v>
       </c>
       <c r="D31" s="5" t="str">
-        <v>4.7.9</v>
+        <v>7.3.3</v>
       </c>
       <c r="E31" s="5" t="str">
-        <v>July</v>
+        <v>April</v>
       </c>
       <c r="F31" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G31" s="5">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" ht="30" customHeight="1">
       <c r="A32" s="4" t="str">
-        <v>2bcb622a-8c2d-42bf-b6d6-66f328cc3800</v>
+        <v>23dc5f3f-6ebf-450a-84c1-684fd22121ce</v>
       </c>
       <c r="B32" s="5" t="str">
-        <v>e6152fe5-3374-46e7-b9d2-9ae15409c7f5</v>
+        <v>95436008-f23c-41f2-9563-c6c56d3d4026</v>
       </c>
       <c r="C32" s="5" t="str">
-        <v>Rustic Frozen Chicken</v>
+        <v>Electronic Wooden Chair</v>
       </c>
       <c r="D32" s="5" t="str">
-        <v>1.8.8</v>
+        <v>7.0.4</v>
       </c>
       <c r="E32" s="5" t="str">
-        <v>February</v>
+        <v>August</v>
       </c>
       <c r="F32" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G32" s="5">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" ht="30" customHeight="1">
       <c r="A33" s="4" t="str">
-        <v>9dfecbec-e53d-419d-8e5b-e139bc6682fe</v>
+        <v>c98e85a3-df4d-4372-ae55-7081bb85d791</v>
       </c>
       <c r="B33" s="5" t="str">
-        <v>02fba024-2f6c-4772-97ee-368132e411a9</v>
+        <v>3fca8e29-e98e-4f26-994c-44bde577703a</v>
       </c>
       <c r="C33" s="5" t="str">
-        <v>Elegant Plastic Fish</v>
+        <v>Luxurious Fresh Pants</v>
       </c>
       <c r="D33" s="5" t="str">
-        <v>5.7.1</v>
+        <v>8.5.8</v>
       </c>
       <c r="E33" s="5" t="str">
-        <v>March</v>
+        <v>December</v>
       </c>
       <c r="F33" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G33" s="5">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1">
       <c r="A34" s="4" t="str">
-        <v>9ce4627e-6ad4-4ecf-915e-34f8edbb5114</v>
+        <v>4920558f-0350-48c6-adb2-979b751cf7dc</v>
       </c>
       <c r="B34" s="5" t="str">
-        <v>84b8e0f6-7a4c-4f2d-8683-27838e826a22</v>
+        <v>a68dea5d-9c83-44d9-85e7-afa3870e6707</v>
       </c>
       <c r="C34" s="5" t="str">
-        <v>Luxurious Bronze Cheese</v>
+        <v>Generic Concrete Towels</v>
       </c>
       <c r="D34" s="5" t="str">
-        <v>6.6.1</v>
+        <v>7.1.3</v>
       </c>
       <c r="E34" s="5" t="str">
-        <v>May</v>
+        <v>February</v>
       </c>
       <c r="F34" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G34" s="5">
-        <v>46</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" ht="30" customHeight="1">
       <c r="A35" s="4" t="str">
-        <v>df9c8217-e982-47a7-9e4c-76a309ab5337</v>
+        <v>7a19da62-cbdc-4915-8144-cfe6f32dce1a</v>
       </c>
       <c r="B35" s="5" t="str">
-        <v>28b8dcc3-1696-4cd0-9911-ffe9d4dd38a5</v>
+        <v>f2e84adf-7583-4cfb-b32e-626bc8e1016b</v>
       </c>
       <c r="C35" s="5" t="str">
-        <v>Awesome Rubber Sausages</v>
+        <v>Intelligent Wooden Hat</v>
       </c>
       <c r="D35" s="5" t="str">
-        <v>0.0.8</v>
+        <v>9.1.2</v>
       </c>
       <c r="E35" s="5" t="str">
-        <v>July</v>
+        <v>April</v>
       </c>
       <c r="F35" s="5" t="str">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G35" s="5">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" ht="30" customHeight="1">
       <c r="A36" s="4" t="str">
-        <v>8c271c88-be22-4c92-a20a-b1226d577d59</v>
+        <v>67f31117-f12f-402c-91d7-bd097918e362</v>
       </c>
       <c r="B36" s="5" t="str">
-        <v>479887c4-18e5-4670-8b24-05c134c6c55d</v>
+        <v>c5d3505d-44eb-47c1-9734-60f152d4ca5d</v>
       </c>
       <c r="C36" s="5" t="str">
-        <v>Sleek Granite Shoes</v>
+        <v>Refined Rubber Salad</v>
       </c>
       <c r="D36" s="5" t="str">
-        <v>3.7.2</v>
+        <v>0.3.8</v>
       </c>
       <c r="E36" s="5" t="str">
-        <v>January</v>
+        <v>September</v>
       </c>
       <c r="F36" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G36" s="5">
-        <v>45</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" ht="30" customHeight="1">
       <c r="A37" s="4" t="str">
-        <v>b4e4b1da-7c67-4a05-b3eb-c7de32125b4e</v>
+        <v>50f2d2a9-b943-41d0-819a-303edea09667</v>
       </c>
       <c r="B37" s="5" t="str">
-        <v>2186c89a-2dad-40f7-960f-2a333ea58127</v>
+        <v>843aa254-0c90-47cf-acf7-60ec166c4300</v>
       </c>
       <c r="C37" s="5" t="str">
-        <v>Generic Frozen Salad</v>
+        <v>Bespoke Cotton Ball</v>
       </c>
       <c r="D37" s="5" t="str">
-        <v>7.1.2</v>
+        <v>1.2.0</v>
       </c>
       <c r="E37" s="5" t="str">
-        <v>January</v>
+        <v>June</v>
       </c>
       <c r="F37" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G37" s="5">
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" ht="30" customHeight="1">
       <c r="A38" s="4" t="str">
-        <v>b0b41839-f14a-4fa1-af28-7166aa923b89</v>
+        <v>406c5bf5-b53c-4eeb-a845-e1e2aa0350d4</v>
       </c>
       <c r="B38" s="5" t="str">
-        <v>2eb5fbeb-4488-45e2-8814-fe3409afc6e0</v>
+        <v>511e0ee8-2f6c-490b-ab28-972604eea8d3</v>
       </c>
       <c r="C38" s="5" t="str">
-        <v>Oriental Plastic Chair</v>
+        <v>Elegant Steel Car</v>
       </c>
       <c r="D38" s="5" t="str">
-        <v>5.9.2</v>
+        <v>5.3.5</v>
       </c>
       <c r="E38" s="5" t="str">
-        <v>January</v>
+        <v>November</v>
       </c>
       <c r="F38" s="5" t="str">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G38" s="5">
-        <v>61</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" ht="30" customHeight="1">
       <c r="A39" s="4" t="str">
-        <v>86440df6-456c-4b4b-89bf-2005b19272b4</v>
+        <v>369be0da-3d55-41ea-9dd3-f4cae7994f3a</v>
       </c>
       <c r="B39" s="5" t="str">
-        <v>75fff9da-9548-4471-8750-3da51097a35c</v>
+        <v>5717b994-666e-425e-a980-d0d5d42e27c4</v>
       </c>
       <c r="C39" s="5" t="str">
-        <v>Bespoke Bronze Tuna</v>
+        <v>Recycled Soft Soap</v>
       </c>
       <c r="D39" s="5" t="str">
-        <v>9.1.3</v>
+        <v>2.2.1</v>
       </c>
       <c r="E39" s="5" t="str">
-        <v>October</v>
+        <v>March</v>
       </c>
       <c r="F39" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G39" s="5">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" ht="30" customHeight="1">
       <c r="A40" s="4" t="str">
-        <v>19085622-b8a0-4fcc-b102-c8ce1fdee17b</v>
+        <v>cacfca81-e258-4670-a9dd-752317682079</v>
       </c>
       <c r="B40" s="5" t="str">
-        <v>12b12ca1-8456-4121-8e6b-14c162a45ffa</v>
+        <v>6794ff77-4f8b-4844-b873-e4a265f89d40</v>
       </c>
       <c r="C40" s="5" t="str">
-        <v>Bespoke Steel Tuna</v>
+        <v>Awesome Bronze Towels</v>
       </c>
       <c r="D40" s="5" t="str">
-        <v>7.5.2</v>
+        <v>5.7.5</v>
       </c>
       <c r="E40" s="5" t="str">
-        <v>January</v>
+        <v>March</v>
       </c>
       <c r="F40" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G40" s="5">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" ht="30" customHeight="1">
       <c r="A41" s="4" t="str">
-        <v>6acf9a91-8a16-467b-9ac4-2c211f3d5781</v>
+        <v>a22d9d82-134c-4ebc-a197-bb17895b814e</v>
       </c>
       <c r="B41" s="5" t="str">
-        <v>0a4cb599-47a1-48fb-a95d-87246af5c1dc</v>
+        <v>26a2c745-050c-4bb3-be8f-a5a1dbbef7c7</v>
       </c>
       <c r="C41" s="5" t="str">
-        <v>Licensed Fresh Mouse</v>
+        <v>Handmade Granite Soap</v>
       </c>
       <c r="D41" s="5" t="str">
-        <v>3.0.5</v>
+        <v>3.2.9</v>
       </c>
       <c r="E41" s="5" t="str">
-        <v>May</v>
+        <v>March</v>
       </c>
       <c r="F41" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G41" s="5">
-        <v>52</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" ht="30" customHeight="1">
       <c r="A42" s="4" t="str">
-        <v>2a13cc6e-d2ab-4795-91a7-fdca90e55cf1</v>
+        <v>c6b2cc75-029e-473a-9ef7-98aec10fb449</v>
       </c>
       <c r="B42" s="5" t="str">
-        <v>c68a70f3-cdb3-4421-a7e2-f75ee152ee16</v>
+        <v>d0420817-8f3e-4e23-88f6-57bfce5a927a</v>
       </c>
       <c r="C42" s="5" t="str">
-        <v>Licensed Cotton Bacon</v>
+        <v>Bespoke Plastic Salad</v>
       </c>
       <c r="D42" s="5" t="str">
-        <v>3.1.0</v>
+        <v>1.0.1</v>
       </c>
       <c r="E42" s="5" t="str">
-        <v>April</v>
+        <v>May</v>
       </c>
       <c r="F42" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G42" s="5">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" ht="30" customHeight="1">
       <c r="A43" s="4" t="str">
-        <v>9ff8f035-d621-4e0c-80f2-b09f9261a83c</v>
+        <v>1b093ff3-171a-419d-9a0a-344cc23c84c4</v>
       </c>
       <c r="B43" s="5" t="str">
-        <v>6b5d42cd-faa0-4c63-9ded-771b9a7d08a2</v>
+        <v>1266aaf9-e7b0-44be-b870-a237d5822bf1</v>
       </c>
       <c r="C43" s="5" t="str">
-        <v>Incredible Rubber Computer</v>
+        <v>Oriental Frozen Bike</v>
       </c>
       <c r="D43" s="5" t="str">
-        <v>4.6.7</v>
+        <v>7.4.1</v>
       </c>
       <c r="E43" s="5" t="str">
-        <v>April</v>
+        <v>January</v>
       </c>
       <c r="F43" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G43" s="5">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" ht="30" customHeight="1">
       <c r="A44" s="4" t="str">
-        <v>95c42a11-594e-4e9c-9823-e4330749ca7c</v>
+        <v>39187941-7952-4c70-b93c-5cd90a1e48f8</v>
       </c>
       <c r="B44" s="5" t="str">
-        <v>f4a62b14-c465-4899-8b52-3b3d0aebda22</v>
+        <v>016340e5-e550-4fc0-b8d1-235f0ef4eb57</v>
       </c>
       <c r="C44" s="5" t="str">
-        <v>Handcrafted Metal Shoes</v>
+        <v>Electronic Fresh Gloves</v>
       </c>
       <c r="D44" s="5" t="str">
-        <v>5.6.3</v>
+        <v>0.2.7</v>
       </c>
       <c r="E44" s="5" t="str">
         <v>October</v>
       </c>
       <c r="F44" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G44" s="5">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" ht="30" customHeight="1">
       <c r="A45" s="4" t="str">
-        <v>8e339dde-8f79-44ae-9afc-003372990729</v>
+        <v>76849dc0-465f-4760-99cd-d99593b71959</v>
       </c>
       <c r="B45" s="5" t="str">
-        <v>af2038c2-53ea-4917-94f6-e53d16d9cc70</v>
+        <v>7a37a6ab-240b-4e9e-b433-90b7767c042d</v>
       </c>
       <c r="C45" s="5" t="str">
-        <v>Awesome Cotton Hat</v>
+        <v>Unbranded Bronze Shirt</v>
       </c>
       <c r="D45" s="5" t="str">
-        <v>1.5.5</v>
+        <v>7.3.8</v>
       </c>
       <c r="E45" s="5" t="str">
-        <v>April</v>
+        <v>September</v>
       </c>
       <c r="F45" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G45" s="5">
-        <v>36</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" ht="30" customHeight="1">
       <c r="A46" s="4" t="str">
-        <v>4582024b-c942-4170-8cac-8db9f2c21f4f</v>
+        <v>6a9d96cd-7d48-40f7-a12c-0a41c06a56f8</v>
       </c>
       <c r="B46" s="5" t="str">
-        <v>868e9bfd-709f-4f01-87c4-71279414c224</v>
+        <v>b7fb2a56-e386-44a5-add5-4353959ff849</v>
       </c>
       <c r="C46" s="5" t="str">
-        <v>Incredible Rubber Tuna</v>
+        <v>Ergonomic Cotton Shirt</v>
       </c>
       <c r="D46" s="5" t="str">
-        <v>4.5.8</v>
+        <v>9.5.3</v>
       </c>
       <c r="E46" s="5" t="str">
-        <v>December</v>
+        <v>March</v>
       </c>
       <c r="F46" s="5" t="str">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G46" s="5">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" ht="30" customHeight="1">
       <c r="A47" s="4" t="str">
-        <v>9658c0a5-593c-45bf-8e02-239ef9db0797</v>
+        <v>930f32e9-5718-4b7c-921b-bb0b24d8a3fc</v>
       </c>
       <c r="B47" s="5" t="str">
-        <v>81fd269b-9fc9-45e8-9d4e-506d34ab9d96</v>
+        <v>68f1b627-1082-441a-948a-c0a2d824585b</v>
       </c>
       <c r="C47" s="5" t="str">
-        <v>Sleek Bronze Shirt</v>
+        <v>Incredible Metal Bike</v>
       </c>
       <c r="D47" s="5" t="str">
-        <v>6.6.5</v>
+        <v>5.4.6</v>
       </c>
       <c r="E47" s="5" t="str">
-        <v>June</v>
+        <v>December</v>
       </c>
       <c r="F47" s="5" t="str">
         <v>2023</v>
@@ -1576,131 +1576,131 @@
     </row>
     <row r="48" ht="30" customHeight="1">
       <c r="A48" s="4" t="str">
-        <v>63c1b211-2bb8-47d9-ae97-ebd7d9430d96</v>
+        <v>1fa4e04e-1d71-4357-bb0d-42d9aa7655ab</v>
       </c>
       <c r="B48" s="5" t="str">
-        <v>2ee820db-ad6f-4e85-8a7e-48322a1cf4f8</v>
+        <v>072f5b25-41a4-42f6-9051-7848e049d26f</v>
       </c>
       <c r="C48" s="5" t="str">
-        <v>Ergonomic Frozen Chips</v>
+        <v>Recycled Cotton Ball</v>
       </c>
       <c r="D48" s="5" t="str">
-        <v>3.9.1</v>
+        <v>5.7.9</v>
       </c>
       <c r="E48" s="5" t="str">
-        <v>July</v>
+        <v>October</v>
       </c>
       <c r="F48" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G48" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" ht="30" customHeight="1">
       <c r="A49" s="4" t="str">
-        <v>835276e0-0beb-4343-9b3f-f831c7702f29</v>
+        <v>79b744fa-bd01-4f96-bcd5-bbc6dd6f47b9</v>
       </c>
       <c r="B49" s="5" t="str">
-        <v>05730539-bbc6-4320-b44a-34cae1032960</v>
+        <v>3e86445f-62de-4c06-9cb4-f15ebe2bd829</v>
       </c>
       <c r="C49" s="5" t="str">
-        <v>Bespoke Steel Tuna</v>
+        <v>Unbranded Fresh Computer</v>
       </c>
       <c r="D49" s="5" t="str">
-        <v>9.3.8</v>
+        <v>2.7.1</v>
       </c>
       <c r="E49" s="5" t="str">
-        <v>December</v>
+        <v>January</v>
       </c>
       <c r="F49" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G49" s="5">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" ht="30" customHeight="1">
       <c r="A50" s="4" t="str">
-        <v>5bd7b32e-2ef3-4d89-8c40-1789d7962159</v>
+        <v>e61fdf2c-0aa5-4151-89ea-44f4a86a6879</v>
       </c>
       <c r="B50" s="5" t="str">
-        <v>601be037-f587-40fb-bedf-786604c27560</v>
+        <v>3fe2f8d1-bb42-40d7-b857-5c11e75d6bf7</v>
       </c>
       <c r="C50" s="5" t="str">
-        <v>Handmade Concrete Ball</v>
+        <v>Tasty Fresh Chicken</v>
       </c>
       <c r="D50" s="5" t="str">
-        <v>1.1.9</v>
+        <v>8.2.9</v>
       </c>
       <c r="E50" s="5" t="str">
-        <v>August</v>
+        <v>April</v>
       </c>
       <c r="F50" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G50" s="5">
-        <v>38</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" ht="30" customHeight="1">
       <c r="A51" s="4" t="str">
-        <v>354d29ed-0e29-4048-a85d-d5023a8f5c55</v>
+        <v>57a98edd-bdf8-42ad-8bb5-97f6a0aec04a</v>
       </c>
       <c r="B51" s="5" t="str">
-        <v>66691758-eecd-43ac-9dab-2e9d5ee93c98</v>
+        <v>badc56be-b539-4268-a5f6-f5ed7afae14a</v>
       </c>
       <c r="C51" s="5" t="str">
-        <v>Electronic Bronze Pizza</v>
+        <v>Practical Fresh Bacon</v>
       </c>
       <c r="D51" s="5" t="str">
-        <v>5.0.9</v>
+        <v>0.9.7</v>
       </c>
       <c r="E51" s="5" t="str">
-        <v>March</v>
+        <v>October</v>
       </c>
       <c r="F51" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G51" s="5">
-        <v>1</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" ht="30" customHeight="1">
       <c r="A52" s="4" t="str">
-        <v>eefe644c-2a72-48e8-856d-54f1e4ebe67e</v>
+        <v>39c46bbe-b5d2-4f0f-9928-1d3e3a6b4cba</v>
       </c>
       <c r="B52" s="5" t="str">
-        <v>c563c30f-0053-4a36-a1fe-cee07bcdfee5</v>
+        <v>0755067d-75db-408f-8808-835e4d3af651</v>
       </c>
       <c r="C52" s="5" t="str">
-        <v>Luxurious Wooden Bacon</v>
+        <v>Incredible Rubber Tuna</v>
       </c>
       <c r="D52" s="5" t="str">
-        <v>8.8.0</v>
+        <v>2.2.9</v>
       </c>
       <c r="E52" s="5" t="str">
-        <v>November</v>
+        <v>December</v>
       </c>
       <c r="F52" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G52" s="5">
-        <v>36</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" ht="30" customHeight="1">
       <c r="A53" s="4" t="str">
-        <v>c3bc06f7-7440-4981-9c5e-9639f302d439</v>
+        <v>0b5aebe9-1ab2-44e7-80da-ca81d1d823d8</v>
       </c>
       <c r="B53" s="5" t="str">
-        <v>464f7767-68c5-4152-bace-76b6249206f3</v>
+        <v>56985ac1-93ed-4ee8-b31f-1dcca3d58405</v>
       </c>
       <c r="C53" s="5" t="str">
-        <v>Incredible Cotton Gloves</v>
+        <v>Rustic Steel Bike</v>
       </c>
       <c r="D53" s="5" t="str">
-        <v>4.9.5</v>
+        <v>1.8.0</v>
       </c>
       <c r="E53" s="5" t="str">
         <v>March</v>
@@ -1709,251 +1709,251 @@
         <v>2023</v>
       </c>
       <c r="G53" s="5">
-        <v>55</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" ht="30" customHeight="1">
       <c r="A54" s="4" t="str">
-        <v>2c7ff04c-1c15-4a12-9874-e55b15f72067</v>
+        <v>057bd020-9d8b-4447-9da0-8effb09ab224</v>
       </c>
       <c r="B54" s="5" t="str">
-        <v>6821cfb6-0a38-4545-b403-c0409c58e171</v>
+        <v>7a5afab9-8449-4be9-827e-2d4acba7270d</v>
       </c>
       <c r="C54" s="5" t="str">
-        <v>Refined Soft Chair</v>
+        <v>Handcrafted Rubber Tuna</v>
       </c>
       <c r="D54" s="5" t="str">
-        <v>4.2.9</v>
+        <v>0.4.5</v>
       </c>
       <c r="E54" s="5" t="str">
-        <v>July</v>
+        <v>November</v>
       </c>
       <c r="F54" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G54" s="5">
-        <v>32</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" ht="30" customHeight="1">
       <c r="A55" s="4" t="str">
-        <v>6be3a530-c846-4023-b43d-4e51834973ab</v>
+        <v>a2d26164-2932-4023-9725-11d6fc564359</v>
       </c>
       <c r="B55" s="5" t="str">
-        <v>2ae66705-c7e7-4a4d-9f06-dee91eb71a99</v>
+        <v>1c83b68f-6ca9-416e-8842-7f3cdcdff49f</v>
       </c>
       <c r="C55" s="5" t="str">
-        <v>Handcrafted Steel Soap</v>
+        <v>Unbranded Cotton Fish</v>
       </c>
       <c r="D55" s="5" t="str">
-        <v>2.3.1</v>
+        <v>4.3.2</v>
       </c>
       <c r="E55" s="5" t="str">
-        <v>May</v>
+        <v>November</v>
       </c>
       <c r="F55" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G55" s="5">
-        <v>98</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" ht="30" customHeight="1">
       <c r="A56" s="4" t="str">
-        <v>e99de7fc-4e8a-4679-9a8b-0bc1c868e178</v>
+        <v>dcc75fde-fa16-4154-9271-08e7f69b0ef0</v>
       </c>
       <c r="B56" s="5" t="str">
-        <v>1234be2b-63cb-4234-80e9-0d60704badcb</v>
+        <v>1508d3d5-c80e-40b3-ade7-f5ec8230a264</v>
       </c>
       <c r="C56" s="5" t="str">
-        <v>Sleek Bronze Hat</v>
+        <v>Oriental Plastic Computer</v>
       </c>
       <c r="D56" s="5" t="str">
-        <v>2.1.8</v>
+        <v>7.9.5</v>
       </c>
       <c r="E56" s="5" t="str">
-        <v>August</v>
+        <v>January</v>
       </c>
       <c r="F56" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G56" s="5">
-        <v>8</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" ht="30" customHeight="1">
       <c r="A57" s="4" t="str">
-        <v>6db81d20-df88-435a-8dda-2ffae21d4378</v>
+        <v>87858788-8d61-47f0-82d2-b89c522f600b</v>
       </c>
       <c r="B57" s="5" t="str">
-        <v>870e2722-a807-4e47-aca7-c8de8491eda8</v>
+        <v>b08a9d00-0964-45cc-9d68-961d477960de</v>
       </c>
       <c r="C57" s="5" t="str">
-        <v>Tasty Bronze Chips</v>
+        <v>Refined Plastic Tuna</v>
       </c>
       <c r="D57" s="5" t="str">
-        <v>5.4.0</v>
+        <v>3.5.7</v>
       </c>
       <c r="E57" s="5" t="str">
-        <v>February</v>
+        <v>April</v>
       </c>
       <c r="F57" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G57" s="5">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" ht="30" customHeight="1">
       <c r="A58" s="4" t="str">
-        <v>e37ecee1-7e79-4c3c-9ff1-04847b9b5b2d</v>
+        <v>9f643228-a6c1-4595-acaf-a655b9e9c23f</v>
       </c>
       <c r="B58" s="5" t="str">
-        <v>8dc14153-5bf4-4239-a7b2-e703e01cca54</v>
+        <v>66c45cc0-2327-429e-b57d-bd938c6d2b31</v>
       </c>
       <c r="C58" s="5" t="str">
-        <v>Electronic Steel Bacon</v>
+        <v>Intelligent Plastic Salad</v>
       </c>
       <c r="D58" s="5" t="str">
-        <v>6.7.6</v>
+        <v>9.5.5</v>
       </c>
       <c r="E58" s="5" t="str">
-        <v>August</v>
+        <v>July</v>
       </c>
       <c r="F58" s="5" t="str">
         <v>2022</v>
       </c>
       <c r="G58" s="5">
-        <v>74</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" ht="30" customHeight="1">
       <c r="A59" s="4" t="str">
-        <v>aa14a90f-e164-4149-b040-439acd5e5263</v>
+        <v>f4740773-9207-464a-bdeb-5a46213a0d5d</v>
       </c>
       <c r="B59" s="5" t="str">
-        <v>1e6f07ad-8868-4a1c-94d1-d2c7ec35e998</v>
+        <v>a09552a9-1c9c-43ce-a080-4103d16e7707</v>
       </c>
       <c r="C59" s="5" t="str">
-        <v>Luxurious Bronze Pants</v>
+        <v>Practical Fresh Shirt</v>
       </c>
       <c r="D59" s="5" t="str">
-        <v>7.9.2</v>
+        <v>1.7.5</v>
       </c>
       <c r="E59" s="5" t="str">
-        <v>July</v>
+        <v>March</v>
       </c>
       <c r="F59" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G59" s="5">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" ht="30" customHeight="1">
       <c r="A60" s="4" t="str">
-        <v>914f4dc3-aa63-4581-b397-609fbdfb5dfb</v>
+        <v>e97909bd-fc37-4bb0-ab8b-3c5a03c4d93d</v>
       </c>
       <c r="B60" s="5" t="str">
-        <v>a4b44115-3484-418e-87e6-779014fe7c1b</v>
+        <v>eb80715c-ed51-4c53-a0be-cda2e07b9a8f</v>
       </c>
       <c r="C60" s="5" t="str">
-        <v>Bespoke Rubber Bike</v>
+        <v>Awesome Frozen Bike</v>
       </c>
       <c r="D60" s="5" t="str">
-        <v>2.9.7</v>
+        <v>2.7.9</v>
       </c>
       <c r="E60" s="5" t="str">
-        <v>April</v>
+        <v>December</v>
       </c>
       <c r="F60" s="5" t="str">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G60" s="5">
-        <v>23</v>
+        <v>90</v>
       </c>
     </row>
     <row r="61" ht="30" customHeight="1">
       <c r="A61" s="4" t="str">
-        <v>24cb97ac-a149-423d-91a4-0da7bf5240e1</v>
+        <v>c3c7acd3-405b-4936-9128-c69b0b407ab1</v>
       </c>
       <c r="B61" s="5" t="str">
-        <v>0be10113-02d5-4b7c-8108-9cabf501d012</v>
+        <v>56ab48d3-29ea-4b53-ac7e-5d8a9bdee47f</v>
       </c>
       <c r="C61" s="5" t="str">
-        <v>Practical Rubber Chips</v>
+        <v>Tasty Soft Sausages</v>
       </c>
       <c r="D61" s="5" t="str">
-        <v>9.3.5</v>
+        <v>4.8.5</v>
       </c>
       <c r="E61" s="5" t="str">
-        <v>June</v>
+        <v>December</v>
       </c>
       <c r="F61" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G61" s="5">
-        <v>85</v>
+        <v>54</v>
       </c>
     </row>
     <row r="62" ht="30" customHeight="1">
       <c r="A62" s="4" t="str">
-        <v>1788bca1-f6ac-496f-b674-6ccbb60cf3b9</v>
+        <v>97e03655-7d11-491c-9bca-b527c6a42ff5</v>
       </c>
       <c r="B62" s="5" t="str">
-        <v>fad00c6a-6e0c-4b80-a8c2-5cce2eb14dc7</v>
+        <v>5a3e01fa-cc5b-4f03-bb4e-cd130ec3ee4b</v>
       </c>
       <c r="C62" s="5" t="str">
-        <v>Practical Bronze Keyboard</v>
+        <v>Handcrafted Wooden Pants</v>
       </c>
       <c r="D62" s="5" t="str">
-        <v>1.5.9</v>
+        <v>4.8.8</v>
       </c>
       <c r="E62" s="5" t="str">
-        <v>October</v>
+        <v>September</v>
       </c>
       <c r="F62" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G62" s="5">
-        <v>6</v>
+        <v>87</v>
       </c>
     </row>
     <row r="63" ht="30" customHeight="1">
       <c r="A63" s="4" t="str">
-        <v>55b78e92-a715-4f16-bf50-65fd39133ce0</v>
+        <v>1d53987d-35b2-4c8d-81ac-f2d69a139d16</v>
       </c>
       <c r="B63" s="5" t="str">
-        <v>c0e60052-f4e6-4111-95c2-7d0383237612</v>
+        <v>14a51ed7-e4d6-4590-b6f1-7bf95947c4e9</v>
       </c>
       <c r="C63" s="5" t="str">
-        <v>Small Frozen Pizza</v>
+        <v>Incredible Concrete Ball</v>
       </c>
       <c r="D63" s="5" t="str">
-        <v>3.7.3</v>
+        <v>3.6.2</v>
       </c>
       <c r="E63" s="5" t="str">
-        <v>January</v>
+        <v>October</v>
       </c>
       <c r="F63" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G63" s="5">
-        <v>27</v>
+        <v>84</v>
       </c>
     </row>
     <row r="64" ht="30" customHeight="1">
       <c r="A64" s="4" t="str">
-        <v>6b031a32-fc11-497d-9c26-3bc91a8a47bf</v>
+        <v>1aa78a37-4181-485c-9cd1-90cf6f4c85c1</v>
       </c>
       <c r="B64" s="5" t="str">
-        <v>9d1229b4-7689-4f4f-8192-3b22f4b09a2e</v>
+        <v>23ca0406-baf7-4335-9b0e-a12368b290a3</v>
       </c>
       <c r="C64" s="5" t="str">
-        <v>Recycled Soft Bacon</v>
+        <v>Licensed Cotton Shoes</v>
       </c>
       <c r="D64" s="5" t="str">
-        <v>1.2.2</v>
+        <v>8.6.3</v>
       </c>
       <c r="E64" s="5" t="str">
         <v>February</v>
@@ -1962,113 +1962,113 @@
         <v>2023</v>
       </c>
       <c r="G64" s="5">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="65" ht="30" customHeight="1">
       <c r="A65" s="4" t="str">
-        <v>749650fa-4da2-48f2-8b5b-23ee3b56843b</v>
+        <v>c2c9cbf7-122f-4bbd-be35-694a67ea2214</v>
       </c>
       <c r="B65" s="5" t="str">
-        <v>3381d339-e39a-4a7f-9fe2-c817fb594156</v>
+        <v>3ac4af47-92f5-4526-9fcd-8955e4d8bc70</v>
       </c>
       <c r="C65" s="5" t="str">
-        <v>Electronic Granite Bacon</v>
+        <v>Oriental Metal Pants</v>
       </c>
       <c r="D65" s="5" t="str">
-        <v>8.0.1</v>
+        <v>9.6.4</v>
       </c>
       <c r="E65" s="5" t="str">
-        <v>November</v>
+        <v>January</v>
       </c>
       <c r="F65" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G65" s="5">
-        <v>31</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" ht="30" customHeight="1">
       <c r="A66" s="4" t="str">
-        <v>de4507ed-2f68-4e34-b182-bbf29e6a6a7c</v>
+        <v>c8f2bdc8-940c-4133-80c9-41147a5e9539</v>
       </c>
       <c r="B66" s="5" t="str">
-        <v>da718708-4f09-418d-bcee-f4d5dd32c291</v>
+        <v>2b26f5d9-1456-4266-a8ab-3c813cdbf128</v>
       </c>
       <c r="C66" s="5" t="str">
-        <v>Refined Fresh Pizza</v>
+        <v>Recycled Plastic Car</v>
       </c>
       <c r="D66" s="5" t="str">
-        <v>0.2.9</v>
+        <v>2.9.5</v>
       </c>
       <c r="E66" s="5" t="str">
-        <v>June</v>
+        <v>April</v>
       </c>
       <c r="F66" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G66" s="5">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="67" ht="30" customHeight="1">
       <c r="A67" s="4" t="str">
-        <v>ab1963c6-4079-49e8-8c22-42ae676abe51</v>
+        <v>7e311719-0ec1-4276-bab3-ef15cdb46069</v>
       </c>
       <c r="B67" s="5" t="str">
-        <v>19766afe-ef02-405c-8ed7-dcff903fe400</v>
+        <v>75a95ab8-eee9-4932-bc35-13e45b917e39</v>
       </c>
       <c r="C67" s="5" t="str">
-        <v>Intelligent Soft Cheese</v>
+        <v>Incredible Metal Bike</v>
       </c>
       <c r="D67" s="5" t="str">
-        <v>2.2.4</v>
+        <v>4.4.7</v>
       </c>
       <c r="E67" s="5" t="str">
-        <v>August</v>
+        <v>October</v>
       </c>
       <c r="F67" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G67" s="5">
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="68" ht="30" customHeight="1">
       <c r="A68" s="4" t="str">
-        <v>56c66691-ae3c-48af-bffa-95336f05c897</v>
+        <v>0162e2e6-f8db-4be3-b810-4c20f88d399b</v>
       </c>
       <c r="B68" s="5" t="str">
-        <v>fa557a6e-8e7e-4d74-9bb5-4e897f7d9851</v>
+        <v>7978f736-ad65-4166-9832-f44d157b4f14</v>
       </c>
       <c r="C68" s="5" t="str">
-        <v>Fantastic Fresh Chicken</v>
+        <v>Rustic Bronze Hat</v>
       </c>
       <c r="D68" s="5" t="str">
-        <v>6.8.8</v>
+        <v>7.0.7</v>
       </c>
       <c r="E68" s="5" t="str">
-        <v>December</v>
+        <v>March</v>
       </c>
       <c r="F68" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G68" s="5">
-        <v>74</v>
+        <v>88</v>
       </c>
     </row>
     <row r="69" ht="30" customHeight="1">
       <c r="A69" s="4" t="str">
-        <v>34499e9b-da5a-4c3f-9dba-55b3c61123d0</v>
+        <v>d59a0011-0475-47d7-9a43-0358b6510b67</v>
       </c>
       <c r="B69" s="5" t="str">
-        <v>79636a8b-32e8-4668-b35e-f237ae934eaa</v>
+        <v>ccd99918-b6c3-479a-bcbc-bf36d624af89</v>
       </c>
       <c r="C69" s="5" t="str">
-        <v>Generic Bronze Mouse</v>
+        <v>Unbranded Granite Mouse</v>
       </c>
       <c r="D69" s="5" t="str">
-        <v>8.6.3</v>
+        <v>6.9.2</v>
       </c>
       <c r="E69" s="5" t="str">
         <v>December</v>
@@ -2077,182 +2077,182 @@
         <v>2023</v>
       </c>
       <c r="G69" s="5">
-        <v>35</v>
+        <v>53</v>
       </c>
     </row>
     <row r="70" ht="30" customHeight="1">
       <c r="A70" s="4" t="str">
-        <v>e0f61352-7910-4ef7-9e79-16724cd0f139</v>
+        <v>4a5ae1e6-b1a2-450f-9715-7219a85ec686</v>
       </c>
       <c r="B70" s="5" t="str">
-        <v>8d3eca56-87c0-4606-9c4e-15efca4c08dd</v>
+        <v>cb3a482d-bee6-4f1a-83c8-ea6ad4ef1bf5</v>
       </c>
       <c r="C70" s="5" t="str">
-        <v>Elegant Granite Mouse</v>
+        <v>Recycled Concrete Car</v>
       </c>
       <c r="D70" s="5" t="str">
-        <v>4.1.8</v>
+        <v>2.4.8</v>
       </c>
       <c r="E70" s="5" t="str">
-        <v>March</v>
+        <v>November</v>
       </c>
       <c r="F70" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G70" s="5">
-        <v>90</v>
+        <v>27</v>
       </c>
     </row>
     <row r="71" ht="30" customHeight="1">
       <c r="A71" s="4" t="str">
-        <v>cb43706d-d9e6-4a3f-970e-7037f1dc2351</v>
+        <v>9bc58a44-a1c7-4d7f-a0cc-431923f9e437</v>
       </c>
       <c r="B71" s="5" t="str">
-        <v>03e62f7b-bc6f-4817-98e9-af86e2095afd</v>
+        <v>98a69bbf-8b28-44e1-85f6-f4918efa7830</v>
       </c>
       <c r="C71" s="5" t="str">
-        <v>Fantastic Plastic Mouse</v>
+        <v>Modern Rubber Chips</v>
       </c>
       <c r="D71" s="5" t="str">
-        <v>4.8.4</v>
+        <v>7.5.7</v>
       </c>
       <c r="E71" s="5" t="str">
-        <v>March</v>
+        <v>November</v>
       </c>
       <c r="F71" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G71" s="5">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="72" ht="30" customHeight="1">
       <c r="A72" s="4" t="str">
-        <v>bd67d8bc-9ff9-431f-bfd4-a849b5d8e27d</v>
+        <v>c65b8a54-ee85-4b23-a2df-af9e7681a7df</v>
       </c>
       <c r="B72" s="5" t="str">
-        <v>5f518949-f0f6-4de2-819f-982783395be4</v>
+        <v>d09f45a0-f232-440d-99f7-ba385294d69a</v>
       </c>
       <c r="C72" s="5" t="str">
-        <v>Oriental Cotton Shirt</v>
+        <v>Sleek Frozen Gloves</v>
       </c>
       <c r="D72" s="5" t="str">
-        <v>7.2.7</v>
+        <v>4.7.5</v>
       </c>
       <c r="E72" s="5" t="str">
-        <v>September</v>
+        <v>August</v>
       </c>
       <c r="F72" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G72" s="5">
-        <v>56</v>
+        <v>25</v>
       </c>
     </row>
     <row r="73" ht="30" customHeight="1">
       <c r="A73" s="4" t="str">
-        <v>3c420f5c-6f92-4622-982c-548b9c40a84f</v>
+        <v>e6ad3761-4dcf-4ed2-ad53-5f6aeed475b6</v>
       </c>
       <c r="B73" s="5" t="str">
-        <v>da452fa9-50ad-4c56-b943-bd263eee1549</v>
+        <v>337f8395-a929-45f6-999c-5abe6008884d</v>
       </c>
       <c r="C73" s="5" t="str">
-        <v>Bespoke Frozen Soap</v>
+        <v>Ergonomic Cotton Shoes</v>
       </c>
       <c r="D73" s="5" t="str">
-        <v>7.4.3</v>
+        <v>8.4.6</v>
       </c>
       <c r="E73" s="5" t="str">
-        <v>May</v>
+        <v>April</v>
       </c>
       <c r="F73" s="5" t="str">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G73" s="5">
-        <v>32</v>
+        <v>73</v>
       </c>
     </row>
     <row r="74" ht="30" customHeight="1">
       <c r="A74" s="4" t="str">
-        <v>69e280b5-f8ef-4328-9d9a-aebd4106e864</v>
+        <v>e0ace7f6-ff87-4865-a705-f06226f5aaa9</v>
       </c>
       <c r="B74" s="5" t="str">
-        <v>51056112-ad25-4e56-961f-70baeebeeb78</v>
+        <v>46891b4d-9f00-449e-9e9e-b20abf94a57e</v>
       </c>
       <c r="C74" s="5" t="str">
-        <v>Handmade Rubber Hat</v>
+        <v>Oriental Bronze Chips</v>
       </c>
       <c r="D74" s="5" t="str">
-        <v>1.7.8</v>
+        <v>9.7.8</v>
       </c>
       <c r="E74" s="5" t="str">
-        <v>May</v>
+        <v>January</v>
       </c>
       <c r="F74" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G74" s="5">
-        <v>69</v>
+        <v>34</v>
       </c>
     </row>
     <row r="75" ht="30" customHeight="1">
       <c r="A75" s="4" t="str">
-        <v>f8689c6a-39ae-4865-b5f4-cbffa7d1bfc9</v>
+        <v>ccf54998-037f-4618-8c79-e1e5d694458e</v>
       </c>
       <c r="B75" s="5" t="str">
-        <v>7c92f0a5-65b0-444f-8d7f-fe31a085683c</v>
+        <v>71ab73df-305b-481e-b0a0-4856e8f37c07</v>
       </c>
       <c r="C75" s="5" t="str">
-        <v>Intelligent Soft Fish</v>
+        <v>Elegant Concrete Gloves</v>
       </c>
       <c r="D75" s="5" t="str">
-        <v>6.5.6</v>
+        <v>7.9.7</v>
       </c>
       <c r="E75" s="5" t="str">
-        <v>March</v>
+        <v>September</v>
       </c>
       <c r="F75" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G75" s="5">
-        <v>79</v>
+        <v>97</v>
       </c>
     </row>
     <row r="76" ht="30" customHeight="1">
       <c r="A76" s="4" t="str">
-        <v>0150f27e-33a7-4653-abc4-c329fa3a0a6b</v>
+        <v>a9f188b6-617c-4b5b-8a25-843ac29a71f5</v>
       </c>
       <c r="B76" s="5" t="str">
-        <v>ce8f11c9-08df-4484-85cf-6161da484bea</v>
+        <v>e2bcdfbb-7bc1-43d4-86c3-40aa1685cb8f</v>
       </c>
       <c r="C76" s="5" t="str">
-        <v>Handcrafted Plastic Chicken</v>
+        <v>Ergonomic Bronze Bike</v>
       </c>
       <c r="D76" s="5" t="str">
-        <v>1.8.7</v>
+        <v>8.2.6</v>
       </c>
       <c r="E76" s="5" t="str">
-        <v>January</v>
+        <v>July</v>
       </c>
       <c r="F76" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G76" s="5">
-        <v>28</v>
+        <v>52</v>
       </c>
     </row>
     <row r="77" ht="30" customHeight="1">
       <c r="A77" s="4" t="str">
-        <v>c653aebf-5567-414b-a286-0dd5b7d9d641</v>
+        <v>c6fb2282-47dd-45e1-9b6a-ad8572b308e1</v>
       </c>
       <c r="B77" s="5" t="str">
-        <v>d748f9b3-243d-41ab-bfb0-547a83ceba5f</v>
+        <v>38908d65-00a0-464e-8090-cf3bb91e7b91</v>
       </c>
       <c r="C77" s="5" t="str">
-        <v>Elegant Steel Chicken</v>
+        <v>Rustic Concrete Pants</v>
       </c>
       <c r="D77" s="5" t="str">
-        <v>5.4.9</v>
+        <v>1.4.0</v>
       </c>
       <c r="E77" s="5" t="str">
         <v>April</v>
@@ -2261,559 +2261,559 @@
         <v>2023</v>
       </c>
       <c r="G77" s="5">
-        <v>74</v>
+        <v>15</v>
       </c>
     </row>
     <row r="78" ht="30" customHeight="1">
       <c r="A78" s="4" t="str">
-        <v>46b6e175-45fd-4e7b-a301-4a1717da4b46</v>
+        <v>1f681467-3c19-4924-b3d9-7b80f6ae2e77</v>
       </c>
       <c r="B78" s="5" t="str">
-        <v>14f7f2af-e684-4643-a728-be30c87274fb</v>
+        <v>c9240813-4947-4ab6-9b4b-81bcb0893fd3</v>
       </c>
       <c r="C78" s="5" t="str">
-        <v>Luxurious Plastic Fish</v>
+        <v>Bespoke Metal Car</v>
       </c>
       <c r="D78" s="5" t="str">
-        <v>5.9.7</v>
+        <v>0.3.0</v>
       </c>
       <c r="E78" s="5" t="str">
-        <v>August</v>
+        <v>October</v>
       </c>
       <c r="F78" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G78" s="5">
-        <v>9</v>
+        <v>48</v>
       </c>
     </row>
     <row r="79" ht="30" customHeight="1">
       <c r="A79" s="4" t="str">
-        <v>4c604dbb-df60-4d42-8a2e-f10faaf4b316</v>
+        <v>bebe33bc-a7fb-4819-88d1-46b87ba20968</v>
       </c>
       <c r="B79" s="5" t="str">
-        <v>14c7398a-f245-4667-91ae-a20e719d4ce9</v>
+        <v>03f980a7-ff54-4838-aa5a-4c2ad2eabd8e</v>
       </c>
       <c r="C79" s="5" t="str">
-        <v>Elegant Steel Shoes</v>
+        <v>Elegant Wooden Bacon</v>
       </c>
       <c r="D79" s="5" t="str">
-        <v>4.9.8</v>
+        <v>7.4.7</v>
       </c>
       <c r="E79" s="5" t="str">
-        <v>July</v>
+        <v>March</v>
       </c>
       <c r="F79" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G79" s="5">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="80" ht="30" customHeight="1">
       <c r="A80" s="4" t="str">
-        <v>591eca31-abfd-459a-b954-f52f9dbfc01d</v>
+        <v>591b6e55-6f72-448a-acbf-081cedf0c5f6</v>
       </c>
       <c r="B80" s="5" t="str">
-        <v>cd92080e-6f62-41c8-ae53-822353edfc25</v>
+        <v>96ba4cf9-37d6-4cf9-9dea-33ef114e07ad</v>
       </c>
       <c r="C80" s="5" t="str">
-        <v>Recycled Cotton Fish</v>
+        <v>Licensed Granite Soap</v>
       </c>
       <c r="D80" s="5" t="str">
-        <v>9.0.1</v>
+        <v>2.7.9</v>
       </c>
       <c r="E80" s="5" t="str">
-        <v>March</v>
+        <v>June</v>
       </c>
       <c r="F80" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G80" s="5">
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
     <row r="81" ht="30" customHeight="1">
       <c r="A81" s="4" t="str">
-        <v>6d5d7e95-e777-45dd-8e3c-77275bbbb91f</v>
+        <v>2f3ab84b-e9bd-4624-b5e5-c54aa9ae03f4</v>
       </c>
       <c r="B81" s="5" t="str">
-        <v>90c61e50-45b8-41d8-b223-f58721f98587</v>
+        <v>96831afd-bd51-4dc7-bf3c-040805af958f</v>
       </c>
       <c r="C81" s="5" t="str">
-        <v>Rustic Concrete Sausages</v>
+        <v>Fantastic Granite Shirt</v>
       </c>
       <c r="D81" s="5" t="str">
-        <v>8.1.3</v>
+        <v>1.3.6</v>
       </c>
       <c r="E81" s="5" t="str">
-        <v>July</v>
+        <v>November</v>
       </c>
       <c r="F81" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G81" s="5">
-        <v>23</v>
+        <v>99</v>
       </c>
     </row>
     <row r="82" ht="30" customHeight="1">
       <c r="A82" s="4" t="str">
-        <v>cb744bee-975f-4890-96f9-27793a1ec308</v>
+        <v>f1d0c06a-7a7b-476b-93fd-1509f0c754c8</v>
       </c>
       <c r="B82" s="5" t="str">
-        <v>c158aa32-6230-408e-bca3-6090d22f8581</v>
+        <v>89ead73b-c0ff-4556-a4c3-50dab723b047</v>
       </c>
       <c r="C82" s="5" t="str">
-        <v>Electronic Bronze Gloves</v>
+        <v>Refined Cotton Shoes</v>
       </c>
       <c r="D82" s="5" t="str">
-        <v>5.5.7</v>
+        <v>9.0.5</v>
       </c>
       <c r="E82" s="5" t="str">
-        <v>August</v>
+        <v>June</v>
       </c>
       <c r="F82" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G82" s="5">
-        <v>65</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" ht="30" customHeight="1">
       <c r="A83" s="4" t="str">
-        <v>b6bea2ed-ea92-4112-9df8-201a18a71806</v>
+        <v>0e13b35b-4018-4dd5-ab9d-1c9a063ed018</v>
       </c>
       <c r="B83" s="5" t="str">
-        <v>346f2deb-f473-4abe-a9da-f8879eabe80b</v>
+        <v>d9cb4300-c2ea-4c50-b1d5-2934fd5ab2b0</v>
       </c>
       <c r="C83" s="5" t="str">
-        <v>Handmade Plastic Car</v>
+        <v>Licensed Cotton Cheese</v>
       </c>
       <c r="D83" s="5" t="str">
-        <v>1.6.5</v>
+        <v>7.9.6</v>
       </c>
       <c r="E83" s="5" t="str">
-        <v>August</v>
+        <v>March</v>
       </c>
       <c r="F83" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G83" s="5">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="84" ht="30" customHeight="1">
       <c r="A84" s="4" t="str">
-        <v>123fe60f-1666-406c-aeb0-aa523d5dac06</v>
+        <v>510a7384-f1c7-499b-a88d-88a290d2e9b2</v>
       </c>
       <c r="B84" s="5" t="str">
-        <v>ed37af3e-2c67-4713-8299-296c6fd3cb14</v>
+        <v>6f2bc06f-7fe5-4e4b-9d32-897baa160d7a</v>
       </c>
       <c r="C84" s="5" t="str">
-        <v>Gorgeous Fresh Pants</v>
+        <v>Sleek Fresh Bike</v>
       </c>
       <c r="D84" s="5" t="str">
-        <v>0.6.4</v>
+        <v>7.1.6</v>
       </c>
       <c r="E84" s="5" t="str">
-        <v>October</v>
+        <v>April</v>
       </c>
       <c r="F84" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G84" s="5">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85" ht="30" customHeight="1">
       <c r="A85" s="4" t="str">
-        <v>9c6891f1-9610-44f7-b181-352928efc6a3</v>
+        <v>3ccd702e-c2b5-46ed-a4e3-ace1fded4b1d</v>
       </c>
       <c r="B85" s="5" t="str">
-        <v>222c03e7-4063-4a4a-a0de-c17435bb9397</v>
+        <v>2ff351b7-2814-4ad0-b296-8b4b11c33886</v>
       </c>
       <c r="C85" s="5" t="str">
-        <v>Small Soft Table</v>
+        <v>Bespoke Plastic Pants</v>
       </c>
       <c r="D85" s="5" t="str">
-        <v>7.6.1</v>
+        <v>1.0.0</v>
       </c>
       <c r="E85" s="5" t="str">
-        <v>September</v>
+        <v>January</v>
       </c>
       <c r="F85" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G85" s="5">
-        <v>75</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" ht="30" customHeight="1">
       <c r="A86" s="4" t="str">
-        <v>b7d8b712-c1e3-4021-b08f-f77238c76dc5</v>
+        <v>bbc19718-3b0d-434d-8b80-836f8fe2325e</v>
       </c>
       <c r="B86" s="5" t="str">
-        <v>f9ad247c-d335-48b6-833c-724f91ad887d</v>
+        <v>3e238c28-a249-4f0f-91a3-f3279e38f5e3</v>
       </c>
       <c r="C86" s="5" t="str">
-        <v>Unbranded Wooden Keyboard</v>
+        <v>Incredible Bronze Chicken</v>
       </c>
       <c r="D86" s="5" t="str">
-        <v>4.7.5</v>
+        <v>7.0.9</v>
       </c>
       <c r="E86" s="5" t="str">
-        <v>December</v>
+        <v>June</v>
       </c>
       <c r="F86" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G86" s="5">
-        <v>68</v>
+        <v>24</v>
       </c>
     </row>
     <row r="87" ht="30" customHeight="1">
       <c r="A87" s="4" t="str">
-        <v>fb1b0efc-4571-467e-af6f-04423fa532e2</v>
+        <v>df5ea204-5869-4eb1-910d-68dc6961e49d</v>
       </c>
       <c r="B87" s="5" t="str">
-        <v>eb5bc999-9594-4a71-a564-948b171b2aca</v>
+        <v>241029fd-775f-4bf4-943a-641eb3f37e4d</v>
       </c>
       <c r="C87" s="5" t="str">
-        <v>Incredible Wooden Ball</v>
+        <v>Intelligent Bronze Mouse</v>
       </c>
       <c r="D87" s="5" t="str">
-        <v>9.1.7</v>
+        <v>0.3.4</v>
       </c>
       <c r="E87" s="5" t="str">
-        <v>January</v>
+        <v>November</v>
       </c>
       <c r="F87" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G87" s="5">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="88" ht="30" customHeight="1">
       <c r="A88" s="4" t="str">
-        <v>fc94902e-9a93-4c4c-924b-b4abe6531919</v>
+        <v>09d90f59-0261-4c17-aac8-9fa7f3e3ba88</v>
       </c>
       <c r="B88" s="5" t="str">
-        <v>be92b4d8-75c9-4b9d-b7db-3eb0e4a4a260</v>
+        <v>27e2f468-32ca-4ce3-b92d-446e21f3a4cd</v>
       </c>
       <c r="C88" s="5" t="str">
-        <v>Rustic Rubber Computer</v>
+        <v>Generic Bronze Chips</v>
       </c>
       <c r="D88" s="5" t="str">
-        <v>5.1.3</v>
+        <v>0.2.9</v>
       </c>
       <c r="E88" s="5" t="str">
-        <v>November</v>
+        <v>May</v>
       </c>
       <c r="F88" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G88" s="5">
-        <v>90</v>
+        <v>15</v>
       </c>
     </row>
     <row r="89" ht="30" customHeight="1">
       <c r="A89" s="4" t="str">
-        <v>13485624-49b4-43e6-bbb8-f7d19f4504ac</v>
+        <v>ed29f3bf-fce0-421b-ae6d-77eb84ad5ebc</v>
       </c>
       <c r="B89" s="5" t="str">
-        <v>960a526e-c3f4-4266-9f8c-3883e0eaaf78</v>
+        <v>01c501c2-1df1-44bd-b34b-cc1ae564752a</v>
       </c>
       <c r="C89" s="5" t="str">
-        <v>Luxurious Cotton Tuna</v>
+        <v>Fantastic Fresh Hat</v>
       </c>
       <c r="D89" s="5" t="str">
-        <v>4.9.1</v>
+        <v>6.1.5</v>
       </c>
       <c r="E89" s="5" t="str">
-        <v>March</v>
+        <v>August</v>
       </c>
       <c r="F89" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G89" s="5">
-        <v>97</v>
+        <v>51</v>
       </c>
     </row>
     <row r="90" ht="30" customHeight="1">
       <c r="A90" s="4" t="str">
-        <v>fa4060f5-1a3b-4640-96b3-c3b8355e63b2</v>
+        <v>4d41434c-c195-401c-a9df-f35570ccb099</v>
       </c>
       <c r="B90" s="5" t="str">
-        <v>244640a2-be6c-4f2b-a19a-383b5aef9752</v>
+        <v>b54eb8f4-61e7-4368-a70d-4bb99f5185cf</v>
       </c>
       <c r="C90" s="5" t="str">
-        <v>Tasty Cotton Sausages</v>
+        <v>Tasty Frozen Mouse</v>
       </c>
       <c r="D90" s="5" t="str">
-        <v>8.5.9</v>
+        <v>5.0.2</v>
       </c>
       <c r="E90" s="5" t="str">
-        <v>November</v>
+        <v>January</v>
       </c>
       <c r="F90" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G90" s="5">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="91" ht="30" customHeight="1">
       <c r="A91" s="4" t="str">
-        <v>40e2d70f-abf4-4884-b247-7e0ebaccd793</v>
+        <v>ff542297-7399-4a0c-b7ad-c215766f3780</v>
       </c>
       <c r="B91" s="5" t="str">
-        <v>be338f38-10ae-4c10-bc0a-4560bb6150d0</v>
+        <v>f056ab12-0d74-4bbd-ac3d-8c0756b90bc2</v>
       </c>
       <c r="C91" s="5" t="str">
-        <v>Elegant Granite Table</v>
+        <v>Incredible Plastic Cheese</v>
       </c>
       <c r="D91" s="5" t="str">
-        <v>4.2.2</v>
+        <v>1.0.4</v>
       </c>
       <c r="E91" s="5" t="str">
-        <v>May</v>
+        <v>January</v>
       </c>
       <c r="F91" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G91" s="5">
-        <v>22</v>
+        <v>45</v>
       </c>
     </row>
     <row r="92" ht="30" customHeight="1">
       <c r="A92" s="4" t="str">
-        <v>d1a9c12b-edd8-43c6-91db-a2620ca711af</v>
+        <v>70efc27a-bd47-41a1-af00-5e4faa91f3cf</v>
       </c>
       <c r="B92" s="5" t="str">
-        <v>903c3283-8e4d-413b-8251-6e070b756aa6</v>
+        <v>27a94e79-f87f-4f4c-9978-dcef70678c60</v>
       </c>
       <c r="C92" s="5" t="str">
-        <v>Awesome Plastic Computer</v>
+        <v>Generic Plastic Salad</v>
       </c>
       <c r="D92" s="5" t="str">
-        <v>3.1.4</v>
+        <v>6.2.5</v>
       </c>
       <c r="E92" s="5" t="str">
-        <v>April</v>
+        <v>November</v>
       </c>
       <c r="F92" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G92" s="5">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="93" ht="30" customHeight="1">
       <c r="A93" s="4" t="str">
-        <v>5cc2e9f7-7a52-4081-be54-bd189865c750</v>
+        <v>410d38b2-af72-446a-b76c-8c0e7f3f7fed</v>
       </c>
       <c r="B93" s="5" t="str">
-        <v>324ff42c-b071-40a8-8bbc-19ed7eb3036f</v>
+        <v>495c0145-2c15-41c0-a739-ec84cbfc66ae</v>
       </c>
       <c r="C93" s="5" t="str">
-        <v>Rustic Granite Table</v>
+        <v>Intelligent Frozen Mouse</v>
       </c>
       <c r="D93" s="5" t="str">
-        <v>6.1.9</v>
+        <v>1.8.6</v>
       </c>
       <c r="E93" s="5" t="str">
-        <v>January</v>
+        <v>March</v>
       </c>
       <c r="F93" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G93" s="5">
-        <v>96</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" ht="30" customHeight="1">
       <c r="A94" s="4" t="str">
-        <v>d773aa80-1089-41ed-8eba-b65dce86c72e</v>
+        <v>124a2e3b-b001-440e-bd2e-0ffdb8fa0d31</v>
       </c>
       <c r="B94" s="5" t="str">
-        <v>ad8a82ce-ac7b-4925-8f7c-d87276798301</v>
+        <v>9f600a36-ab40-45da-94d3-7eb3ce50711c</v>
       </c>
       <c r="C94" s="5" t="str">
-        <v>Fantastic Bronze Pants</v>
+        <v>Practical Granite Ball</v>
       </c>
       <c r="D94" s="5" t="str">
-        <v>1.7.8</v>
+        <v>6.5.4</v>
       </c>
       <c r="E94" s="5" t="str">
-        <v>July</v>
+        <v>June</v>
       </c>
       <c r="F94" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G94" s="5">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="95" ht="30" customHeight="1">
       <c r="A95" s="4" t="str">
-        <v>ad206f96-0609-47d1-b0a9-ba26b55fd66a</v>
+        <v>aaf7d193-a010-4eea-a8c3-88fd90aae8e3</v>
       </c>
       <c r="B95" s="5" t="str">
-        <v>1fb376ae-bd31-4aba-b918-af440f26dd83</v>
+        <v>6717c7d0-a843-48e7-81f7-616bc20ecd5f</v>
       </c>
       <c r="C95" s="5" t="str">
-        <v>Licensed Rubber Chicken</v>
+        <v>Ergonomic Granite Soap</v>
       </c>
       <c r="D95" s="5" t="str">
-        <v>8.9.5</v>
+        <v>5.0.7</v>
       </c>
       <c r="E95" s="5" t="str">
-        <v>September</v>
+        <v>July</v>
       </c>
       <c r="F95" s="5" t="str">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G95" s="5">
-        <v>76</v>
+        <v>25</v>
       </c>
     </row>
     <row r="96" ht="30" customHeight="1">
       <c r="A96" s="4" t="str">
-        <v>2b39be18-a1a5-46fa-9c8c-f21f13f523eb</v>
+        <v>70840b2d-0f92-4de8-b0b1-f8880fbce40e</v>
       </c>
       <c r="B96" s="5" t="str">
-        <v>30aeafdb-657b-4aa1-98d7-aa9ec18e30df</v>
+        <v>8874ea54-927a-46ff-8f04-49f03b8e03e2</v>
       </c>
       <c r="C96" s="5" t="str">
-        <v>Incredible Frozen Chicken</v>
+        <v>Electronic Wooden Hat</v>
       </c>
       <c r="D96" s="5" t="str">
-        <v>7.9.4</v>
+        <v>5.7.1</v>
       </c>
       <c r="E96" s="5" t="str">
-        <v>April</v>
+        <v>August</v>
       </c>
       <c r="F96" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G96" s="5">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="97" ht="30" customHeight="1">
       <c r="A97" s="4" t="str">
-        <v>ebb9f168-3a81-4ae8-b8eb-ddba7ef53bb8</v>
+        <v>d0f13232-57cf-42af-a791-d0fbe2b453fe</v>
       </c>
       <c r="B97" s="5" t="str">
-        <v>20aabdc2-628c-4142-a2e9-88d53bef6a2f</v>
+        <v>7f852f98-5c98-4852-a9f0-de0a81de322b</v>
       </c>
       <c r="C97" s="5" t="str">
-        <v>Modern Fresh Gloves</v>
+        <v>Recycled Plastic Fish</v>
       </c>
       <c r="D97" s="5" t="str">
-        <v>2.4.6</v>
+        <v>0.2.4</v>
       </c>
       <c r="E97" s="5" t="str">
-        <v>January</v>
+        <v>March</v>
       </c>
       <c r="F97" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G97" s="5">
-        <v>44</v>
+        <v>76</v>
       </c>
     </row>
     <row r="98" ht="30" customHeight="1">
       <c r="A98" s="4" t="str">
-        <v>e4e0bc62-c4ed-4fdb-8b31-3e6e0ac94001</v>
+        <v>f253429c-7b46-4f4b-95d4-ef2b2f0a1f14</v>
       </c>
       <c r="B98" s="5" t="str">
-        <v>80108ebf-ff64-4c53-bdfc-1279cffe4343</v>
+        <v>349bc9dd-d5c5-406b-a7c4-91d0b835e015</v>
       </c>
       <c r="C98" s="5" t="str">
-        <v>Generic Concrete Chair</v>
+        <v>Bespoke Cotton Shoes</v>
       </c>
       <c r="D98" s="5" t="str">
-        <v>8.4.7</v>
+        <v>7.8.1</v>
       </c>
       <c r="E98" s="5" t="str">
-        <v>December</v>
+        <v>November</v>
       </c>
       <c r="F98" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G98" s="5">
-        <v>50</v>
+        <v>65</v>
       </c>
     </row>
     <row r="99" ht="30" customHeight="1">
       <c r="A99" s="4" t="str">
-        <v>be5247f4-79ee-476c-aded-0c15fbfee671</v>
+        <v>8dd600dc-0560-43d9-af9d-1c919f6d99f6</v>
       </c>
       <c r="B99" s="5" t="str">
-        <v>d0a4d0a2-a304-450a-aee1-8bde0c4d7d95</v>
+        <v>c8fc214b-eb25-48d2-8c68-fe16bd2d0d25</v>
       </c>
       <c r="C99" s="5" t="str">
-        <v>Handmade Metal Pizza</v>
+        <v>Handcrafted Fresh Towels</v>
       </c>
       <c r="D99" s="5" t="str">
-        <v>9.3.9</v>
+        <v>9.8.1</v>
       </c>
       <c r="E99" s="5" t="str">
-        <v>November</v>
+        <v>April</v>
       </c>
       <c r="F99" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G99" s="5">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="100" ht="30" customHeight="1">
       <c r="A100" s="4" t="str">
-        <v>7e32749a-5aec-4203-85d4-5c17a9641441</v>
+        <v>29ef72f9-e729-40d8-ac15-18f9b54bc90e</v>
       </c>
       <c r="B100" s="5" t="str">
-        <v>e67774ab-4b7e-4f72-963a-253132e5dd60</v>
+        <v>4d5da15c-3e1e-43ea-91ba-f2072094b3f0</v>
       </c>
       <c r="C100" s="5" t="str">
-        <v>Fantastic Wooden Shirt</v>
+        <v>Ergonomic Cotton Computer</v>
       </c>
       <c r="D100" s="5" t="str">
-        <v>3.7.7</v>
+        <v>2.0.4</v>
       </c>
       <c r="E100" s="5" t="str">
-        <v>February</v>
+        <v>May</v>
       </c>
       <c r="F100" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G100" s="5">
-        <v>37</v>
+        <v>90</v>
       </c>
     </row>
     <row r="101" ht="30" customHeight="1">
       <c r="A101" s="4" t="str">
-        <v>4da1b7c1-cd54-4a1b-b12d-b912ef26cef2</v>
+        <v>c9dd9064-398e-4824-b47b-4e77358300b7</v>
       </c>
       <c r="B101" s="5" t="str">
-        <v>106a9b6f-53c3-4abb-9298-7ebf4c0214ed</v>
+        <v>f7602fc1-e3cd-4a9e-98cc-eee2ee9bea4f</v>
       </c>
       <c r="C101" s="5" t="str">
-        <v>Licensed Granite Shirt</v>
+        <v>Awesome Plastic Pizza</v>
       </c>
       <c r="D101" s="5" t="str">
-        <v>1.6.3</v>
+        <v>8.0.1</v>
       </c>
       <c r="E101" s="5" t="str">
-        <v>December</v>
+        <v>September</v>
       </c>
       <c r="F101" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G101" s="5">
-        <v>76</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: remove json-as-xlsx & full manual workbook generation
</commit_message>
<xml_diff>
--- a/consumption.xlsx
+++ b/consumption.xlsx
@@ -518,85 +518,85 @@
     </row>
     <row r="2" ht="30" customHeight="1">
       <c r="A2" s="4" t="str">
-        <v>4613ac17-9ff8-444a-84bc-fd6266f1fd27</v>
+        <v>34b33bd0-6003-413f-a53a-043aad39d380</v>
       </c>
       <c r="B2" s="5" t="str">
-        <v>87a0ae47-5c6d-4bca-9fc5-5ad099373c8f</v>
+        <v>4e215bf3-d610-427c-974f-dcd1f8efbf2d</v>
       </c>
       <c r="C2" s="5" t="str">
-        <v>Licensed Plastic Computer</v>
+        <v>Gorgeous Soft Car</v>
       </c>
       <c r="D2" s="5" t="str">
-        <v>3.7.1</v>
+        <v>9.7.7</v>
       </c>
       <c r="E2" s="5" t="str">
-        <v>July</v>
+        <v>May</v>
       </c>
       <c r="F2" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G2" s="5">
-        <v>80</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" ht="30" customHeight="1">
       <c r="A3" s="4" t="str">
-        <v>b756d4bc-e5a7-4c85-8e05-c9c948dc655a</v>
+        <v>e112ebfa-87df-4a01-8f6d-77ca41f98206</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>612a55b8-cd6e-42c8-a9d4-207ac7170ab1</v>
+        <v>7a264f3e-95de-4d84-a2af-b88a19c20ac1</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>Practical Fresh Sausages</v>
+        <v>Elegant Steel Pants</v>
       </c>
       <c r="D3" s="5" t="str">
-        <v>1.0.7</v>
+        <v>4.4.3</v>
       </c>
       <c r="E3" s="5" t="str">
-        <v>December</v>
+        <v>October</v>
       </c>
       <c r="F3" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G3" s="5">
-        <v>82</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" ht="30" customHeight="1">
       <c r="A4" s="4" t="str">
-        <v>9f02d59a-f199-491f-8625-bb3bafe868f3</v>
+        <v>25a3fefd-46e4-438d-9616-680b9cb9112e</v>
       </c>
       <c r="B4" s="5" t="str">
-        <v>9331d5d2-e45e-4bce-9e56-b824ccfd2c7a</v>
+        <v>523f98b0-88e0-4f72-b8ba-75200b23fd37</v>
       </c>
       <c r="C4" s="5" t="str">
-        <v>Handmade Concrete Table</v>
+        <v>Refined Granite Soap</v>
       </c>
       <c r="D4" s="5" t="str">
-        <v>4.0.0</v>
+        <v>4.6.1</v>
       </c>
       <c r="E4" s="5" t="str">
-        <v>September</v>
+        <v>December</v>
       </c>
       <c r="F4" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G4" s="5">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" ht="30" customHeight="1">
       <c r="A5" s="4" t="str">
-        <v>b857659d-d027-459f-befa-6b522568f9ca</v>
+        <v>4ec38995-aa08-44bc-8950-dd8d4abd01fe</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>844da8fc-4676-4f5c-ba25-db67a5159c42</v>
+        <v>2fa9a101-0ff9-4bab-ae98-c8698cc4f67c</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>Small Rubber Chips</v>
+        <v>Rustic Metal Pizza</v>
       </c>
       <c r="D5" s="5" t="str">
-        <v>4.2.7</v>
+        <v>6.1.9</v>
       </c>
       <c r="E5" s="5" t="str">
         <v>March</v>
@@ -605,21 +605,21 @@
         <v>2023</v>
       </c>
       <c r="G5" s="5">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" ht="30" customHeight="1">
       <c r="A6" s="4" t="str">
-        <v>982daf32-755c-4657-8580-7d2102675c3e</v>
+        <v>72f5b294-94b7-43e9-8307-893552d18ebe</v>
       </c>
       <c r="B6" s="5" t="str">
-        <v>5d4c8629-c32b-475b-805a-0347d7dfbd37</v>
+        <v>c18250b2-43be-4e06-a803-a6506277c53f</v>
       </c>
       <c r="C6" s="5" t="str">
-        <v>Small Bronze Chips</v>
+        <v>Modern Steel Bike</v>
       </c>
       <c r="D6" s="5" t="str">
-        <v>2.2.9</v>
+        <v>1.2.6</v>
       </c>
       <c r="E6" s="5" t="str">
         <v>February</v>
@@ -628,21 +628,21 @@
         <v>2023</v>
       </c>
       <c r="G6" s="5">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" ht="30" customHeight="1">
       <c r="A7" s="4" t="str">
-        <v>477ba9c1-92bf-4916-a55a-ebf8ce0cb369</v>
+        <v>0ff4845a-ddb1-46dc-9d4c-277ddaa96f32</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>2f4aff62-f4d3-438c-a483-0165f0cc006d</v>
+        <v>40570070-1421-4526-aa96-1631ec5ef164</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>Fantastic Plastic Soap</v>
+        <v>Oriental Bronze Keyboard</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>0.4.1</v>
+        <v>0.1.3</v>
       </c>
       <c r="E7" s="5" t="str">
         <v>January</v>
@@ -651,320 +651,320 @@
         <v>2023</v>
       </c>
       <c r="G7" s="5">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" ht="30" customHeight="1">
       <c r="A8" s="4" t="str">
-        <v>7e7e59ec-e9db-4437-a3b9-8e0844a4155f</v>
+        <v>cb2978fd-e371-486e-b435-550465065e5e</v>
       </c>
       <c r="B8" s="5" t="str">
-        <v>3ceff741-0e15-4723-ab53-374715545318</v>
+        <v>ff7f7ce9-9a0c-466d-b367-0da96c4f76ad</v>
       </c>
       <c r="C8" s="5" t="str">
-        <v>Incredible Bronze Towels</v>
+        <v>Oriental Granite Pizza</v>
       </c>
       <c r="D8" s="5" t="str">
-        <v>6.5.2</v>
+        <v>6.0.1</v>
       </c>
       <c r="E8" s="5" t="str">
-        <v>June</v>
+        <v>October</v>
       </c>
       <c r="F8" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G8" s="5">
-        <v>71</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" ht="30" customHeight="1">
       <c r="A9" s="4" t="str">
-        <v>ac20943f-e535-4bff-970d-0533e641f63f</v>
+        <v>eb9cef16-7eec-4845-bf17-04c12309a8bc</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>132d8ddd-9fc4-4598-b470-de94da418f80</v>
+        <v>071457ed-66c7-445e-99c8-3c21f1586b5b</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>Generic Bronze Car</v>
+        <v>Practical Concrete Shirt</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>5.6.2</v>
+        <v>9.9.5</v>
       </c>
       <c r="E9" s="5" t="str">
-        <v>August</v>
+        <v>October</v>
       </c>
       <c r="F9" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G9" s="5">
-        <v>59</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" ht="30" customHeight="1">
       <c r="A10" s="4" t="str">
-        <v>7eb4db9d-4adc-4e94-884b-16b634d08bfa</v>
+        <v>5581307a-d670-42ed-a1df-0ffb6bd83be4</v>
       </c>
       <c r="B10" s="5" t="str">
-        <v>c1e50f29-e941-4ab1-8cbb-0ba4a45a8c8c</v>
+        <v>fec831fc-7432-4ad1-90fe-e7c47fad2af0</v>
       </c>
       <c r="C10" s="5" t="str">
-        <v>Rustic Soft Mouse</v>
+        <v>Licensed Fresh Cheese</v>
       </c>
       <c r="D10" s="5" t="str">
-        <v>9.0.7</v>
+        <v>4.9.0</v>
       </c>
       <c r="E10" s="5" t="str">
-        <v>February</v>
+        <v>March</v>
       </c>
       <c r="F10" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G10" s="5">
-        <v>53</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" ht="30" customHeight="1">
       <c r="A11" s="4" t="str">
-        <v>cecd6da0-99b5-46e5-9983-ec1309d1c3ff</v>
+        <v>c29c7f7f-42aa-43dc-ac49-fc02b16c11b7</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>dad80883-9909-479c-8e72-d5462c092a2e</v>
+        <v>9b292b93-97fc-47fd-81c1-7e7cb965804e</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>Small Wooden Ball</v>
+        <v>Handmade Fresh Computer</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v>5.5.0</v>
+        <v>0.1.7</v>
       </c>
       <c r="E11" s="5" t="str">
-        <v>October</v>
+        <v>February</v>
       </c>
       <c r="F11" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G11" s="5">
-        <v>74</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" ht="30" customHeight="1">
       <c r="A12" s="4" t="str">
-        <v>3d8120c0-980d-4361-8e85-547639f9cd4b</v>
+        <v>28c59347-e2d5-4b12-9f98-353d4d0ea374</v>
       </c>
       <c r="B12" s="5" t="str">
-        <v>c887573c-79e7-41ae-9765-4e6a29fd377b</v>
+        <v>c33c5fca-9cb9-498f-9626-4e07d180132b</v>
       </c>
       <c r="C12" s="5" t="str">
-        <v>Luxurious Steel Car</v>
+        <v>Handmade Cotton Computer</v>
       </c>
       <c r="D12" s="5" t="str">
-        <v>6.8.3</v>
+        <v>1.4.3</v>
       </c>
       <c r="E12" s="5" t="str">
-        <v>October</v>
+        <v>August</v>
       </c>
       <c r="F12" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G12" s="5">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" ht="30" customHeight="1">
       <c r="A13" s="4" t="str">
-        <v>a462d786-d915-4857-bc8a-ebcfc8972151</v>
+        <v>ae71347b-acde-42e2-b3da-7791b336726b</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>a80d8975-3899-48a3-b9d3-352193eb381f</v>
+        <v>e93de6fa-d8bb-4855-99d5-f5363294d82d</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>Small Plastic Gloves</v>
+        <v>Electronic Fresh Bacon</v>
       </c>
       <c r="D13" s="5" t="str">
-        <v>8.3.0</v>
+        <v>4.3.6</v>
       </c>
       <c r="E13" s="5" t="str">
-        <v>July</v>
+        <v>June</v>
       </c>
       <c r="F13" s="5" t="str">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G13" s="5">
-        <v>5</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" ht="30" customHeight="1">
       <c r="A14" s="4" t="str">
-        <v>8b91e5e6-10bc-44ee-b498-cf9041e320ee</v>
+        <v>6ff168bc-aeea-44dd-a435-8ae383af60fd</v>
       </c>
       <c r="B14" s="5" t="str">
-        <v>bc1231f0-59a6-4815-af25-a2aa8ec939ad</v>
+        <v>2c4bee3b-0936-4786-8c19-4e131ec260da</v>
       </c>
       <c r="C14" s="5" t="str">
-        <v>Small Bronze Salad</v>
+        <v>Practical Rubber Shoes</v>
       </c>
       <c r="D14" s="5" t="str">
-        <v>7.0.0</v>
+        <v>6.5.5</v>
       </c>
       <c r="E14" s="5" t="str">
-        <v>August</v>
+        <v>January</v>
       </c>
       <c r="F14" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G14" s="5">
-        <v>71</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" ht="30" customHeight="1">
       <c r="A15" s="4" t="str">
-        <v>08b972f4-a417-42ab-a00d-ce19f064c00c</v>
+        <v>6c88d20a-9490-4dd3-bf8b-32dd343dd431</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>5c00f071-0f42-4a68-98ff-890d90adc405</v>
+        <v>4dc4c10a-1289-4a12-bedc-9e9e84b0982f</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>Incredible Steel Shirt</v>
+        <v>Fantastic Steel Car</v>
       </c>
       <c r="D15" s="5" t="str">
-        <v>8.6.9</v>
+        <v>5.5.9</v>
       </c>
       <c r="E15" s="5" t="str">
-        <v>July</v>
+        <v>September</v>
       </c>
       <c r="F15" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G15" s="5">
-        <v>85</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" ht="30" customHeight="1">
       <c r="A16" s="4" t="str">
-        <v>07d4bb9b-5fbb-4efd-8fbe-fd5cd29aeb55</v>
+        <v>d2fbd898-aefa-4008-8a7a-ac37be6d8437</v>
       </c>
       <c r="B16" s="5" t="str">
-        <v>55c4f630-f69a-4fe0-b52f-6d60d914e315</v>
+        <v>0c6f56de-6e12-4cd2-889d-4a5cbaa2d695</v>
       </c>
       <c r="C16" s="5" t="str">
-        <v>Awesome Cotton Cheese</v>
+        <v>Gorgeous Plastic Salad</v>
       </c>
       <c r="D16" s="5" t="str">
-        <v>6.2.8</v>
+        <v>1.6.1</v>
       </c>
       <c r="E16" s="5" t="str">
-        <v>August</v>
+        <v>September</v>
       </c>
       <c r="F16" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G16" s="5">
-        <v>22</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" ht="30" customHeight="1">
       <c r="A17" s="4" t="str">
-        <v>b302a143-bd18-4932-b35c-cb6322418d45</v>
+        <v>5c2aa069-5635-493d-a800-9957c0aff3a6</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>111c6d64-72a3-475b-b871-7362a70d7078</v>
+        <v>3f912776-cf19-406d-9ca5-671b49a5555b</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>Awesome Fresh Chair</v>
+        <v>Bespoke Bronze Sausages</v>
       </c>
       <c r="D17" s="5" t="str">
-        <v>0.9.7</v>
+        <v>0.1.5</v>
       </c>
       <c r="E17" s="5" t="str">
-        <v>November</v>
+        <v>August</v>
       </c>
       <c r="F17" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G17" s="5">
-        <v>37</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" ht="30" customHeight="1">
       <c r="A18" s="4" t="str">
-        <v>60c10d00-de7d-48bf-9985-0ce0faed0693</v>
+        <v>be74075c-d583-4ccc-b31f-a3083c63efcb</v>
       </c>
       <c r="B18" s="5" t="str">
-        <v>efd588bc-3791-4b5a-a4b6-1f951b66cf5d</v>
+        <v>adb41fcb-940e-4c5f-bef8-5d8a4c40c2fd</v>
       </c>
       <c r="C18" s="5" t="str">
-        <v>Sleek Rubber Bacon</v>
+        <v>Recycled Rubber Salad</v>
       </c>
       <c r="D18" s="5" t="str">
-        <v>9.9.0</v>
+        <v>0.4.8</v>
       </c>
       <c r="E18" s="5" t="str">
-        <v>August</v>
+        <v>November</v>
       </c>
       <c r="F18" s="5" t="str">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G18" s="5">
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" ht="30" customHeight="1">
       <c r="A19" s="4" t="str">
-        <v>b1521c6d-09c3-447c-bdb1-bfeae5006797</v>
+        <v>1131efe5-be45-4a1c-9a52-b4457d6dd675</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>ff224f8b-cce0-49e1-bc0d-5d1878bdb678</v>
+        <v>757d06d3-50f4-4273-aaf6-b00e9d3c1e79</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v>Intelligent Plastic Cheese</v>
+        <v>Handmade Granite Bike</v>
       </c>
       <c r="D19" s="5" t="str">
-        <v>4.2.7</v>
+        <v>7.5.7</v>
       </c>
       <c r="E19" s="5" t="str">
-        <v>June</v>
+        <v>August</v>
       </c>
       <c r="F19" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G19" s="5">
-        <v>60</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" ht="30" customHeight="1">
       <c r="A20" s="4" t="str">
-        <v>72c01f58-a4af-4f03-b9a5-41fbdb0d5af5</v>
+        <v>3a59bb9a-339c-40c6-8418-8c53b13a810f</v>
       </c>
       <c r="B20" s="5" t="str">
-        <v>73439b8e-1ec6-4841-8661-1b8b04e7d296</v>
+        <v>0bc084ae-28fb-45e6-9897-38cd1b316e9e</v>
       </c>
       <c r="C20" s="5" t="str">
-        <v>Luxurious Bronze Shoes</v>
+        <v>Handcrafted Rubber Mouse</v>
       </c>
       <c r="D20" s="5" t="str">
-        <v>5.3.1</v>
+        <v>2.7.4</v>
       </c>
       <c r="E20" s="5" t="str">
-        <v>August</v>
+        <v>September</v>
       </c>
       <c r="F20" s="5" t="str">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G20" s="5">
-        <v>72</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" ht="30" customHeight="1">
       <c r="A21" s="4" t="str">
-        <v>937a79d3-6e32-43d7-b592-3ebcfb088317</v>
+        <v>7afa5630-4587-4614-8baf-cdbd75fe17d0</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>11accd79-ed95-4858-855d-b0ff596b7657</v>
+        <v>06e56272-9940-4845-afa5-71ee203c668e</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v>Handcrafted Wooden Cheese</v>
+        <v>Intelligent Metal Fish</v>
       </c>
       <c r="D21" s="5" t="str">
-        <v>7.8.8</v>
+        <v>6.9.2</v>
       </c>
       <c r="E21" s="5" t="str">
         <v>May</v>
@@ -973,21 +973,21 @@
         <v>2023</v>
       </c>
       <c r="G21" s="5">
-        <v>85</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" ht="30" customHeight="1">
       <c r="A22" s="4" t="str">
-        <v>ef7f8545-a45f-4c3e-a7b1-cb312c07fe61</v>
+        <v>167fa290-744a-4188-a5e0-716ad8a11703</v>
       </c>
       <c r="B22" s="5" t="str">
-        <v>35687b17-4cee-41fe-9fc6-d90ce6c6e833</v>
+        <v>a6381e49-372d-444f-85f0-638b3fa7dd52</v>
       </c>
       <c r="C22" s="5" t="str">
-        <v>Handcrafted Rubber Gloves</v>
+        <v>Tasty Bronze Bacon</v>
       </c>
       <c r="D22" s="5" t="str">
-        <v>2.7.8</v>
+        <v>0.8.6</v>
       </c>
       <c r="E22" s="5" t="str">
         <v>May</v>
@@ -996,90 +996,90 @@
         <v>2023</v>
       </c>
       <c r="G22" s="5">
-        <v>41</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" ht="30" customHeight="1">
       <c r="A23" s="4" t="str">
-        <v>c783863a-7ff4-47f8-940d-d0f409009d04</v>
+        <v>2559dbd8-d0f7-4a0b-94c7-dda2e2283d0f</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>f688b3a4-473d-4e1b-b8b6-98f4bd6946e1</v>
+        <v>55f48857-6a4a-45fc-a29c-00a985101882</v>
       </c>
       <c r="C23" s="5" t="str">
-        <v>Recycled Bronze Chicken</v>
+        <v>Practical Steel Cheese</v>
       </c>
       <c r="D23" s="5" t="str">
-        <v>4.4.8</v>
+        <v>7.9.1</v>
       </c>
       <c r="E23" s="5" t="str">
-        <v>September</v>
+        <v>December</v>
       </c>
       <c r="F23" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G23" s="5">
-        <v>78</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" ht="30" customHeight="1">
       <c r="A24" s="4" t="str">
-        <v>30cd03fa-a779-48d0-b532-c90fe83acdff</v>
+        <v>35c090eb-20d2-4ec1-816a-539976f22947</v>
       </c>
       <c r="B24" s="5" t="str">
-        <v>ff4e04c5-9d4d-45f2-8ce5-e9f2867bbfe0</v>
+        <v>9cf12718-6889-4ba1-9de0-b9731c12cef4</v>
       </c>
       <c r="C24" s="5" t="str">
-        <v>Elegant Plastic Salad</v>
+        <v>Generic Granite Bike</v>
       </c>
       <c r="D24" s="5" t="str">
-        <v>2.4.8</v>
+        <v>7.5.8</v>
       </c>
       <c r="E24" s="5" t="str">
-        <v>September</v>
+        <v>June</v>
       </c>
       <c r="F24" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G24" s="5">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" ht="30" customHeight="1">
       <c r="A25" s="4" t="str">
-        <v>659430ec-7ff2-4e48-9036-eb4bbd190d95</v>
+        <v>f9828696-cd23-4f5e-9b78-ce8b9c37de16</v>
       </c>
       <c r="B25" s="5" t="str">
-        <v>6961cfde-77b8-4a16-9477-b9eb6bd98c80</v>
+        <v>1e0f81f3-0c88-40dc-a06d-8908a78d5c57</v>
       </c>
       <c r="C25" s="5" t="str">
-        <v>Oriental Fresh Hat</v>
+        <v>Small Metal Towels</v>
       </c>
       <c r="D25" s="5" t="str">
-        <v>2.1.0</v>
+        <v>2.4.9</v>
       </c>
       <c r="E25" s="5" t="str">
-        <v>August</v>
+        <v>May</v>
       </c>
       <c r="F25" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G25" s="5">
-        <v>69</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" ht="30" customHeight="1">
       <c r="A26" s="4" t="str">
-        <v>b9ceccaa-0bba-49c7-9dcc-6c4c30f45bb6</v>
+        <v>49bc5864-0e4c-4953-abb0-d44cba8a1a98</v>
       </c>
       <c r="B26" s="5" t="str">
-        <v>38ccc966-4c45-4faf-9c87-ac33be50ba05</v>
+        <v>c4335ea1-9d7c-4676-9db1-21da052a2e39</v>
       </c>
       <c r="C26" s="5" t="str">
-        <v>Tasty Rubber Tuna</v>
+        <v>Luxurious Bronze Sausages</v>
       </c>
       <c r="D26" s="5" t="str">
-        <v>1.3.9</v>
+        <v>2.8.4</v>
       </c>
       <c r="E26" s="5" t="str">
         <v>November</v>
@@ -1088,21 +1088,21 @@
         <v>2023</v>
       </c>
       <c r="G26" s="5">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" ht="30" customHeight="1">
       <c r="A27" s="4" t="str">
-        <v>dc7300b8-7009-42a1-b19f-e52f75fa4db2</v>
+        <v>f8e12a06-a0d3-4953-8f37-2f55bb56e5b0</v>
       </c>
       <c r="B27" s="5" t="str">
-        <v>f08c65ae-3557-4141-bee0-6cf104da7ba9</v>
+        <v>0d312693-49e0-46d7-8cb9-f3511c1bdbea</v>
       </c>
       <c r="C27" s="5" t="str">
-        <v>Sleek Plastic Shoes</v>
+        <v>Gorgeous Granite Towels</v>
       </c>
       <c r="D27" s="5" t="str">
-        <v>4.4.7</v>
+        <v>1.9.8</v>
       </c>
       <c r="E27" s="5" t="str">
         <v>March</v>
@@ -1111,113 +1111,113 @@
         <v>2023</v>
       </c>
       <c r="G27" s="5">
-        <v>59</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" ht="30" customHeight="1">
       <c r="A28" s="4" t="str">
-        <v>c255c2c2-14cb-45b9-a9b5-2c8781ac95a4</v>
+        <v>6d11a3f9-5b52-427b-a43d-68c4129091d3</v>
       </c>
       <c r="B28" s="5" t="str">
-        <v>97639545-0d6b-4336-9f01-878642bd95ff</v>
+        <v>999f24d1-af76-483d-8e98-691108512506</v>
       </c>
       <c r="C28" s="5" t="str">
-        <v>Small Concrete Chicken</v>
+        <v>Bespoke Plastic Shirt</v>
       </c>
       <c r="D28" s="5" t="str">
-        <v>9.0.3</v>
+        <v>5.5.0</v>
       </c>
       <c r="E28" s="5" t="str">
-        <v>December</v>
+        <v>June</v>
       </c>
       <c r="F28" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G28" s="5">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" ht="30" customHeight="1">
       <c r="A29" s="4" t="str">
-        <v>d98f4314-1eb0-4b75-8e53-e358b327cdac</v>
+        <v>e281f38d-25f4-4eeb-ab1f-995d02c7c8fb</v>
       </c>
       <c r="B29" s="5" t="str">
-        <v>dec2e37d-1438-4b1b-9fd7-28ba3d5656f6</v>
+        <v>5ab1d532-d374-4047-a39f-89afdd0e4818</v>
       </c>
       <c r="C29" s="5" t="str">
-        <v>Small Wooden Shoes</v>
+        <v>Luxurious Rubber Pizza</v>
       </c>
       <c r="D29" s="5" t="str">
-        <v>7.0.2</v>
+        <v>2.9.1</v>
       </c>
       <c r="E29" s="5" t="str">
-        <v>January</v>
+        <v>October</v>
       </c>
       <c r="F29" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G29" s="5">
-        <v>90</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" ht="30" customHeight="1">
       <c r="A30" s="4" t="str">
-        <v>3e4866ad-89ee-4681-b7e9-adde6dcf0c17</v>
+        <v>037c0a8b-f377-49c0-8d4a-1ee995f8b448</v>
       </c>
       <c r="B30" s="5" t="str">
-        <v>7776f8c6-afca-4330-bf1f-378385ede03b</v>
+        <v>016da422-4f2e-4240-a8a7-c2fa1d4aef15</v>
       </c>
       <c r="C30" s="5" t="str">
-        <v>Handmade Steel Bike</v>
+        <v>Handmade Plastic Shirt</v>
       </c>
       <c r="D30" s="5" t="str">
-        <v>6.6.7</v>
+        <v>9.2.0</v>
       </c>
       <c r="E30" s="5" t="str">
-        <v>May</v>
+        <v>November</v>
       </c>
       <c r="F30" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G30" s="5">
-        <v>71</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" ht="30" customHeight="1">
       <c r="A31" s="4" t="str">
-        <v>62d85c84-3151-4556-880b-b02d64cb2034</v>
+        <v>5c9c3be6-7336-4da4-a129-6444bc30b4e5</v>
       </c>
       <c r="B31" s="5" t="str">
-        <v>877a530f-98fb-4659-9184-a76ca3f8aea7</v>
+        <v>989de251-6edf-4f0e-9ffc-117915bf58af</v>
       </c>
       <c r="C31" s="5" t="str">
-        <v>Sleek Wooden Cheese</v>
+        <v>Refined Bronze Ball</v>
       </c>
       <c r="D31" s="5" t="str">
-        <v>7.3.3</v>
+        <v>8.8.9</v>
       </c>
       <c r="E31" s="5" t="str">
-        <v>April</v>
+        <v>March</v>
       </c>
       <c r="F31" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G31" s="5">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" ht="30" customHeight="1">
       <c r="A32" s="4" t="str">
-        <v>23dc5f3f-6ebf-450a-84c1-684fd22121ce</v>
+        <v>0c05175f-294e-402e-9813-ce56ac61f67e</v>
       </c>
       <c r="B32" s="5" t="str">
-        <v>95436008-f23c-41f2-9563-c6c56d3d4026</v>
+        <v>9b5349db-4613-45c9-bf27-39f7b45265f3</v>
       </c>
       <c r="C32" s="5" t="str">
-        <v>Electronic Wooden Chair</v>
+        <v>Modern Metal Sausages</v>
       </c>
       <c r="D32" s="5" t="str">
-        <v>7.0.4</v>
+        <v>7.2.9</v>
       </c>
       <c r="E32" s="5" t="str">
         <v>August</v>
@@ -1226,205 +1226,205 @@
         <v>2023</v>
       </c>
       <c r="G32" s="5">
-        <v>28</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" ht="30" customHeight="1">
       <c r="A33" s="4" t="str">
-        <v>c98e85a3-df4d-4372-ae55-7081bb85d791</v>
+        <v>ffde588b-0a81-408b-8fe3-23f2855be680</v>
       </c>
       <c r="B33" s="5" t="str">
-        <v>3fca8e29-e98e-4f26-994c-44bde577703a</v>
+        <v>8fcb25da-442f-456a-b722-b8b855a904ee</v>
       </c>
       <c r="C33" s="5" t="str">
-        <v>Luxurious Fresh Pants</v>
+        <v>Incredible Concrete Bike</v>
       </c>
       <c r="D33" s="5" t="str">
-        <v>8.5.8</v>
+        <v>2.4.6</v>
       </c>
       <c r="E33" s="5" t="str">
-        <v>December</v>
+        <v>July</v>
       </c>
       <c r="F33" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G33" s="5">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" ht="30" customHeight="1">
       <c r="A34" s="4" t="str">
-        <v>4920558f-0350-48c6-adb2-979b751cf7dc</v>
+        <v>e63e8c57-e16b-48bb-8b0a-71dc8dd1fc30</v>
       </c>
       <c r="B34" s="5" t="str">
-        <v>a68dea5d-9c83-44d9-85e7-afa3870e6707</v>
+        <v>de9fcafb-530f-4e6e-bd15-3663a304455a</v>
       </c>
       <c r="C34" s="5" t="str">
-        <v>Generic Concrete Towels</v>
+        <v>Small Metal Computer</v>
       </c>
       <c r="D34" s="5" t="str">
-        <v>7.1.3</v>
+        <v>9.8.6</v>
       </c>
       <c r="E34" s="5" t="str">
-        <v>February</v>
+        <v>May</v>
       </c>
       <c r="F34" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G34" s="5">
-        <v>31</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" ht="30" customHeight="1">
       <c r="A35" s="4" t="str">
-        <v>7a19da62-cbdc-4915-8144-cfe6f32dce1a</v>
+        <v>6c344a35-10a6-4f4f-806f-981cfaf2248c</v>
       </c>
       <c r="B35" s="5" t="str">
-        <v>f2e84adf-7583-4cfb-b32e-626bc8e1016b</v>
+        <v>0c2c35f4-5936-4562-a8f2-65d595803a45</v>
       </c>
       <c r="C35" s="5" t="str">
-        <v>Intelligent Wooden Hat</v>
+        <v>Elegant Steel Sausages</v>
       </c>
       <c r="D35" s="5" t="str">
-        <v>9.1.2</v>
+        <v>3.0.9</v>
       </c>
       <c r="E35" s="5" t="str">
-        <v>April</v>
+        <v>January</v>
       </c>
       <c r="F35" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G35" s="5">
-        <v>86</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" ht="30" customHeight="1">
       <c r="A36" s="4" t="str">
-        <v>67f31117-f12f-402c-91d7-bd097918e362</v>
+        <v>56ec406d-57aa-4e9c-9fd6-90a2092654be</v>
       </c>
       <c r="B36" s="5" t="str">
-        <v>c5d3505d-44eb-47c1-9734-60f152d4ca5d</v>
+        <v>7584fee8-19cd-49bc-9235-9b177b12c320</v>
       </c>
       <c r="C36" s="5" t="str">
-        <v>Refined Rubber Salad</v>
+        <v>Tasty Cotton Computer</v>
       </c>
       <c r="D36" s="5" t="str">
-        <v>0.3.8</v>
+        <v>5.5.2</v>
       </c>
       <c r="E36" s="5" t="str">
-        <v>September</v>
+        <v>June</v>
       </c>
       <c r="F36" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G36" s="5">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" ht="30" customHeight="1">
       <c r="A37" s="4" t="str">
-        <v>50f2d2a9-b943-41d0-819a-303edea09667</v>
+        <v>b7a9a005-702a-4227-a9cc-a581cd65bbd5</v>
       </c>
       <c r="B37" s="5" t="str">
-        <v>843aa254-0c90-47cf-acf7-60ec166c4300</v>
+        <v>8421c4af-04ca-46f6-9e06-ffb508f1e217</v>
       </c>
       <c r="C37" s="5" t="str">
-        <v>Bespoke Cotton Ball</v>
+        <v>Oriental Fresh Bike</v>
       </c>
       <c r="D37" s="5" t="str">
-        <v>1.2.0</v>
+        <v>7.8.3</v>
       </c>
       <c r="E37" s="5" t="str">
-        <v>June</v>
+        <v>September</v>
       </c>
       <c r="F37" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G37" s="5">
-        <v>27</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" ht="30" customHeight="1">
       <c r="A38" s="4" t="str">
-        <v>406c5bf5-b53c-4eeb-a845-e1e2aa0350d4</v>
+        <v>c0f0a8ce-86c1-4a6e-a5c9-08e1d49270c0</v>
       </c>
       <c r="B38" s="5" t="str">
-        <v>511e0ee8-2f6c-490b-ab28-972604eea8d3</v>
+        <v>e1154320-3b8f-4752-8b7d-342a935096d7</v>
       </c>
       <c r="C38" s="5" t="str">
-        <v>Elegant Steel Car</v>
+        <v>Sleek Metal Chips</v>
       </c>
       <c r="D38" s="5" t="str">
-        <v>5.3.5</v>
+        <v>4.5.4</v>
       </c>
       <c r="E38" s="5" t="str">
-        <v>November</v>
+        <v>April</v>
       </c>
       <c r="F38" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G38" s="5">
-        <v>19</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" ht="30" customHeight="1">
       <c r="A39" s="4" t="str">
-        <v>369be0da-3d55-41ea-9dd3-f4cae7994f3a</v>
+        <v>9a9125a9-b9ea-4c55-9beb-3bb80beaefbe</v>
       </c>
       <c r="B39" s="5" t="str">
-        <v>5717b994-666e-425e-a980-d0d5d42e27c4</v>
+        <v>90c978b7-8def-4884-ba47-5e1ebd5cb9b3</v>
       </c>
       <c r="C39" s="5" t="str">
-        <v>Recycled Soft Soap</v>
+        <v>Electronic Soft Pizza</v>
       </c>
       <c r="D39" s="5" t="str">
-        <v>2.2.1</v>
+        <v>1.6.2</v>
       </c>
       <c r="E39" s="5" t="str">
-        <v>March</v>
+        <v>December</v>
       </c>
       <c r="F39" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G39" s="5">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" ht="30" customHeight="1">
       <c r="A40" s="4" t="str">
-        <v>cacfca81-e258-4670-a9dd-752317682079</v>
+        <v>88dc4f8a-c84c-4db1-89f9-9ae306341773</v>
       </c>
       <c r="B40" s="5" t="str">
-        <v>6794ff77-4f8b-4844-b873-e4a265f89d40</v>
+        <v>1d5c424e-37f1-493c-a386-68c8bc1c749c</v>
       </c>
       <c r="C40" s="5" t="str">
-        <v>Awesome Bronze Towels</v>
+        <v>Oriental Metal Tuna</v>
       </c>
       <c r="D40" s="5" t="str">
-        <v>5.7.5</v>
+        <v>0.1.3</v>
       </c>
       <c r="E40" s="5" t="str">
-        <v>March</v>
+        <v>July</v>
       </c>
       <c r="F40" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G40" s="5">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" ht="30" customHeight="1">
       <c r="A41" s="4" t="str">
-        <v>a22d9d82-134c-4ebc-a197-bb17895b814e</v>
+        <v>1c822b7c-1c9c-4f72-98be-568d9b6ddc5d</v>
       </c>
       <c r="B41" s="5" t="str">
-        <v>26a2c745-050c-4bb3-be8f-a5a1dbbef7c7</v>
+        <v>0f5ccc99-cc3d-41e5-ab6a-07e5033081eb</v>
       </c>
       <c r="C41" s="5" t="str">
-        <v>Handmade Granite Soap</v>
+        <v>Practical Fresh Bike</v>
       </c>
       <c r="D41" s="5" t="str">
-        <v>3.2.9</v>
+        <v>8.3.8</v>
       </c>
       <c r="E41" s="5" t="str">
         <v>March</v>
@@ -1433,44 +1433,44 @@
         <v>2023</v>
       </c>
       <c r="G41" s="5">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" ht="30" customHeight="1">
       <c r="A42" s="4" t="str">
-        <v>c6b2cc75-029e-473a-9ef7-98aec10fb449</v>
+        <v>6c26f6f9-04c6-4a5b-8725-6bc663ba0add</v>
       </c>
       <c r="B42" s="5" t="str">
-        <v>d0420817-8f3e-4e23-88f6-57bfce5a927a</v>
+        <v>4cba5149-a8f0-4daf-bef9-0f03e303862e</v>
       </c>
       <c r="C42" s="5" t="str">
-        <v>Bespoke Plastic Salad</v>
+        <v>Luxurious Plastic Soap</v>
       </c>
       <c r="D42" s="5" t="str">
-        <v>1.0.1</v>
+        <v>3.0.7</v>
       </c>
       <c r="E42" s="5" t="str">
-        <v>May</v>
+        <v>August</v>
       </c>
       <c r="F42" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G42" s="5">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" ht="30" customHeight="1">
       <c r="A43" s="4" t="str">
-        <v>1b093ff3-171a-419d-9a0a-344cc23c84c4</v>
+        <v>19ba57a6-d927-45f1-94ce-92517fd7c24a</v>
       </c>
       <c r="B43" s="5" t="str">
-        <v>1266aaf9-e7b0-44be-b870-a237d5822bf1</v>
+        <v>81eaa5a5-3b6b-4af4-8056-f3c409f97cba</v>
       </c>
       <c r="C43" s="5" t="str">
-        <v>Oriental Frozen Bike</v>
+        <v>Oriental Rubber Tuna</v>
       </c>
       <c r="D43" s="5" t="str">
-        <v>7.4.1</v>
+        <v>9.9.8</v>
       </c>
       <c r="E43" s="5" t="str">
         <v>January</v>
@@ -1479,44 +1479,44 @@
         <v>2022</v>
       </c>
       <c r="G43" s="5">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" ht="30" customHeight="1">
       <c r="A44" s="4" t="str">
-        <v>39187941-7952-4c70-b93c-5cd90a1e48f8</v>
+        <v>b1dc217d-9fb0-430a-bc73-10a1d74875f6</v>
       </c>
       <c r="B44" s="5" t="str">
-        <v>016340e5-e550-4fc0-b8d1-235f0ef4eb57</v>
+        <v>05419c7f-549d-46ec-97c6-262559d176c2</v>
       </c>
       <c r="C44" s="5" t="str">
-        <v>Electronic Fresh Gloves</v>
+        <v>Electronic Concrete Shoes</v>
       </c>
       <c r="D44" s="5" t="str">
-        <v>0.2.7</v>
+        <v>1.7.2</v>
       </c>
       <c r="E44" s="5" t="str">
-        <v>October</v>
+        <v>August</v>
       </c>
       <c r="F44" s="5" t="str">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G44" s="5">
-        <v>8</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" ht="30" customHeight="1">
       <c r="A45" s="4" t="str">
-        <v>76849dc0-465f-4760-99cd-d99593b71959</v>
+        <v>98d27ade-9e82-4b45-85f9-0ca974079689</v>
       </c>
       <c r="B45" s="5" t="str">
-        <v>7a37a6ab-240b-4e9e-b433-90b7767c042d</v>
+        <v>a2b519a6-d987-4808-809c-b626a10df912</v>
       </c>
       <c r="C45" s="5" t="str">
-        <v>Unbranded Bronze Shirt</v>
+        <v>Bespoke Metal Cheese</v>
       </c>
       <c r="D45" s="5" t="str">
-        <v>7.3.8</v>
+        <v>7.5.6</v>
       </c>
       <c r="E45" s="5" t="str">
         <v>September</v>
@@ -1525,90 +1525,90 @@
         <v>2023</v>
       </c>
       <c r="G45" s="5">
-        <v>91</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" ht="30" customHeight="1">
       <c r="A46" s="4" t="str">
-        <v>6a9d96cd-7d48-40f7-a12c-0a41c06a56f8</v>
+        <v>dbf0f602-985b-431a-ae66-aa8d6f2d4db8</v>
       </c>
       <c r="B46" s="5" t="str">
-        <v>b7fb2a56-e386-44a5-add5-4353959ff849</v>
+        <v>ae519698-9aae-402d-b628-215659fafacf</v>
       </c>
       <c r="C46" s="5" t="str">
-        <v>Ergonomic Cotton Shirt</v>
+        <v>Generic Soft Car</v>
       </c>
       <c r="D46" s="5" t="str">
-        <v>9.5.3</v>
+        <v>4.1.0</v>
       </c>
       <c r="E46" s="5" t="str">
-        <v>March</v>
+        <v>July</v>
       </c>
       <c r="F46" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G46" s="5">
-        <v>14</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" ht="30" customHeight="1">
       <c r="A47" s="4" t="str">
-        <v>930f32e9-5718-4b7c-921b-bb0b24d8a3fc</v>
+        <v>61f71966-6402-491a-874a-8fac1db1ed79</v>
       </c>
       <c r="B47" s="5" t="str">
-        <v>68f1b627-1082-441a-948a-c0a2d824585b</v>
+        <v>c9a4d400-47de-4e58-99c9-c9b763622aeb</v>
       </c>
       <c r="C47" s="5" t="str">
-        <v>Incredible Metal Bike</v>
+        <v>Practical Rubber Salad</v>
       </c>
       <c r="D47" s="5" t="str">
-        <v>5.4.6</v>
+        <v>0.4.5</v>
       </c>
       <c r="E47" s="5" t="str">
-        <v>December</v>
+        <v>May</v>
       </c>
       <c r="F47" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G47" s="5">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" ht="30" customHeight="1">
       <c r="A48" s="4" t="str">
-        <v>1fa4e04e-1d71-4357-bb0d-42d9aa7655ab</v>
+        <v>09afe4e3-8883-45a4-b78d-b3db39feff1a</v>
       </c>
       <c r="B48" s="5" t="str">
-        <v>072f5b25-41a4-42f6-9051-7848e049d26f</v>
+        <v>2aaaa256-09d3-46b4-9062-0bbb09ddc4a5</v>
       </c>
       <c r="C48" s="5" t="str">
-        <v>Recycled Cotton Ball</v>
+        <v>Fantastic Concrete Pizza</v>
       </c>
       <c r="D48" s="5" t="str">
-        <v>5.7.9</v>
+        <v>7.7.8</v>
       </c>
       <c r="E48" s="5" t="str">
-        <v>October</v>
+        <v>January</v>
       </c>
       <c r="F48" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G48" s="5">
-        <v>2</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" ht="30" customHeight="1">
       <c r="A49" s="4" t="str">
-        <v>79b744fa-bd01-4f96-bcd5-bbc6dd6f47b9</v>
+        <v>35f96c5d-d7fe-4ec0-8447-4f1d46b53d38</v>
       </c>
       <c r="B49" s="5" t="str">
-        <v>3e86445f-62de-4c06-9cb4-f15ebe2bd829</v>
+        <v>686bfc2b-cdaa-420b-8084-f23ec893e771</v>
       </c>
       <c r="C49" s="5" t="str">
-        <v>Unbranded Fresh Computer</v>
+        <v>Intelligent Bronze Chicken</v>
       </c>
       <c r="D49" s="5" t="str">
-        <v>2.7.1</v>
+        <v>2.1.8</v>
       </c>
       <c r="E49" s="5" t="str">
         <v>January</v>
@@ -1617,320 +1617,320 @@
         <v>2023</v>
       </c>
       <c r="G49" s="5">
-        <v>66</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" ht="30" customHeight="1">
       <c r="A50" s="4" t="str">
-        <v>e61fdf2c-0aa5-4151-89ea-44f4a86a6879</v>
+        <v>2e569080-9b77-4d6d-9ca3-89f5e15d0948</v>
       </c>
       <c r="B50" s="5" t="str">
-        <v>3fe2f8d1-bb42-40d7-b857-5c11e75d6bf7</v>
+        <v>2adf7e4b-4caf-49c8-8e1b-1c89030f8d33</v>
       </c>
       <c r="C50" s="5" t="str">
-        <v>Tasty Fresh Chicken</v>
+        <v>Awesome Metal Chips</v>
       </c>
       <c r="D50" s="5" t="str">
-        <v>8.2.9</v>
+        <v>7.6.2</v>
       </c>
       <c r="E50" s="5" t="str">
-        <v>April</v>
+        <v>March</v>
       </c>
       <c r="F50" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G50" s="5">
-        <v>70</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" ht="30" customHeight="1">
       <c r="A51" s="4" t="str">
-        <v>57a98edd-bdf8-42ad-8bb5-97f6a0aec04a</v>
+        <v>37834f13-c251-4125-89bb-850aa0361876</v>
       </c>
       <c r="B51" s="5" t="str">
-        <v>badc56be-b539-4268-a5f6-f5ed7afae14a</v>
+        <v>beb09d2a-3be2-4b9c-a182-99a39d2fa3d2</v>
       </c>
       <c r="C51" s="5" t="str">
-        <v>Practical Fresh Bacon</v>
+        <v>Awesome Cotton Computer</v>
       </c>
       <c r="D51" s="5" t="str">
-        <v>0.9.7</v>
+        <v>6.6.7</v>
       </c>
       <c r="E51" s="5" t="str">
-        <v>October</v>
+        <v>January</v>
       </c>
       <c r="F51" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G51" s="5">
-        <v>65</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" ht="30" customHeight="1">
       <c r="A52" s="4" t="str">
-        <v>39c46bbe-b5d2-4f0f-9928-1d3e3a6b4cba</v>
+        <v>29759d05-e094-4f4a-ae2f-8940eefc8073</v>
       </c>
       <c r="B52" s="5" t="str">
-        <v>0755067d-75db-408f-8808-835e4d3af651</v>
+        <v>2ea152ea-33ef-4347-ae70-4a37d11fe47a</v>
       </c>
       <c r="C52" s="5" t="str">
-        <v>Incredible Rubber Tuna</v>
+        <v>Bespoke Metal Sausages</v>
       </c>
       <c r="D52" s="5" t="str">
-        <v>2.2.9</v>
+        <v>3.9.6</v>
       </c>
       <c r="E52" s="5" t="str">
-        <v>December</v>
+        <v>April</v>
       </c>
       <c r="F52" s="5" t="str">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G52" s="5">
-        <v>65</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" ht="30" customHeight="1">
       <c r="A53" s="4" t="str">
-        <v>0b5aebe9-1ab2-44e7-80da-ca81d1d823d8</v>
+        <v>a349e2da-d3c5-4d30-adde-2187af23eb79</v>
       </c>
       <c r="B53" s="5" t="str">
-        <v>56985ac1-93ed-4ee8-b31f-1dcca3d58405</v>
+        <v>11434bc3-8398-45c7-9dc7-6c2fecfb21d6</v>
       </c>
       <c r="C53" s="5" t="str">
-        <v>Rustic Steel Bike</v>
+        <v>Ergonomic Wooden Mouse</v>
       </c>
       <c r="D53" s="5" t="str">
-        <v>1.8.0</v>
+        <v>1.7.3</v>
       </c>
       <c r="E53" s="5" t="str">
-        <v>March</v>
+        <v>June</v>
       </c>
       <c r="F53" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G53" s="5">
-        <v>72</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" ht="30" customHeight="1">
       <c r="A54" s="4" t="str">
-        <v>057bd020-9d8b-4447-9da0-8effb09ab224</v>
+        <v>3dca88bf-e8ef-4cbe-a626-f4494b4a584a</v>
       </c>
       <c r="B54" s="5" t="str">
-        <v>7a5afab9-8449-4be9-827e-2d4acba7270d</v>
+        <v>0f93af90-850b-4981-a2ba-4368f6c4f016</v>
       </c>
       <c r="C54" s="5" t="str">
-        <v>Handcrafted Rubber Tuna</v>
+        <v>Small Steel Towels</v>
       </c>
       <c r="D54" s="5" t="str">
-        <v>0.4.5</v>
+        <v>8.4.4</v>
       </c>
       <c r="E54" s="5" t="str">
-        <v>November</v>
+        <v>September</v>
       </c>
       <c r="F54" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G54" s="5">
-        <v>74</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55" ht="30" customHeight="1">
       <c r="A55" s="4" t="str">
-        <v>a2d26164-2932-4023-9725-11d6fc564359</v>
+        <v>3fadf0bb-a7d3-428e-995c-93b7de845c1e</v>
       </c>
       <c r="B55" s="5" t="str">
-        <v>1c83b68f-6ca9-416e-8842-7f3cdcdff49f</v>
+        <v>bb6aec98-f2a5-4bc4-b8b8-fce68dfec17c</v>
       </c>
       <c r="C55" s="5" t="str">
-        <v>Unbranded Cotton Fish</v>
+        <v>Oriental Plastic Gloves</v>
       </c>
       <c r="D55" s="5" t="str">
-        <v>4.3.2</v>
+        <v>0.7.3</v>
       </c>
       <c r="E55" s="5" t="str">
-        <v>November</v>
+        <v>September</v>
       </c>
       <c r="F55" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G55" s="5">
-        <v>83</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" ht="30" customHeight="1">
       <c r="A56" s="4" t="str">
-        <v>dcc75fde-fa16-4154-9271-08e7f69b0ef0</v>
+        <v>1b89bd1e-aed0-496a-b846-009494461d41</v>
       </c>
       <c r="B56" s="5" t="str">
-        <v>1508d3d5-c80e-40b3-ade7-f5ec8230a264</v>
+        <v>8c3eb2e8-683c-4adc-96ef-ae49e56d1173</v>
       </c>
       <c r="C56" s="5" t="str">
-        <v>Oriental Plastic Computer</v>
+        <v>Luxurious Wooden Car</v>
       </c>
       <c r="D56" s="5" t="str">
-        <v>7.9.5</v>
+        <v>5.5.1</v>
       </c>
       <c r="E56" s="5" t="str">
-        <v>January</v>
+        <v>March</v>
       </c>
       <c r="F56" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G56" s="5">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" ht="30" customHeight="1">
       <c r="A57" s="4" t="str">
-        <v>87858788-8d61-47f0-82d2-b89c522f600b</v>
+        <v>59c8ae71-6ff0-4ed6-a0c4-42334852670a</v>
       </c>
       <c r="B57" s="5" t="str">
-        <v>b08a9d00-0964-45cc-9d68-961d477960de</v>
+        <v>35c9a3d3-ac88-4cc0-a046-25477c6556db</v>
       </c>
       <c r="C57" s="5" t="str">
-        <v>Refined Plastic Tuna</v>
+        <v>Small Frozen Pizza</v>
       </c>
       <c r="D57" s="5" t="str">
-        <v>3.5.7</v>
+        <v>1.1.3</v>
       </c>
       <c r="E57" s="5" t="str">
-        <v>April</v>
+        <v>December</v>
       </c>
       <c r="F57" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G57" s="5">
-        <v>57</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" ht="30" customHeight="1">
       <c r="A58" s="4" t="str">
-        <v>9f643228-a6c1-4595-acaf-a655b9e9c23f</v>
+        <v>6f6e0e1d-b33b-48a9-ad9c-bbbe3ec1b0f0</v>
       </c>
       <c r="B58" s="5" t="str">
-        <v>66c45cc0-2327-429e-b57d-bd938c6d2b31</v>
+        <v>99b569d5-ffae-4b36-82af-e3023197e618</v>
       </c>
       <c r="C58" s="5" t="str">
-        <v>Intelligent Plastic Salad</v>
+        <v>Generic Steel Bike</v>
       </c>
       <c r="D58" s="5" t="str">
-        <v>9.5.5</v>
+        <v>9.4.4</v>
       </c>
       <c r="E58" s="5" t="str">
-        <v>July</v>
+        <v>June</v>
       </c>
       <c r="F58" s="5" t="str">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G58" s="5">
-        <v>22</v>
+        <v>45</v>
       </c>
     </row>
     <row r="59" ht="30" customHeight="1">
       <c r="A59" s="4" t="str">
-        <v>f4740773-9207-464a-bdeb-5a46213a0d5d</v>
+        <v>eb29d20c-c743-4d80-b359-02e63ee24ec5</v>
       </c>
       <c r="B59" s="5" t="str">
-        <v>a09552a9-1c9c-43ce-a080-4103d16e7707</v>
+        <v>72dd7e6b-97b9-4140-8f37-a7bd238b7b9f</v>
       </c>
       <c r="C59" s="5" t="str">
-        <v>Practical Fresh Shirt</v>
+        <v>Refined Granite Pizza</v>
       </c>
       <c r="D59" s="5" t="str">
-        <v>1.7.5</v>
+        <v>1.1.3</v>
       </c>
       <c r="E59" s="5" t="str">
-        <v>March</v>
+        <v>October</v>
       </c>
       <c r="F59" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G59" s="5">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" ht="30" customHeight="1">
       <c r="A60" s="4" t="str">
-        <v>e97909bd-fc37-4bb0-ab8b-3c5a03c4d93d</v>
+        <v>ef590bb1-c383-4944-bb69-f33e127214b6</v>
       </c>
       <c r="B60" s="5" t="str">
-        <v>eb80715c-ed51-4c53-a0be-cda2e07b9a8f</v>
+        <v>05e1eda8-e6a8-40f2-ade4-3f28ac8df13f</v>
       </c>
       <c r="C60" s="5" t="str">
-        <v>Awesome Frozen Bike</v>
+        <v>Sleek Granite Table</v>
       </c>
       <c r="D60" s="5" t="str">
-        <v>2.7.9</v>
+        <v>8.1.9</v>
       </c>
       <c r="E60" s="5" t="str">
-        <v>December</v>
+        <v>November</v>
       </c>
       <c r="F60" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G60" s="5">
-        <v>90</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" ht="30" customHeight="1">
       <c r="A61" s="4" t="str">
-        <v>c3c7acd3-405b-4936-9128-c69b0b407ab1</v>
+        <v>df0383fb-cb4b-4afc-bc4b-b3c9f2d1d23f</v>
       </c>
       <c r="B61" s="5" t="str">
-        <v>56ab48d3-29ea-4b53-ac7e-5d8a9bdee47f</v>
+        <v>3c8791d0-903f-4227-8082-c03679b22579</v>
       </c>
       <c r="C61" s="5" t="str">
-        <v>Tasty Soft Sausages</v>
+        <v>Intelligent Fresh Soap</v>
       </c>
       <c r="D61" s="5" t="str">
-        <v>4.8.5</v>
+        <v>2.2.1</v>
       </c>
       <c r="E61" s="5" t="str">
-        <v>December</v>
+        <v>February</v>
       </c>
       <c r="F61" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G61" s="5">
-        <v>54</v>
+        <v>86</v>
       </c>
     </row>
     <row r="62" ht="30" customHeight="1">
       <c r="A62" s="4" t="str">
-        <v>97e03655-7d11-491c-9bca-b527c6a42ff5</v>
+        <v>53e2b822-2130-427a-bbf1-f9b375805a20</v>
       </c>
       <c r="B62" s="5" t="str">
-        <v>5a3e01fa-cc5b-4f03-bb4e-cd130ec3ee4b</v>
+        <v>a8f9932c-bc4f-4b07-93f4-0cbb22a42b09</v>
       </c>
       <c r="C62" s="5" t="str">
-        <v>Handcrafted Wooden Pants</v>
+        <v>Handcrafted Plastic Mouse</v>
       </c>
       <c r="D62" s="5" t="str">
-        <v>4.8.8</v>
+        <v>1.4.0</v>
       </c>
       <c r="E62" s="5" t="str">
-        <v>September</v>
+        <v>October</v>
       </c>
       <c r="F62" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G62" s="5">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="63" ht="30" customHeight="1">
       <c r="A63" s="4" t="str">
-        <v>1d53987d-35b2-4c8d-81ac-f2d69a139d16</v>
+        <v>b94b6240-206e-4389-8dd3-ac7053bad5ec</v>
       </c>
       <c r="B63" s="5" t="str">
-        <v>14a51ed7-e4d6-4590-b6f1-7bf95947c4e9</v>
+        <v>58972a4a-65f3-46b6-b849-18d6df3559a3</v>
       </c>
       <c r="C63" s="5" t="str">
-        <v>Incredible Concrete Ball</v>
+        <v>Elegant Rubber Keyboard</v>
       </c>
       <c r="D63" s="5" t="str">
-        <v>3.6.2</v>
+        <v>0.9.2</v>
       </c>
       <c r="E63" s="5" t="str">
         <v>October</v>
@@ -1939,228 +1939,228 @@
         <v>2023</v>
       </c>
       <c r="G63" s="5">
-        <v>84</v>
+        <v>57</v>
       </c>
     </row>
     <row r="64" ht="30" customHeight="1">
       <c r="A64" s="4" t="str">
-        <v>1aa78a37-4181-485c-9cd1-90cf6f4c85c1</v>
+        <v>939ae9ba-2c4b-41e9-90f4-17543898d46f</v>
       </c>
       <c r="B64" s="5" t="str">
-        <v>23ca0406-baf7-4335-9b0e-a12368b290a3</v>
+        <v>796189e5-de4d-40f2-9633-b36e49015e49</v>
       </c>
       <c r="C64" s="5" t="str">
-        <v>Licensed Cotton Shoes</v>
+        <v>Licensed Bronze Ball</v>
       </c>
       <c r="D64" s="5" t="str">
-        <v>8.6.3</v>
+        <v>9.1.2</v>
       </c>
       <c r="E64" s="5" t="str">
-        <v>February</v>
+        <v>April</v>
       </c>
       <c r="F64" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G64" s="5">
-        <v>80</v>
+        <v>46</v>
       </c>
     </row>
     <row r="65" ht="30" customHeight="1">
       <c r="A65" s="4" t="str">
-        <v>c2c9cbf7-122f-4bbd-be35-694a67ea2214</v>
+        <v>8bdf9b71-c09c-4814-b681-f0a3f2d89ea9</v>
       </c>
       <c r="B65" s="5" t="str">
-        <v>3ac4af47-92f5-4526-9fcd-8955e4d8bc70</v>
+        <v>4ac311dc-2721-46b4-96ee-6d36af38e5ae</v>
       </c>
       <c r="C65" s="5" t="str">
-        <v>Oriental Metal Pants</v>
+        <v>Tasty Soft Ball</v>
       </c>
       <c r="D65" s="5" t="str">
-        <v>9.6.4</v>
+        <v>8.6.7</v>
       </c>
       <c r="E65" s="5" t="str">
-        <v>January</v>
+        <v>September</v>
       </c>
       <c r="F65" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G65" s="5">
-        <v>94</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" ht="30" customHeight="1">
       <c r="A66" s="4" t="str">
-        <v>c8f2bdc8-940c-4133-80c9-41147a5e9539</v>
+        <v>89c3eb99-a0e1-4fad-b8de-78bb42d685ad</v>
       </c>
       <c r="B66" s="5" t="str">
-        <v>2b26f5d9-1456-4266-a8ab-3c813cdbf128</v>
+        <v>1b1fadfa-cbef-4525-bc9c-eccd7700e034</v>
       </c>
       <c r="C66" s="5" t="str">
-        <v>Recycled Plastic Car</v>
+        <v>Intelligent Granite Tuna</v>
       </c>
       <c r="D66" s="5" t="str">
-        <v>2.9.5</v>
+        <v>7.6.3</v>
       </c>
       <c r="E66" s="5" t="str">
-        <v>April</v>
+        <v>May</v>
       </c>
       <c r="F66" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G66" s="5">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="67" ht="30" customHeight="1">
       <c r="A67" s="4" t="str">
-        <v>7e311719-0ec1-4276-bab3-ef15cdb46069</v>
+        <v>2788ea4d-75db-4765-b360-bbd02f114710</v>
       </c>
       <c r="B67" s="5" t="str">
-        <v>75a95ab8-eee9-4932-bc35-13e45b917e39</v>
+        <v>13d8d73a-26ee-45b8-9364-12357a882271</v>
       </c>
       <c r="C67" s="5" t="str">
-        <v>Incredible Metal Bike</v>
+        <v>Rustic Cotton Pants</v>
       </c>
       <c r="D67" s="5" t="str">
-        <v>4.4.7</v>
+        <v>4.8.9</v>
       </c>
       <c r="E67" s="5" t="str">
         <v>October</v>
       </c>
       <c r="F67" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G67" s="5">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="68" ht="30" customHeight="1">
       <c r="A68" s="4" t="str">
-        <v>0162e2e6-f8db-4be3-b810-4c20f88d399b</v>
+        <v>c764a40c-9af4-40ba-8889-f21eb96828fd</v>
       </c>
       <c r="B68" s="5" t="str">
-        <v>7978f736-ad65-4166-9832-f44d157b4f14</v>
+        <v>9821d71e-554e-45cd-ae7a-f7b48aa2d75f</v>
       </c>
       <c r="C68" s="5" t="str">
-        <v>Rustic Bronze Hat</v>
+        <v>Elegant Rubber Mouse</v>
       </c>
       <c r="D68" s="5" t="str">
-        <v>7.0.7</v>
+        <v>3.1.5</v>
       </c>
       <c r="E68" s="5" t="str">
-        <v>March</v>
+        <v>February</v>
       </c>
       <c r="F68" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G68" s="5">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" ht="30" customHeight="1">
       <c r="A69" s="4" t="str">
-        <v>d59a0011-0475-47d7-9a43-0358b6510b67</v>
+        <v>c0d398e5-dc8b-487d-bb1e-295ef9edaac1</v>
       </c>
       <c r="B69" s="5" t="str">
-        <v>ccd99918-b6c3-479a-bcbc-bf36d624af89</v>
+        <v>8b3bb8b4-7387-4361-afba-2c2195cbb7df</v>
       </c>
       <c r="C69" s="5" t="str">
-        <v>Unbranded Granite Mouse</v>
+        <v>Electronic Granite Shirt</v>
       </c>
       <c r="D69" s="5" t="str">
-        <v>6.9.2</v>
+        <v>4.4.2</v>
       </c>
       <c r="E69" s="5" t="str">
-        <v>December</v>
+        <v>October</v>
       </c>
       <c r="F69" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G69" s="5">
-        <v>53</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70" ht="30" customHeight="1">
       <c r="A70" s="4" t="str">
-        <v>4a5ae1e6-b1a2-450f-9715-7219a85ec686</v>
+        <v>8daf9bbd-f9ce-4a71-ba2f-dd03993f6773</v>
       </c>
       <c r="B70" s="5" t="str">
-        <v>cb3a482d-bee6-4f1a-83c8-ea6ad4ef1bf5</v>
+        <v>4165ea30-81d4-4982-8dbb-5a9b0bfcf248</v>
       </c>
       <c r="C70" s="5" t="str">
-        <v>Recycled Concrete Car</v>
+        <v>Tasty Metal Mouse</v>
       </c>
       <c r="D70" s="5" t="str">
-        <v>2.4.8</v>
+        <v>2.8.4</v>
       </c>
       <c r="E70" s="5" t="str">
-        <v>November</v>
+        <v>May</v>
       </c>
       <c r="F70" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G70" s="5">
-        <v>27</v>
+        <v>79</v>
       </c>
     </row>
     <row r="71" ht="30" customHeight="1">
       <c r="A71" s="4" t="str">
-        <v>9bc58a44-a1c7-4d7f-a0cc-431923f9e437</v>
+        <v>1d46b417-6868-4a22-a134-b44a4b04d5f6</v>
       </c>
       <c r="B71" s="5" t="str">
-        <v>98a69bbf-8b28-44e1-85f6-f4918efa7830</v>
+        <v>ed65a046-1d2b-468c-b733-b467401f5adb</v>
       </c>
       <c r="C71" s="5" t="str">
-        <v>Modern Rubber Chips</v>
+        <v>Generic Wooden Bacon</v>
       </c>
       <c r="D71" s="5" t="str">
-        <v>7.5.7</v>
+        <v>4.9.3</v>
       </c>
       <c r="E71" s="5" t="str">
-        <v>November</v>
+        <v>April</v>
       </c>
       <c r="F71" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G71" s="5">
-        <v>26</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72" ht="30" customHeight="1">
       <c r="A72" s="4" t="str">
-        <v>c65b8a54-ee85-4b23-a2df-af9e7681a7df</v>
+        <v>4acdf8b3-a792-4a5c-85ff-4222cee08935</v>
       </c>
       <c r="B72" s="5" t="str">
-        <v>d09f45a0-f232-440d-99f7-ba385294d69a</v>
+        <v>da6e96f0-7bc1-4008-aece-0f4840e7a35c</v>
       </c>
       <c r="C72" s="5" t="str">
-        <v>Sleek Frozen Gloves</v>
+        <v>Elegant Rubber Computer</v>
       </c>
       <c r="D72" s="5" t="str">
-        <v>4.7.5</v>
+        <v>5.7.7</v>
       </c>
       <c r="E72" s="5" t="str">
-        <v>August</v>
+        <v>February</v>
       </c>
       <c r="F72" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G72" s="5">
-        <v>25</v>
+        <v>86</v>
       </c>
     </row>
     <row r="73" ht="30" customHeight="1">
       <c r="A73" s="4" t="str">
-        <v>e6ad3761-4dcf-4ed2-ad53-5f6aeed475b6</v>
+        <v>f2dfaea1-62c7-4bd8-a2cc-7b876cde476c</v>
       </c>
       <c r="B73" s="5" t="str">
-        <v>337f8395-a929-45f6-999c-5abe6008884d</v>
+        <v>95da880e-6d50-4344-805b-b1e59833455f</v>
       </c>
       <c r="C73" s="5" t="str">
-        <v>Ergonomic Cotton Shoes</v>
+        <v>Luxurious Soft Table</v>
       </c>
       <c r="D73" s="5" t="str">
-        <v>8.4.6</v>
+        <v>7.3.5</v>
       </c>
       <c r="E73" s="5" t="str">
         <v>April</v>
@@ -2169,231 +2169,231 @@
         <v>2023</v>
       </c>
       <c r="G73" s="5">
-        <v>73</v>
+        <v>45</v>
       </c>
     </row>
     <row r="74" ht="30" customHeight="1">
       <c r="A74" s="4" t="str">
-        <v>e0ace7f6-ff87-4865-a705-f06226f5aaa9</v>
+        <v>f7ea0c1c-d25e-4714-8015-a33981556c99</v>
       </c>
       <c r="B74" s="5" t="str">
-        <v>46891b4d-9f00-449e-9e9e-b20abf94a57e</v>
+        <v>5af758fe-754a-4b22-909c-f7010eecb265</v>
       </c>
       <c r="C74" s="5" t="str">
-        <v>Oriental Bronze Chips</v>
+        <v>Luxurious Rubber Soap</v>
       </c>
       <c r="D74" s="5" t="str">
-        <v>9.7.8</v>
+        <v>7.2.1</v>
       </c>
       <c r="E74" s="5" t="str">
-        <v>January</v>
+        <v>February</v>
       </c>
       <c r="F74" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G74" s="5">
-        <v>34</v>
+        <v>66</v>
       </c>
     </row>
     <row r="75" ht="30" customHeight="1">
       <c r="A75" s="4" t="str">
-        <v>ccf54998-037f-4618-8c79-e1e5d694458e</v>
+        <v>3f592bc3-93fc-4c03-bbfa-8de31af6a153</v>
       </c>
       <c r="B75" s="5" t="str">
-        <v>71ab73df-305b-481e-b0a0-4856e8f37c07</v>
+        <v>78b71bfb-bc5d-4e0f-ae93-d4661a4b35da</v>
       </c>
       <c r="C75" s="5" t="str">
-        <v>Elegant Concrete Gloves</v>
+        <v>Bespoke Cotton Keyboard</v>
       </c>
       <c r="D75" s="5" t="str">
-        <v>7.9.7</v>
+        <v>7.0.8</v>
       </c>
       <c r="E75" s="5" t="str">
-        <v>September</v>
+        <v>August</v>
       </c>
       <c r="F75" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G75" s="5">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" ht="30" customHeight="1">
       <c r="A76" s="4" t="str">
-        <v>a9f188b6-617c-4b5b-8a25-843ac29a71f5</v>
+        <v>5f8d5a59-5ed8-430e-b33b-4a29f8307767</v>
       </c>
       <c r="B76" s="5" t="str">
-        <v>e2bcdfbb-7bc1-43d4-86c3-40aa1685cb8f</v>
+        <v>98daa25e-8c70-4c33-ba0a-3cebcb9bb7ba</v>
       </c>
       <c r="C76" s="5" t="str">
-        <v>Ergonomic Bronze Bike</v>
+        <v>Incredible Frozen Table</v>
       </c>
       <c r="D76" s="5" t="str">
-        <v>8.2.6</v>
+        <v>7.8.5</v>
       </c>
       <c r="E76" s="5" t="str">
-        <v>July</v>
+        <v>February</v>
       </c>
       <c r="F76" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G76" s="5">
-        <v>52</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77" ht="30" customHeight="1">
       <c r="A77" s="4" t="str">
-        <v>c6fb2282-47dd-45e1-9b6a-ad8572b308e1</v>
+        <v>11c8b2a1-73ce-4238-9f41-84466b5cac29</v>
       </c>
       <c r="B77" s="5" t="str">
-        <v>38908d65-00a0-464e-8090-cf3bb91e7b91</v>
+        <v>adb28995-f1f7-43a7-ac8f-4acc6801da5b</v>
       </c>
       <c r="C77" s="5" t="str">
-        <v>Rustic Concrete Pants</v>
+        <v>Tasty Rubber Bacon</v>
       </c>
       <c r="D77" s="5" t="str">
-        <v>1.4.0</v>
+        <v>6.1.3</v>
       </c>
       <c r="E77" s="5" t="str">
-        <v>April</v>
+        <v>November</v>
       </c>
       <c r="F77" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G77" s="5">
-        <v>15</v>
+        <v>79</v>
       </c>
     </row>
     <row r="78" ht="30" customHeight="1">
       <c r="A78" s="4" t="str">
-        <v>1f681467-3c19-4924-b3d9-7b80f6ae2e77</v>
+        <v>528ad153-2c72-4e81-bbec-d21942ada254</v>
       </c>
       <c r="B78" s="5" t="str">
-        <v>c9240813-4947-4ab6-9b4b-81bcb0893fd3</v>
+        <v>423d3f1c-ba96-4454-99c2-79705c17d381</v>
       </c>
       <c r="C78" s="5" t="str">
-        <v>Bespoke Metal Car</v>
+        <v>Intelligent Steel Soap</v>
       </c>
       <c r="D78" s="5" t="str">
-        <v>0.3.0</v>
+        <v>3.5.2</v>
       </c>
       <c r="E78" s="5" t="str">
-        <v>October</v>
+        <v>July</v>
       </c>
       <c r="F78" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G78" s="5">
-        <v>48</v>
+        <v>67</v>
       </c>
     </row>
     <row r="79" ht="30" customHeight="1">
       <c r="A79" s="4" t="str">
-        <v>bebe33bc-a7fb-4819-88d1-46b87ba20968</v>
+        <v>343ec0dc-7a86-4f4f-9ebe-6dbb8633f460</v>
       </c>
       <c r="B79" s="5" t="str">
-        <v>03f980a7-ff54-4838-aa5a-4c2ad2eabd8e</v>
+        <v>af248e4e-aff5-475c-ba54-ba0f05a22ece</v>
       </c>
       <c r="C79" s="5" t="str">
-        <v>Elegant Wooden Bacon</v>
+        <v>Handcrafted Fresh Bacon</v>
       </c>
       <c r="D79" s="5" t="str">
-        <v>7.4.7</v>
+        <v>1.9.3</v>
       </c>
       <c r="E79" s="5" t="str">
-        <v>March</v>
+        <v>September</v>
       </c>
       <c r="F79" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G79" s="5">
-        <v>86</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80" ht="30" customHeight="1">
       <c r="A80" s="4" t="str">
-        <v>591b6e55-6f72-448a-acbf-081cedf0c5f6</v>
+        <v>948a8317-6c08-4015-bf47-8ae6029c4c06</v>
       </c>
       <c r="B80" s="5" t="str">
-        <v>96ba4cf9-37d6-4cf9-9dea-33ef114e07ad</v>
+        <v>575e6a42-eec7-4b50-bb09-58850867988f</v>
       </c>
       <c r="C80" s="5" t="str">
-        <v>Licensed Granite Soap</v>
+        <v>Modern Granite Soap</v>
       </c>
       <c r="D80" s="5" t="str">
-        <v>2.7.9</v>
+        <v>8.5.8</v>
       </c>
       <c r="E80" s="5" t="str">
-        <v>June</v>
+        <v>February</v>
       </c>
       <c r="F80" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G80" s="5">
-        <v>29</v>
+        <v>56</v>
       </c>
     </row>
     <row r="81" ht="30" customHeight="1">
       <c r="A81" s="4" t="str">
-        <v>2f3ab84b-e9bd-4624-b5e5-c54aa9ae03f4</v>
+        <v>2e9db7f9-1f12-4799-a0ce-d8b2462240e1</v>
       </c>
       <c r="B81" s="5" t="str">
-        <v>96831afd-bd51-4dc7-bf3c-040805af958f</v>
+        <v>a5d7de95-c492-4a81-84d3-4c95a42f2165</v>
       </c>
       <c r="C81" s="5" t="str">
-        <v>Fantastic Granite Shirt</v>
+        <v>Bespoke Bronze Towels</v>
       </c>
       <c r="D81" s="5" t="str">
-        <v>1.3.6</v>
+        <v>0.4.0</v>
       </c>
       <c r="E81" s="5" t="str">
-        <v>November</v>
+        <v>April</v>
       </c>
       <c r="F81" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G81" s="5">
-        <v>99</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82" ht="30" customHeight="1">
       <c r="A82" s="4" t="str">
-        <v>f1d0c06a-7a7b-476b-93fd-1509f0c754c8</v>
+        <v>b638f0ec-7bcc-4bbf-969c-9e7cd45a826f</v>
       </c>
       <c r="B82" s="5" t="str">
-        <v>89ead73b-c0ff-4556-a4c3-50dab723b047</v>
+        <v>52a1991d-8525-4453-9b0a-09957655cbf5</v>
       </c>
       <c r="C82" s="5" t="str">
-        <v>Refined Cotton Shoes</v>
+        <v>Small Cotton Bacon</v>
       </c>
       <c r="D82" s="5" t="str">
-        <v>9.0.5</v>
+        <v>9.0.1</v>
       </c>
       <c r="E82" s="5" t="str">
-        <v>June</v>
+        <v>March</v>
       </c>
       <c r="F82" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G82" s="5">
-        <v>99</v>
+        <v>55</v>
       </c>
     </row>
     <row r="83" ht="30" customHeight="1">
       <c r="A83" s="4" t="str">
-        <v>0e13b35b-4018-4dd5-ab9d-1c9a063ed018</v>
+        <v>aeaed1f9-b45f-4299-9a15-7f97b33a10ef</v>
       </c>
       <c r="B83" s="5" t="str">
-        <v>d9cb4300-c2ea-4c50-b1d5-2934fd5ab2b0</v>
+        <v>27386af5-bd5f-4571-863c-7c59486a266d</v>
       </c>
       <c r="C83" s="5" t="str">
-        <v>Licensed Cotton Cheese</v>
+        <v>Handcrafted Rubber Bacon</v>
       </c>
       <c r="D83" s="5" t="str">
-        <v>7.9.6</v>
+        <v>6.8.5</v>
       </c>
       <c r="E83" s="5" t="str">
-        <v>March</v>
+        <v>June</v>
       </c>
       <c r="F83" s="5" t="str">
         <v>2023</v>
@@ -2404,177 +2404,177 @@
     </row>
     <row r="84" ht="30" customHeight="1">
       <c r="A84" s="4" t="str">
-        <v>510a7384-f1c7-499b-a88d-88a290d2e9b2</v>
+        <v>7ce83269-3fb5-47c9-b382-f661b9968ff9</v>
       </c>
       <c r="B84" s="5" t="str">
-        <v>6f2bc06f-7fe5-4e4b-9d32-897baa160d7a</v>
+        <v>025d43f4-f1dc-4e2a-8cb2-1e477ce3e401</v>
       </c>
       <c r="C84" s="5" t="str">
-        <v>Sleek Fresh Bike</v>
+        <v>Awesome Wooden Bacon</v>
       </c>
       <c r="D84" s="5" t="str">
-        <v>7.1.6</v>
+        <v>2.2.1</v>
       </c>
       <c r="E84" s="5" t="str">
-        <v>April</v>
+        <v>August</v>
       </c>
       <c r="F84" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G84" s="5">
-        <v>17</v>
+        <v>48</v>
       </c>
     </row>
     <row r="85" ht="30" customHeight="1">
       <c r="A85" s="4" t="str">
-        <v>3ccd702e-c2b5-46ed-a4e3-ace1fded4b1d</v>
+        <v>bdedad62-c5dc-4b6d-a862-fcbd197e98d0</v>
       </c>
       <c r="B85" s="5" t="str">
-        <v>2ff351b7-2814-4ad0-b296-8b4b11c33886</v>
+        <v>024425b7-8a07-4780-9e83-35fb89ef9680</v>
       </c>
       <c r="C85" s="5" t="str">
-        <v>Bespoke Plastic Pants</v>
+        <v>Modern Fresh Keyboard</v>
       </c>
       <c r="D85" s="5" t="str">
-        <v>1.0.0</v>
+        <v>8.9.2</v>
       </c>
       <c r="E85" s="5" t="str">
-        <v>January</v>
+        <v>May</v>
       </c>
       <c r="F85" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G85" s="5">
-        <v>11</v>
+        <v>89</v>
       </c>
     </row>
     <row r="86" ht="30" customHeight="1">
       <c r="A86" s="4" t="str">
-        <v>bbc19718-3b0d-434d-8b80-836f8fe2325e</v>
+        <v>4e3c54b8-a8ca-4a15-bf4d-dbaadc7570de</v>
       </c>
       <c r="B86" s="5" t="str">
-        <v>3e238c28-a249-4f0f-91a3-f3279e38f5e3</v>
+        <v>597c73c5-65fd-4852-87f3-3109e058d178</v>
       </c>
       <c r="C86" s="5" t="str">
-        <v>Incredible Bronze Chicken</v>
+        <v>Unbranded Soft Hat</v>
       </c>
       <c r="D86" s="5" t="str">
-        <v>7.0.9</v>
+        <v>8.3.1</v>
       </c>
       <c r="E86" s="5" t="str">
-        <v>June</v>
+        <v>July</v>
       </c>
       <c r="F86" s="5" t="str">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G86" s="5">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="87" ht="30" customHeight="1">
       <c r="A87" s="4" t="str">
-        <v>df5ea204-5869-4eb1-910d-68dc6961e49d</v>
+        <v>38ee4ce3-eb58-49f3-acd5-2058e2bb0ce5</v>
       </c>
       <c r="B87" s="5" t="str">
-        <v>241029fd-775f-4bf4-943a-641eb3f37e4d</v>
+        <v>a703e173-0ee4-4881-8e9f-4cfc4aa0531d</v>
       </c>
       <c r="C87" s="5" t="str">
-        <v>Intelligent Bronze Mouse</v>
+        <v>Bespoke Bronze Soap</v>
       </c>
       <c r="D87" s="5" t="str">
-        <v>0.3.4</v>
+        <v>5.9.2</v>
       </c>
       <c r="E87" s="5" t="str">
-        <v>November</v>
+        <v>October</v>
       </c>
       <c r="F87" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G87" s="5">
-        <v>15</v>
+        <v>93</v>
       </c>
     </row>
     <row r="88" ht="30" customHeight="1">
       <c r="A88" s="4" t="str">
-        <v>09d90f59-0261-4c17-aac8-9fa7f3e3ba88</v>
+        <v>45efc30f-d63d-46b5-83ce-c0c42f2561eb</v>
       </c>
       <c r="B88" s="5" t="str">
-        <v>27e2f468-32ca-4ce3-b92d-446e21f3a4cd</v>
+        <v>df55ccd6-84f5-4add-9d04-e2e14ed8df7b</v>
       </c>
       <c r="C88" s="5" t="str">
-        <v>Generic Bronze Chips</v>
+        <v>Incredible Rubber Gloves</v>
       </c>
       <c r="D88" s="5" t="str">
-        <v>0.2.9</v>
+        <v>4.5.7</v>
       </c>
       <c r="E88" s="5" t="str">
-        <v>May</v>
+        <v>December</v>
       </c>
       <c r="F88" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G88" s="5">
-        <v>15</v>
+        <v>98</v>
       </c>
     </row>
     <row r="89" ht="30" customHeight="1">
       <c r="A89" s="4" t="str">
-        <v>ed29f3bf-fce0-421b-ae6d-77eb84ad5ebc</v>
+        <v>9e6a0945-0d4e-40c8-821b-7e6109e82055</v>
       </c>
       <c r="B89" s="5" t="str">
-        <v>01c501c2-1df1-44bd-b34b-cc1ae564752a</v>
+        <v>1f067aef-d8b4-4ac6-bd76-dff38e14370a</v>
       </c>
       <c r="C89" s="5" t="str">
-        <v>Fantastic Fresh Hat</v>
+        <v>Intelligent Bronze Gloves</v>
       </c>
       <c r="D89" s="5" t="str">
-        <v>6.1.5</v>
+        <v>9.4.2</v>
       </c>
       <c r="E89" s="5" t="str">
-        <v>August</v>
+        <v>December</v>
       </c>
       <c r="F89" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G89" s="5">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="90" ht="30" customHeight="1">
       <c r="A90" s="4" t="str">
-        <v>4d41434c-c195-401c-a9df-f35570ccb099</v>
+        <v>7f066ceb-6235-4f7e-8f70-235bf6dd4acc</v>
       </c>
       <c r="B90" s="5" t="str">
-        <v>b54eb8f4-61e7-4368-a70d-4bb99f5185cf</v>
+        <v>f25b2234-166a-416f-8452-9dbacc59492d</v>
       </c>
       <c r="C90" s="5" t="str">
-        <v>Tasty Frozen Mouse</v>
+        <v>Handmade Soft Tuna</v>
       </c>
       <c r="D90" s="5" t="str">
-        <v>5.0.2</v>
+        <v>5.1.7</v>
       </c>
       <c r="E90" s="5" t="str">
-        <v>January</v>
+        <v>July</v>
       </c>
       <c r="F90" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G90" s="5">
-        <v>59</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" ht="30" customHeight="1">
       <c r="A91" s="4" t="str">
-        <v>ff542297-7399-4a0c-b7ad-c215766f3780</v>
+        <v>0c23c46f-f443-4d87-ba44-e7472cce607d</v>
       </c>
       <c r="B91" s="5" t="str">
-        <v>f056ab12-0d74-4bbd-ac3d-8c0756b90bc2</v>
+        <v>1c74e943-5a84-46af-8de5-f7d3630fc7a1</v>
       </c>
       <c r="C91" s="5" t="str">
-        <v>Incredible Plastic Cheese</v>
+        <v>Incredible Bronze Bike</v>
       </c>
       <c r="D91" s="5" t="str">
-        <v>1.0.4</v>
+        <v>7.7.4</v>
       </c>
       <c r="E91" s="5" t="str">
         <v>January</v>
@@ -2583,237 +2583,237 @@
         <v>2023</v>
       </c>
       <c r="G91" s="5">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="92" ht="30" customHeight="1">
       <c r="A92" s="4" t="str">
-        <v>70efc27a-bd47-41a1-af00-5e4faa91f3cf</v>
+        <v>0d26b306-78e1-49f6-8bc9-b022da762547</v>
       </c>
       <c r="B92" s="5" t="str">
-        <v>27a94e79-f87f-4f4c-9978-dcef70678c60</v>
+        <v>a29454f6-c5ac-4737-a15a-a932e609f6c0</v>
       </c>
       <c r="C92" s="5" t="str">
-        <v>Generic Plastic Salad</v>
+        <v>Unbranded Plastic Shoes</v>
       </c>
       <c r="D92" s="5" t="str">
-        <v>6.2.5</v>
+        <v>4.0.5</v>
       </c>
       <c r="E92" s="5" t="str">
-        <v>November</v>
+        <v>December</v>
       </c>
       <c r="F92" s="5" t="str">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G92" s="5">
-        <v>85</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" ht="30" customHeight="1">
       <c r="A93" s="4" t="str">
-        <v>410d38b2-af72-446a-b76c-8c0e7f3f7fed</v>
+        <v>421bc0ac-e51a-4b33-ad39-09bcb90d704b</v>
       </c>
       <c r="B93" s="5" t="str">
-        <v>495c0145-2c15-41c0-a739-ec84cbfc66ae</v>
+        <v>47726393-04eb-45d3-9d0b-7b0b95830d26</v>
       </c>
       <c r="C93" s="5" t="str">
-        <v>Intelligent Frozen Mouse</v>
+        <v>Handmade Plastic Pants</v>
       </c>
       <c r="D93" s="5" t="str">
-        <v>1.8.6</v>
+        <v>6.6.1</v>
       </c>
       <c r="E93" s="5" t="str">
-        <v>March</v>
+        <v>April</v>
       </c>
       <c r="F93" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G93" s="5">
-        <v>5</v>
+        <v>52</v>
       </c>
     </row>
     <row r="94" ht="30" customHeight="1">
       <c r="A94" s="4" t="str">
-        <v>124a2e3b-b001-440e-bd2e-0ffdb8fa0d31</v>
+        <v>b1a4f4e8-6043-444b-b540-c1bef5b67460</v>
       </c>
       <c r="B94" s="5" t="str">
-        <v>9f600a36-ab40-45da-94d3-7eb3ce50711c</v>
+        <v>b3e51eda-b9b9-4fdb-8272-5e0a8fc0e73e</v>
       </c>
       <c r="C94" s="5" t="str">
-        <v>Practical Granite Ball</v>
+        <v>Intelligent Frozen Bike</v>
       </c>
       <c r="D94" s="5" t="str">
-        <v>6.5.4</v>
+        <v>5.3.5</v>
       </c>
       <c r="E94" s="5" t="str">
-        <v>June</v>
+        <v>April</v>
       </c>
       <c r="F94" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G94" s="5">
-        <v>22</v>
+        <v>90</v>
       </c>
     </row>
     <row r="95" ht="30" customHeight="1">
       <c r="A95" s="4" t="str">
-        <v>aaf7d193-a010-4eea-a8c3-88fd90aae8e3</v>
+        <v>c7c46c7c-5f0a-4151-9105-2ae9b37ab636</v>
       </c>
       <c r="B95" s="5" t="str">
-        <v>6717c7d0-a843-48e7-81f7-616bc20ecd5f</v>
+        <v>f910f921-e13e-4a30-bec0-04ec98f09ae4</v>
       </c>
       <c r="C95" s="5" t="str">
-        <v>Ergonomic Granite Soap</v>
+        <v>Refined Rubber Keyboard</v>
       </c>
       <c r="D95" s="5" t="str">
-        <v>5.0.7</v>
+        <v>9.2.7</v>
       </c>
       <c r="E95" s="5" t="str">
-        <v>July</v>
+        <v>March</v>
       </c>
       <c r="F95" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G95" s="5">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="96" ht="30" customHeight="1">
       <c r="A96" s="4" t="str">
-        <v>70840b2d-0f92-4de8-b0b1-f8880fbce40e</v>
+        <v>deebc155-487d-4aad-b731-2347debf13bc</v>
       </c>
       <c r="B96" s="5" t="str">
-        <v>8874ea54-927a-46ff-8f04-49f03b8e03e2</v>
+        <v>4788e6b1-69b0-41b4-8f63-8d4653611fb6</v>
       </c>
       <c r="C96" s="5" t="str">
-        <v>Electronic Wooden Hat</v>
+        <v>Tasty Rubber Ball</v>
       </c>
       <c r="D96" s="5" t="str">
-        <v>5.7.1</v>
+        <v>5.7.9</v>
       </c>
       <c r="E96" s="5" t="str">
-        <v>August</v>
+        <v>September</v>
       </c>
       <c r="F96" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G96" s="5">
-        <v>28</v>
+        <v>91</v>
       </c>
     </row>
     <row r="97" ht="30" customHeight="1">
       <c r="A97" s="4" t="str">
-        <v>d0f13232-57cf-42af-a791-d0fbe2b453fe</v>
+        <v>6d1a3026-d51c-49d0-b5d4-ec8c0d1cd00f</v>
       </c>
       <c r="B97" s="5" t="str">
-        <v>7f852f98-5c98-4852-a9f0-de0a81de322b</v>
+        <v>00441895-f1fa-4b46-9dbf-9dab17e54817</v>
       </c>
       <c r="C97" s="5" t="str">
-        <v>Recycled Plastic Fish</v>
+        <v>Handcrafted Granite Gloves</v>
       </c>
       <c r="D97" s="5" t="str">
-        <v>0.2.4</v>
+        <v>7.6.4</v>
       </c>
       <c r="E97" s="5" t="str">
-        <v>March</v>
+        <v>July</v>
       </c>
       <c r="F97" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G97" s="5">
-        <v>76</v>
+        <v>42</v>
       </c>
     </row>
     <row r="98" ht="30" customHeight="1">
       <c r="A98" s="4" t="str">
-        <v>f253429c-7b46-4f4b-95d4-ef2b2f0a1f14</v>
+        <v>0c722923-ecae-45dc-8ea6-f77297a3da8f</v>
       </c>
       <c r="B98" s="5" t="str">
-        <v>349bc9dd-d5c5-406b-a7c4-91d0b835e015</v>
+        <v>dc968b6b-8a8b-4a31-a92c-ace96b9c4f0e</v>
       </c>
       <c r="C98" s="5" t="str">
-        <v>Bespoke Cotton Shoes</v>
+        <v>Small Plastic Soap</v>
       </c>
       <c r="D98" s="5" t="str">
-        <v>7.8.1</v>
+        <v>5.9.3</v>
       </c>
       <c r="E98" s="5" t="str">
-        <v>November</v>
+        <v>February</v>
       </c>
       <c r="F98" s="5" t="str">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="G98" s="5">
-        <v>65</v>
+        <v>32</v>
       </c>
     </row>
     <row r="99" ht="30" customHeight="1">
       <c r="A99" s="4" t="str">
-        <v>8dd600dc-0560-43d9-af9d-1c919f6d99f6</v>
+        <v>88070e4a-9ad0-463a-8e28-f19ac4b4da79</v>
       </c>
       <c r="B99" s="5" t="str">
-        <v>c8fc214b-eb25-48d2-8c68-fe16bd2d0d25</v>
+        <v>6fa3a8d7-6924-480a-8a94-09255197d815</v>
       </c>
       <c r="C99" s="5" t="str">
-        <v>Handcrafted Fresh Towels</v>
+        <v>Generic Wooden Chair</v>
       </c>
       <c r="D99" s="5" t="str">
-        <v>9.8.1</v>
+        <v>8.2.6</v>
       </c>
       <c r="E99" s="5" t="str">
-        <v>April</v>
+        <v>November</v>
       </c>
       <c r="F99" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G99" s="5">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="100" ht="30" customHeight="1">
       <c r="A100" s="4" t="str">
-        <v>29ef72f9-e729-40d8-ac15-18f9b54bc90e</v>
+        <v>1272e394-3ae4-455e-a964-cc95b06eeb15</v>
       </c>
       <c r="B100" s="5" t="str">
-        <v>4d5da15c-3e1e-43ea-91ba-f2072094b3f0</v>
+        <v>bbe88355-58b6-4e81-9458-0141d0418237</v>
       </c>
       <c r="C100" s="5" t="str">
-        <v>Ergonomic Cotton Computer</v>
+        <v>Luxurious Rubber Car</v>
       </c>
       <c r="D100" s="5" t="str">
-        <v>2.0.4</v>
+        <v>5.8.2</v>
       </c>
       <c r="E100" s="5" t="str">
-        <v>May</v>
+        <v>August</v>
       </c>
       <c r="F100" s="5" t="str">
         <v>2023</v>
       </c>
       <c r="G100" s="5">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="101" ht="30" customHeight="1">
       <c r="A101" s="4" t="str">
-        <v>c9dd9064-398e-4824-b47b-4e77358300b7</v>
+        <v>83242a70-59e1-4a20-a25e-2932e5d64699</v>
       </c>
       <c r="B101" s="5" t="str">
-        <v>f7602fc1-e3cd-4a9e-98cc-eee2ee9bea4f</v>
+        <v>c41c85d3-cd49-487f-9c34-107610e1c2e4</v>
       </c>
       <c r="C101" s="5" t="str">
-        <v>Awesome Plastic Pizza</v>
+        <v>Recycled Fresh Hat</v>
       </c>
       <c r="D101" s="5" t="str">
-        <v>8.0.1</v>
+        <v>3.7.9</v>
       </c>
       <c r="E101" s="5" t="str">
-        <v>September</v>
+        <v>August</v>
       </c>
       <c r="F101" s="5" t="str">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="G101" s="5">
-        <v>54</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: implement grid-like layout control for sheets with multiple tables
</commit_message>
<xml_diff>
--- a/consumption.xlsx
+++ b/consumption.xlsx
@@ -409,16 +409,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="5.83203125" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" ht="30" customHeight="1"/>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>